<commit_message>
Update-Modify NG Excel template
</commit_message>
<xml_diff>
--- a/bin/Debug/Template/NGReq_Template.xlsx
+++ b/bin/Debug/Template/NGReq_Template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My Project\My C# project\MC-Dept-App\bin\Debug\Template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Current Works\MC-Dept-App\bin\Debug\Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E764F42-F8F9-41A4-9442-AE92370F4BDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0991527-8626-481C-A6F9-7D0B0EA7BD25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="10" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
     <sheet name="Request Sheet (3)" sheetId="15" state="hidden" r:id="rId9"/>
     <sheet name="Sheet4" sheetId="16" state="hidden" r:id="rId10"/>
     <sheet name="Countable" sheetId="24" r:id="rId11"/>
-    <sheet name="Uncountable" sheetId="23" r:id="rId12"/>
+    <sheet name="Uncountable" sheetId="25" r:id="rId12"/>
     <sheet name="MC" sheetId="8" state="hidden" r:id="rId13"/>
     <sheet name="Sheet5" sheetId="9" state="hidden" r:id="rId14"/>
     <sheet name="NG Dispose" sheetId="6" state="hidden" r:id="rId15"/>
@@ -41,6 +41,17 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -3753,6 +3764,12 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="50" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" indent="6"/>
+    </xf>
     <xf numFmtId="0" fontId="44" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4253,12 +4270,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" indent="6"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -5215,7 +5226,7 @@
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="19" name="Group 18">
+        <xdr:cNvPr id="19" name="GRPFromLoc">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{68D779F1-41F7-4F0F-959D-6121798A6B7B}"/>
@@ -5356,7 +5367,7 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="22" name="Rectangle 21">
+          <xdr:cNvPr id="22" name="FromLocCode">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
                 <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D360ED82-DC43-D227-3FD2-D1B23B94A9BD}"/>
@@ -5419,7 +5430,7 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="23" name="Rectangle 22">
+          <xdr:cNvPr id="23" name="FromLocName">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
                 <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{54CAF664-3219-4ECA-0329-8199BCAD805B}"/>
@@ -5552,7 +5563,7 @@
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="25" name="Group 24">
+        <xdr:cNvPr id="25" name="GRPToLoc">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{364479E8-9B6A-4A0B-955E-1E54CD02AD16}"/>
@@ -5693,7 +5704,7 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="28" name="Rectangle 27">
+          <xdr:cNvPr id="28" name="ToLocCode">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
                 <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{359E8BF8-5F84-E10C-F11D-77A50050A1CC}"/>
@@ -5756,7 +5767,7 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="29" name="Rectangle 28">
+          <xdr:cNvPr id="29" name="ToLocName">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
                 <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D486E231-BEAD-E000-B989-E035C581FC68}"/>
@@ -7912,7 +7923,7 @@
         <xdr:cNvPr id="2" name="Rectangle 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6EA05D2B-3F2C-4B6B-8520-ABAF2EABA445}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5B715361-1D96-42DF-A4F9-D1C1BEA4A874}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7920,7 +7931,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9293492" y="3472962"/>
+          <a:off x="9216559" y="3475160"/>
           <a:ext cx="164592" cy="164592"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -7995,7 +8006,7 @@
         <xdr:cNvPr id="3" name="Group 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A306E6F8-61F8-4FF8-841C-073C60B9F405}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{10FD499C-2FB9-492F-A585-41723F8A0298}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8014,7 +8025,7 @@
           <xdr:cNvPr id="4" name="Group 3">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0AFE52B3-61B8-1FDD-2D69-0A12CFF5A9D8}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1CCFCDB0-E027-4C3E-F219-15C69EBD7962}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -8033,7 +8044,7 @@
             <xdr:cNvPr id="17" name="Rectangle 16">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3BD9DDAB-D565-6060-BFE8-AA53B45C548A}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{592BDD96-F381-28E2-3301-4BFD0582D7EF}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -8079,7 +8090,7 @@
             <xdr:cNvPr id="18" name="TextBox 17">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FF4FA636-A842-66DE-1056-4A631BDB0A26}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B3AE8D7A-C4E6-04EF-6681-A599A26D2360}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -8142,7 +8153,7 @@
           <xdr:cNvPr id="5" name="Group 4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4DEE0761-0F36-2789-27B8-64BB48118FF3}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{40F9ECFF-0E8C-AD8B-7771-D98BFAC6639B}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -8161,7 +8172,7 @@
             <xdr:cNvPr id="15" name="Rectangle 14">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3FF203E2-6F92-BF56-588C-9164736B8EFB}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E20728D8-AAE2-4C3E-FB2C-41EF936D24E0}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -8207,7 +8218,7 @@
             <xdr:cNvPr id="16" name="TextBox 15">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A82CB831-D2BA-249C-3DD9-24D0E035C0D9}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C46F8809-3CBE-4ADF-4DF5-8EA93A24B6FE}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -8270,7 +8281,7 @@
           <xdr:cNvPr id="6" name="Group 5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{090AD19D-1475-BC73-2F0C-CCC0865AEE17}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0AEAFEA1-2CFC-6537-614B-4EFEDCA36CBC}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -8289,7 +8300,7 @@
             <xdr:cNvPr id="13" name="Rectangle 12">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6BC5A378-A35D-CC34-B411-4CBA69230525}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E6719018-C6FE-FFF4-C981-8BB930654CC2}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -8335,7 +8346,7 @@
             <xdr:cNvPr id="14" name="TextBox 13">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B441817E-2E27-094F-55A4-BF882B0B9CCF}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EFF29D83-AE36-6B45-BC8F-A30DED5D2581}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -8398,7 +8409,7 @@
           <xdr:cNvPr id="7" name="Group 6">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{074C270E-4BA7-3625-BA54-B7A50FE03944}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{71D0C573-18A4-74D3-6485-538F3424F9C4}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -8417,7 +8428,7 @@
             <xdr:cNvPr id="11" name="Rectangle 10">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{88C8F15F-BE81-BE1D-50DE-9827550D200C}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{818B3EC7-1EBC-2BA1-3AAE-25F005F7EE97}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -8471,7 +8482,7 @@
             <xdr:cNvPr id="12" name="TextBox 11">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{234CF4C3-99D1-C20D-12B6-4C833AB1587E}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B4175DE6-474F-FE6F-D4D4-7FA0E5D85F09}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -8595,7 +8606,7 @@
           <xdr:cNvPr id="8" name="Group 7">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4C52C77E-900C-45EE-452F-888082966B77}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{204C8A3D-AF49-9476-5845-E15CDC1B6434}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -8614,7 +8625,7 @@
             <xdr:cNvPr id="9" name="Rectangle 8">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{61A2685E-B6AF-0D37-696C-0C2BAD644C32}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{73C0326F-CCF2-E378-3803-B9E2E3102685}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -8660,7 +8671,7 @@
             <xdr:cNvPr id="10" name="TextBox 9">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4108D73C-4323-9DA3-DDD8-AC323A8AEA57}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{88AD937E-286D-AB3E-3877-67F66FE64DE0}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -8736,10 +8747,10 @@
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="19" name="Group 18">
+        <xdr:cNvPr id="19" name="GRPFromLoc">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7CFF1E7F-8FA8-4764-AA1B-B05E481F03F1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{296E185C-EABE-4968-A420-3CEA802F7107}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8758,7 +8769,7 @@
           <xdr:cNvPr id="20" name="Rectangle 19">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{458487EA-08A0-4D97-C8D9-7E372616FAB5}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{924B446F-C398-A61D-18A6-EB2774096A96}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -8817,7 +8828,7 @@
           <xdr:cNvPr id="21" name="Rectangle 20">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{78273E7F-2265-DF9D-F385-96E6BC2A27BC}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0667A16B-0D85-D7E2-9218-49E8028A5225}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -8877,10 +8888,10 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="22" name="Rectangle 21">
+          <xdr:cNvPr id="22" name="FromLocCode">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9F154472-C88C-5948-8DEC-5C4910357F59}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2988A88C-8926-2F21-C984-1FA6C3A96B2D}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -8940,10 +8951,10 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="23" name="Rectangle 22">
+          <xdr:cNvPr id="23" name="FromLocName">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AF03B399-D49A-D911-864D-8BCBAC5CE569}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9F052BE3-195F-C459-63D8-2C254CE82A30}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -9006,7 +9017,7 @@
           <xdr:cNvPr id="24" name="Rectangle 23">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EBD5A245-1FA2-7E9A-CD2E-812556F6750B}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ABBB965B-85AA-5961-917E-E8EB23D2B52C}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -9073,10 +9084,10 @@
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="25" name="Group 24">
+        <xdr:cNvPr id="25" name="GRPToLoc">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{40DCD1D9-8333-45FE-AAAC-D7B1F7A99B41}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2C37898E-AC98-45CC-A847-115E21FBFBF6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9095,7 +9106,7 @@
           <xdr:cNvPr id="26" name="Rectangle 25">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0F164756-A99C-D9D6-D312-042C81A0BCCC}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E5C3D213-4412-24F6-EC3F-7FC07F7095CC}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -9154,7 +9165,7 @@
           <xdr:cNvPr id="27" name="Rectangle 26">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{61D1FF0C-4A05-0638-70E1-DDD066FB0670}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{47F6A34F-2D91-ED51-F8BC-07279EB0E4EB}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -9214,10 +9225,10 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="28" name="Rectangle 27">
+          <xdr:cNvPr id="28" name="ToLocCode">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{328341B8-E74C-6FED-D419-FF9860746DF8}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2F882BB1-5322-2E2B-BBE2-A0AB85768CF7}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -9277,10 +9288,10 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="29" name="Rectangle 28">
+          <xdr:cNvPr id="29" name="ToLocName">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0CE70AA4-D154-3D58-551A-2B61D8FC2093}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6B6FAFF0-6116-0F7B-EC32-04CB879332C5}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -9343,7 +9354,7 @@
           <xdr:cNvPr id="30" name="Rectangle 29">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8FA0ECEC-B4B5-23F0-2712-87F942A3EBF8}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2D5A24E7-A696-DCCB-1036-101188489748}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -9413,7 +9424,7 @@
         <xdr:cNvPr id="31" name="Group 30">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D66C87EF-5007-46DA-A0F9-F55F989773E7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8BF98980-E679-4143-8AA8-79268C4EEA63}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9432,7 +9443,7 @@
           <xdr:cNvPr id="32" name="Rectangle 31">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B1CFD874-6923-FF3F-A96C-FA66B8937C2A}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{263AAD39-256C-CC54-C882-B159694C9264}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -9491,7 +9502,7 @@
           <xdr:cNvPr id="33" name="Rectangle 32">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D20F5ED1-B669-C551-B49B-90F66A2929ED}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{78937EF7-9253-1416-B513-D74C10ED1AAC}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -9554,7 +9565,7 @@
           <xdr:cNvPr id="34" name="Rectangle 33">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8CA4913E-49C2-F6E9-3789-503E7166C1AB}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{341D9736-0526-8E52-2F06-5A10A3DF2ED0}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -9614,7 +9625,7 @@
           <xdr:cNvPr id="35" name="Rectangle 34">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7E3168A4-450A-EA67-1329-B9B1393E3FC3}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E3F31AD2-7126-41C8-08A0-F2646168C1F5}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -9674,7 +9685,7 @@
           <xdr:cNvPr id="36" name="Rectangle 35">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{987044EC-089C-72BA-1DD7-4EED633F53AC}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A4FFE18F-375E-CE4E-F0EF-FEDB65A578C9}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -9733,7 +9744,7 @@
           <xdr:cNvPr id="37" name="Rectangle 36">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{652B5A2D-6359-12FB-CC8B-6B21393191AD}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BEA9857D-9741-F4E6-50C3-C194F8BB8380}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -9792,7 +9803,7 @@
           <xdr:cNvPr id="38" name="Rectangle 37">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{59502E5A-4051-17E3-9819-3BBCEEB2053C}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F95D4AD8-356F-D655-C8BC-DA0169F3FD30}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -9868,7 +9879,7 @@
         <xdr:cNvPr id="39" name="Group 38">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D99020EC-3756-4F36-9A07-AE45D89D47F3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0137E2DD-330B-4076-B356-73BF29626F7D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9887,7 +9898,7 @@
           <xdr:cNvPr id="40" name="Group 39">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DB2D7925-982F-DBED-55BB-4DA26EA8708F}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5CAB6AE7-2B88-9F87-1807-A06C8505DAC2}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -9906,7 +9917,7 @@
             <xdr:cNvPr id="65" name="Rectangle 64">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{02A07244-4318-45A3-AADE-FF7E22DCB0FD}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{908DC405-813D-D075-7EB5-47ADBF63CAE8}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -9965,7 +9976,7 @@
             <xdr:cNvPr id="66" name="Rectangle 65">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7F4FB955-F482-E2D7-69B1-3B746D28C9DC}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{37A0CC4E-A87C-7845-D202-639B67C9A233}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -10025,7 +10036,7 @@
             <xdr:cNvPr id="67" name="Rectangle 66">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C88F9909-30F7-1A69-6EA4-6C5429BB7978}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{25B6FCEE-15DA-95E4-BB67-0A76B66F762E}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -10085,7 +10096,7 @@
           <xdr:cNvPr id="41" name="Group 40">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0AA6FD76-C3E4-90E5-6E12-EDDF4190D8B4}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0AAA6DCA-6200-E3AB-60C0-49929E3D834C}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -10104,7 +10115,7 @@
             <xdr:cNvPr id="62" name="Rectangle 61">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FCF201D0-AC6B-FCEE-CF77-AF140DCB5950}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7A49FF34-88ED-FAF4-F624-A713FE1B04AA}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -10163,7 +10174,7 @@
             <xdr:cNvPr id="63" name="Rectangle 62">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AFC52829-6B93-22F1-17AC-2D725E973678}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{556A12B5-1A31-8521-9F2A-EAA20D483EC6}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -10223,7 +10234,7 @@
             <xdr:cNvPr id="64" name="Rectangle 63">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A70DDD3F-15B7-EC10-8983-481BA99F546D}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7A5E97D0-B61B-6F5F-7FEF-A7150C24175E}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -10283,7 +10294,7 @@
           <xdr:cNvPr id="42" name="Group 41">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{74415A4B-7E6E-2989-6409-7BB92EC50C9E}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0672529A-0612-E5CC-3687-7395660CD0C1}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -10302,7 +10313,7 @@
             <xdr:cNvPr id="59" name="Rectangle 58">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{81004F3C-7177-F60D-13D2-3433E517A568}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{09AE4984-ADEB-C678-65CC-957B9C089515}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -10361,7 +10372,7 @@
             <xdr:cNvPr id="60" name="Rectangle 59">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F610151E-3C4F-08D6-6D9C-B37E917FA2A0}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E0794074-9808-224B-BD26-0DD8515B81AC}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -10421,7 +10432,7 @@
             <xdr:cNvPr id="61" name="Rectangle 60">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C604DD59-73F7-4AF4-EE35-593E09D0DCE7}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F2EB9FB6-0CB0-0016-47D8-D414523F22B7}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -10481,7 +10492,7 @@
           <xdr:cNvPr id="43" name="Group 42">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ADEE455F-4165-E412-A7BF-7263E89C594A}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BD071045-082C-E87A-77D4-D68BF0F27C57}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -10500,7 +10511,7 @@
             <xdr:cNvPr id="56" name="Rectangle 55">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7A4DE601-D797-EDFB-24C8-60DA864E1BBD}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{781CA0B9-2419-1BC6-8CFA-450ADD1D99B6}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -10559,7 +10570,7 @@
             <xdr:cNvPr id="57" name="Rectangle 56">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9AC6DE76-96C8-B9BD-8DF4-16267F46243D}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F7337E8D-CFF4-9FD9-5ACB-AA2D7BE81234}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -10619,7 +10630,7 @@
             <xdr:cNvPr id="58" name="Rectangle 57">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{661FC73C-47C0-C01C-AC96-4647C44C137F}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DF9072D1-27C0-A476-8903-B02035D0BE29}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -10679,7 +10690,7 @@
           <xdr:cNvPr id="44" name="Group 43">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{33530092-10A6-0D3A-0960-9785601BCEB7}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7E53A84C-C2EA-D7B1-A2D9-10417E09654D}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -10698,7 +10709,7 @@
             <xdr:cNvPr id="53" name="Rectangle 52">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{95A29182-705D-0F60-6840-D0873BA87C59}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{53B19993-8659-5A82-7049-33B2D6ED7970}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -10757,7 +10768,7 @@
             <xdr:cNvPr id="54" name="Rectangle 53">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F6675F2D-33AF-9996-3EEB-56C37126670F}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E11B55BE-5AF3-B029-E8E2-EB7D1D0A0AD3}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -10817,7 +10828,7 @@
             <xdr:cNvPr id="55" name="Rectangle 54">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BE886759-49B0-A3C5-9331-7BEA68ED6B8C}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F2763215-9810-D8CF-97E8-A59B12CC7ABC}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -10877,7 +10888,7 @@
           <xdr:cNvPr id="45" name="Group 44">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{30D50B74-DA0F-E151-6502-973B643EBD55}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C62F6A29-BC14-8CCF-7C71-9EBF13E5976C}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -10896,7 +10907,7 @@
             <xdr:cNvPr id="50" name="Rectangle 49">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{25EB4F80-B1EF-B0B0-B81C-4A5418FAB57A}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{25C2704A-4F7F-3D7A-4B4C-175D123722F3}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -10955,7 +10966,7 @@
             <xdr:cNvPr id="51" name="Rectangle 50">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A1F7D6E8-6B81-86E4-EA8D-F117C3F2A42A}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9442E07A-83B4-43FD-2B68-DD7F0435212C}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -11015,7 +11026,7 @@
             <xdr:cNvPr id="52" name="Rectangle 51">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{32B82469-52B4-C8C4-467A-D5F60E37720A}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4096F41C-E112-C89E-301D-6F25EB8A9808}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -11075,7 +11086,7 @@
           <xdr:cNvPr id="46" name="Group 45">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C8AF5BE8-2579-653F-47D1-3D9CC37B6752}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{88CDFCBC-FCAE-468D-2762-9A3FD694D8BB}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -11094,7 +11105,7 @@
             <xdr:cNvPr id="47" name="Rectangle 46">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{22695D89-C34B-7206-98CC-FD70E748272A}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3767F48A-AEB2-6723-AE1E-678C7D308981}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -11153,7 +11164,7 @@
             <xdr:cNvPr id="48" name="Rectangle 47">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0AE1DDCC-263B-87C6-B6A8-D971FE620071}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{495E297F-E058-108C-E2FB-8E378DA5FFE3}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -11213,7 +11224,7 @@
             <xdr:cNvPr id="49" name="Rectangle 48">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0F28EFF4-DCB0-98E7-6D89-01B4EEE0708F}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5658E096-4764-5735-3CCD-9EEFD7C736A6}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -11289,7 +11300,7 @@
         <xdr:cNvPr id="68" name="矢印: 右 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{25624F00-0145-403F-B420-84391F855545}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C9389A14-F463-43F8-BB47-C36F179B54FA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11352,7 +11363,7 @@
         <xdr:cNvPr id="69" name="Rectangle 68">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9D8B7B2B-C613-4C15-A614-B63F5E862382}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DC32D663-18C6-4745-A3E6-0965C2022E26}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11360,8 +11371,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2652347" y="1545980"/>
-          <a:ext cx="2877207" cy="321880"/>
+          <a:off x="2649416" y="1548178"/>
+          <a:ext cx="2860355" cy="322613"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -29168,29 +29179,29 @@
       </c>
     </row>
     <row r="3" spans="1:12" ht="26.25">
-      <c r="A3" s="320" t="s">
+      <c r="A3" s="322" t="s">
         <v>229</v>
       </c>
-      <c r="B3" s="320"/>
-      <c r="C3" s="320"/>
-      <c r="D3" s="320"/>
-      <c r="E3" s="320"/>
-      <c r="F3" s="320"/>
-      <c r="G3" s="320"/>
-      <c r="H3" s="320"/>
-      <c r="I3" s="320"/>
-      <c r="J3" s="320"/>
-      <c r="K3" s="320"/>
-      <c r="L3" s="320"/>
+      <c r="B3" s="322"/>
+      <c r="C3" s="322"/>
+      <c r="D3" s="322"/>
+      <c r="E3" s="322"/>
+      <c r="F3" s="322"/>
+      <c r="G3" s="322"/>
+      <c r="H3" s="322"/>
+      <c r="I3" s="322"/>
+      <c r="J3" s="322"/>
+      <c r="K3" s="322"/>
+      <c r="L3" s="322"/>
     </row>
     <row r="4" spans="1:12" ht="20.100000000000001" customHeight="1">
       <c r="H4" s="56" t="s">
         <v>88</v>
       </c>
-      <c r="I4" s="389">
+      <c r="I4" s="391">
         <v>45390</v>
       </c>
-      <c r="J4" s="389"/>
+      <c r="J4" s="391"/>
       <c r="K4" s="73"/>
       <c r="L4" s="73"/>
     </row>
@@ -29204,12 +29215,12 @@
       <c r="H5" s="56" t="s">
         <v>89</v>
       </c>
-      <c r="I5" s="326" t="s">
+      <c r="I5" s="328" t="s">
         <v>418</v>
       </c>
-      <c r="J5" s="326"/>
-      <c r="K5" s="326"/>
-      <c r="L5" s="326"/>
+      <c r="J5" s="328"/>
+      <c r="K5" s="328"/>
+      <c r="L5" s="328"/>
     </row>
     <row r="6" spans="1:12" ht="20.25" customHeight="1">
       <c r="B6" t="s">
@@ -29218,10 +29229,10 @@
       <c r="H6" s="56" t="s">
         <v>90</v>
       </c>
-      <c r="I6" s="326" t="s">
+      <c r="I6" s="328" t="s">
         <v>419</v>
       </c>
-      <c r="J6" s="326"/>
+      <c r="J6" s="328"/>
       <c r="K6" s="74"/>
       <c r="L6" s="74"/>
     </row>
@@ -29252,32 +29263,32 @@
       <c r="L8" s="13"/>
     </row>
     <row r="9" spans="1:12" ht="13.5" customHeight="1" thickBot="1">
-      <c r="J9" s="327" t="s">
+      <c r="J9" s="329" t="s">
         <v>132</v>
       </c>
-      <c r="K9" s="328" t="s">
+      <c r="K9" s="330" t="s">
         <v>140</v>
       </c>
-      <c r="L9" s="329"/>
+      <c r="L9" s="331"/>
     </row>
     <row r="10" spans="1:12">
       <c r="B10" s="50" t="s">
         <v>55</v>
       </c>
-      <c r="C10" s="323" t="s">
+      <c r="C10" s="325" t="s">
         <v>56</v>
       </c>
-      <c r="D10" s="324"/>
-      <c r="E10" s="325"/>
+      <c r="D10" s="326"/>
+      <c r="E10" s="327"/>
       <c r="F10" s="50" t="s">
         <v>55</v>
       </c>
-      <c r="G10" s="323" t="s">
+      <c r="G10" s="325" t="s">
         <v>56</v>
       </c>
-      <c r="H10" s="324"/>
+      <c r="H10" s="326"/>
       <c r="I10" s="13"/>
-      <c r="J10" s="327"/>
+      <c r="J10" s="329"/>
       <c r="K10" s="9" t="s">
         <v>141</v>
       </c>
@@ -29289,14 +29300,14 @@
       <c r="B11" s="221" t="s">
         <v>417</v>
       </c>
-      <c r="C11" s="387" t="s">
+      <c r="C11" s="389" t="s">
         <v>69</v>
       </c>
-      <c r="D11" s="388"/>
-      <c r="E11" s="325"/>
+      <c r="D11" s="390"/>
+      <c r="E11" s="327"/>
       <c r="F11" s="51"/>
-      <c r="G11" s="321"/>
-      <c r="H11" s="322"/>
+      <c r="G11" s="323"/>
+      <c r="H11" s="324"/>
       <c r="I11" s="13"/>
       <c r="J11" s="9"/>
       <c r="K11" s="10"/>
@@ -30062,10 +30073,10 @@
       <c r="L33" s="9"/>
     </row>
     <row r="34" spans="1:12" ht="16.5" customHeight="1">
-      <c r="A34" s="390" t="s">
+      <c r="A34" s="392" t="s">
         <v>392</v>
       </c>
-      <c r="B34" s="390"/>
+      <c r="B34" s="392"/>
       <c r="C34" s="67"/>
       <c r="D34" s="222"/>
       <c r="E34" s="219"/>
@@ -30082,27 +30093,27 @@
     </row>
     <row r="35" spans="1:12" ht="13.5" customHeight="1"/>
     <row r="36" spans="1:12">
-      <c r="A36" s="328" t="s">
+      <c r="A36" s="330" t="s">
         <v>95</v>
       </c>
-      <c r="B36" s="329"/>
-      <c r="C36" s="393" t="s">
+      <c r="B36" s="331"/>
+      <c r="C36" s="395" t="s">
         <v>93</v>
       </c>
-      <c r="D36" s="394"/>
-      <c r="E36" s="328" t="s">
+      <c r="D36" s="396"/>
+      <c r="E36" s="330" t="s">
         <v>221</v>
       </c>
-      <c r="F36" s="329"/>
-      <c r="G36" s="327" t="s">
+      <c r="F36" s="331"/>
+      <c r="G36" s="329" t="s">
         <v>231</v>
       </c>
-      <c r="H36" s="327"/>
-      <c r="I36" s="327"/>
-      <c r="J36" s="391" t="s">
+      <c r="H36" s="329"/>
+      <c r="I36" s="329"/>
+      <c r="J36" s="393" t="s">
         <v>230</v>
       </c>
-      <c r="K36" s="392"/>
+      <c r="K36" s="394"/>
     </row>
     <row r="37" spans="1:12">
       <c r="A37" s="65"/>
@@ -30163,11 +30174,11 @@
         <v>88</v>
       </c>
       <c r="F41" s="68"/>
-      <c r="G41" s="317" t="s">
+      <c r="G41" s="319" t="s">
         <v>88</v>
       </c>
-      <c r="H41" s="318"/>
-      <c r="I41" s="319"/>
+      <c r="H41" s="320"/>
+      <c r="I41" s="321"/>
       <c r="J41" s="67" t="s">
         <v>88</v>
       </c>
@@ -30208,8 +30219,8 @@
   </sheetPr>
   <dimension ref="A1:M27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -30233,7 +30244,7 @@
       <c r="A1" s="227" t="s">
         <v>142</v>
       </c>
-      <c r="I1" s="421" t="s">
+      <c r="I1" s="254" t="s">
         <v>429</v>
       </c>
       <c r="J1" s="228" t="s">
@@ -30246,28 +30257,28 @@
       </c>
     </row>
     <row r="3" spans="1:13" ht="25.5">
-      <c r="A3" s="396" t="s">
+      <c r="A3" s="398" t="s">
         <v>229</v>
       </c>
-      <c r="B3" s="396"/>
-      <c r="C3" s="396"/>
-      <c r="D3" s="396"/>
-      <c r="E3" s="396"/>
-      <c r="F3" s="396"/>
-      <c r="G3" s="396"/>
-      <c r="H3" s="396"/>
-      <c r="I3" s="396"/>
-      <c r="J3" s="396"/>
-      <c r="K3" s="396"/>
-      <c r="L3" s="396"/>
-      <c r="M3" s="396"/>
+      <c r="B3" s="398"/>
+      <c r="C3" s="398"/>
+      <c r="D3" s="398"/>
+      <c r="E3" s="398"/>
+      <c r="F3" s="398"/>
+      <c r="G3" s="398"/>
+      <c r="H3" s="398"/>
+      <c r="I3" s="398"/>
+      <c r="J3" s="398"/>
+      <c r="K3" s="398"/>
+      <c r="L3" s="398"/>
+      <c r="M3" s="398"/>
     </row>
     <row r="4" spans="1:13" ht="20.100000000000001" customHeight="1">
       <c r="I4" s="230" t="s">
         <v>88</v>
       </c>
-      <c r="J4" s="397"/>
-      <c r="K4" s="397"/>
+      <c r="J4" s="399"/>
+      <c r="K4" s="399"/>
       <c r="L4" s="231"/>
       <c r="M4" s="231"/>
     </row>
@@ -30275,19 +30286,19 @@
       <c r="I5" s="230" t="s">
         <v>89</v>
       </c>
-      <c r="J5" s="398"/>
-      <c r="K5" s="398"/>
-      <c r="L5" s="395"/>
-      <c r="M5" s="395"/>
+      <c r="J5" s="400"/>
+      <c r="K5" s="400"/>
+      <c r="L5" s="397"/>
+      <c r="M5" s="397"/>
     </row>
     <row r="6" spans="1:13" ht="20.25" customHeight="1">
       <c r="I6" s="230" t="s">
         <v>90</v>
       </c>
-      <c r="J6" s="398" t="s">
+      <c r="J6" s="400" t="s">
         <v>423</v>
       </c>
-      <c r="K6" s="398"/>
+      <c r="K6" s="400"/>
       <c r="L6" s="232"/>
       <c r="M6" s="232"/>
     </row>
@@ -30295,13 +30306,13 @@
       <c r="I7" s="230" t="s">
         <v>91</v>
       </c>
-      <c r="J7" s="395"/>
-      <c r="K7" s="395"/>
-      <c r="L7" s="395"/>
+      <c r="J7" s="397"/>
+      <c r="K7" s="397"/>
+      <c r="L7" s="397"/>
       <c r="M7" s="232"/>
     </row>
     <row r="8" spans="1:13" ht="20.25" customHeight="1">
-      <c r="E8" s="422" t="s">
+      <c r="E8" s="255" t="s">
         <v>430</v>
       </c>
       <c r="I8" s="233"/>
@@ -30311,33 +30322,33 @@
       <c r="M8" s="234"/>
     </row>
     <row r="9" spans="1:13" ht="13.5" customHeight="1">
-      <c r="K9" s="405"/>
-      <c r="L9" s="406"/>
-      <c r="M9" s="406"/>
+      <c r="K9" s="407"/>
+      <c r="L9" s="408"/>
+      <c r="M9" s="408"/>
     </row>
     <row r="10" spans="1:13">
       <c r="B10" s="234"/>
-      <c r="C10" s="406"/>
-      <c r="D10" s="406"/>
-      <c r="E10" s="405"/>
+      <c r="C10" s="408"/>
+      <c r="D10" s="408"/>
+      <c r="E10" s="407"/>
       <c r="F10" s="235"/>
       <c r="G10" s="234"/>
-      <c r="H10" s="406"/>
-      <c r="I10" s="406"/>
+      <c r="H10" s="408"/>
+      <c r="I10" s="408"/>
       <c r="J10" s="234"/>
-      <c r="K10" s="405"/>
+      <c r="K10" s="407"/>
       <c r="L10" s="234"/>
       <c r="M10" s="236"/>
     </row>
     <row r="11" spans="1:13" ht="26.25" customHeight="1">
       <c r="B11" s="235"/>
-      <c r="C11" s="405"/>
-      <c r="D11" s="405"/>
-      <c r="E11" s="405"/>
+      <c r="C11" s="407"/>
+      <c r="D11" s="407"/>
+      <c r="E11" s="407"/>
       <c r="F11" s="235"/>
       <c r="G11" s="235"/>
-      <c r="H11" s="405"/>
-      <c r="I11" s="405"/>
+      <c r="H11" s="407"/>
+      <c r="I11" s="407"/>
       <c r="J11" s="234"/>
       <c r="K11" s="234"/>
     </row>
@@ -30355,10 +30366,10 @@
       <c r="D13" s="238" t="s">
         <v>425</v>
       </c>
-      <c r="E13" s="399" t="s">
+      <c r="E13" s="401" t="s">
         <v>51</v>
       </c>
-      <c r="F13" s="400"/>
+      <c r="F13" s="402"/>
       <c r="G13" s="238" t="s">
         <v>52</v>
       </c>
@@ -30386,8 +30397,8 @@
       <c r="B14" s="239"/>
       <c r="C14" s="239"/>
       <c r="D14" s="240"/>
-      <c r="E14" s="401"/>
-      <c r="F14" s="402"/>
+      <c r="E14" s="403"/>
+      <c r="F14" s="404"/>
       <c r="G14" s="241"/>
       <c r="H14" s="242"/>
       <c r="I14" s="243"/>
@@ -30399,12 +30410,12 @@
       <c r="M14" s="247"/>
     </row>
     <row r="15" spans="1:13" ht="16.5" customHeight="1">
-      <c r="A15" s="403" t="s">
+      <c r="A15" s="405" t="s">
         <v>392</v>
       </c>
-      <c r="B15" s="404"/>
-      <c r="C15" s="404"/>
-      <c r="D15" s="404"/>
+      <c r="B15" s="406"/>
+      <c r="C15" s="406"/>
+      <c r="D15" s="406"/>
       <c r="E15" s="248"/>
       <c r="F15" s="248"/>
       <c r="G15" s="248"/>
@@ -30445,12 +30456,12 @@
     <mergeCell ref="H10:I10"/>
     <mergeCell ref="C11:D11"/>
     <mergeCell ref="H11:I11"/>
+    <mergeCell ref="J7:L7"/>
     <mergeCell ref="A3:M3"/>
     <mergeCell ref="J4:K4"/>
     <mergeCell ref="J5:K5"/>
     <mergeCell ref="L5:M5"/>
     <mergeCell ref="J6:K6"/>
-    <mergeCell ref="J7:L7"/>
   </mergeCells>
   <pageMargins left="0.1" right="0.1" top="0.2" bottom="0.2" header="0.1" footer="0.1"/>
   <pageSetup paperSize="9" scale="71" fitToHeight="0" orientation="portrait" r:id="rId1"/>
@@ -30459,7 +30470,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CB17A87-1389-424E-B771-CB2EADC6BB29}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA894C6E-7C3C-4FDB-B679-4ADE0845D6E2}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
     <pageSetUpPr fitToPage="1"/>
@@ -30467,7 +30478,7 @@
   <dimension ref="A1:M27"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="P13" sqref="P13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -30491,7 +30502,7 @@
       <c r="A1" s="227" t="s">
         <v>142</v>
       </c>
-      <c r="I1" s="421" t="s">
+      <c r="I1" s="254" t="s">
         <v>429</v>
       </c>
       <c r="J1" s="228" t="s">
@@ -30504,28 +30515,28 @@
       </c>
     </row>
     <row r="3" spans="1:13" ht="25.5">
-      <c r="A3" s="396" t="s">
+      <c r="A3" s="398" t="s">
         <v>229</v>
       </c>
-      <c r="B3" s="396"/>
-      <c r="C3" s="396"/>
-      <c r="D3" s="396"/>
-      <c r="E3" s="396"/>
-      <c r="F3" s="396"/>
-      <c r="G3" s="396"/>
-      <c r="H3" s="396"/>
-      <c r="I3" s="396"/>
-      <c r="J3" s="396"/>
-      <c r="K3" s="396"/>
-      <c r="L3" s="396"/>
-      <c r="M3" s="396"/>
+      <c r="B3" s="398"/>
+      <c r="C3" s="398"/>
+      <c r="D3" s="398"/>
+      <c r="E3" s="398"/>
+      <c r="F3" s="398"/>
+      <c r="G3" s="398"/>
+      <c r="H3" s="398"/>
+      <c r="I3" s="398"/>
+      <c r="J3" s="398"/>
+      <c r="K3" s="398"/>
+      <c r="L3" s="398"/>
+      <c r="M3" s="398"/>
     </row>
     <row r="4" spans="1:13" ht="20.100000000000001" customHeight="1">
       <c r="I4" s="230" t="s">
         <v>88</v>
       </c>
-      <c r="J4" s="397"/>
-      <c r="K4" s="397"/>
+      <c r="J4" s="399"/>
+      <c r="K4" s="399"/>
       <c r="L4" s="231"/>
       <c r="M4" s="231"/>
     </row>
@@ -30533,19 +30544,19 @@
       <c r="I5" s="230" t="s">
         <v>89</v>
       </c>
-      <c r="J5" s="398"/>
-      <c r="K5" s="398"/>
-      <c r="L5" s="395"/>
-      <c r="M5" s="395"/>
+      <c r="J5" s="400"/>
+      <c r="K5" s="400"/>
+      <c r="L5" s="397"/>
+      <c r="M5" s="397"/>
     </row>
     <row r="6" spans="1:13" ht="20.25" customHeight="1">
       <c r="I6" s="230" t="s">
         <v>90</v>
       </c>
-      <c r="J6" s="398" t="s">
+      <c r="J6" s="400" t="s">
         <v>423</v>
       </c>
-      <c r="K6" s="398"/>
+      <c r="K6" s="400"/>
       <c r="L6" s="232"/>
       <c r="M6" s="232"/>
     </row>
@@ -30553,13 +30564,13 @@
       <c r="I7" s="230" t="s">
         <v>91</v>
       </c>
-      <c r="J7" s="395"/>
-      <c r="K7" s="395"/>
-      <c r="L7" s="395"/>
+      <c r="J7" s="397"/>
+      <c r="K7" s="397"/>
+      <c r="L7" s="397"/>
       <c r="M7" s="232"/>
     </row>
     <row r="8" spans="1:13" ht="20.25" customHeight="1">
-      <c r="E8" s="422" t="s">
+      <c r="E8" s="255" t="s">
         <v>430</v>
       </c>
       <c r="I8" s="233"/>
@@ -30569,33 +30580,33 @@
       <c r="M8" s="234"/>
     </row>
     <row r="9" spans="1:13" ht="13.5" customHeight="1">
-      <c r="K9" s="405"/>
-      <c r="L9" s="406"/>
-      <c r="M9" s="406"/>
+      <c r="K9" s="407"/>
+      <c r="L9" s="408"/>
+      <c r="M9" s="408"/>
     </row>
     <row r="10" spans="1:13">
       <c r="B10" s="234"/>
-      <c r="C10" s="406"/>
-      <c r="D10" s="406"/>
-      <c r="E10" s="405"/>
+      <c r="C10" s="408"/>
+      <c r="D10" s="408"/>
+      <c r="E10" s="407"/>
       <c r="F10" s="235"/>
       <c r="G10" s="234"/>
-      <c r="H10" s="406"/>
-      <c r="I10" s="406"/>
+      <c r="H10" s="408"/>
+      <c r="I10" s="408"/>
       <c r="J10" s="234"/>
-      <c r="K10" s="405"/>
+      <c r="K10" s="407"/>
       <c r="L10" s="234"/>
       <c r="M10" s="236"/>
     </row>
     <row r="11" spans="1:13" ht="26.25" customHeight="1">
       <c r="B11" s="235"/>
-      <c r="C11" s="405"/>
-      <c r="D11" s="405"/>
-      <c r="E11" s="405"/>
+      <c r="C11" s="407"/>
+      <c r="D11" s="407"/>
+      <c r="E11" s="407"/>
       <c r="F11" s="235"/>
       <c r="G11" s="235"/>
-      <c r="H11" s="405"/>
-      <c r="I11" s="405"/>
+      <c r="H11" s="407"/>
+      <c r="I11" s="407"/>
       <c r="J11" s="234"/>
       <c r="K11" s="234"/>
     </row>
@@ -30613,10 +30624,10 @@
       <c r="D13" s="238" t="s">
         <v>425</v>
       </c>
-      <c r="E13" s="399" t="s">
+      <c r="E13" s="401" t="s">
         <v>51</v>
       </c>
-      <c r="F13" s="400"/>
+      <c r="F13" s="402"/>
       <c r="G13" s="238" t="s">
         <v>52</v>
       </c>
@@ -30644,8 +30655,8 @@
       <c r="B14" s="239"/>
       <c r="C14" s="239"/>
       <c r="D14" s="240"/>
-      <c r="E14" s="401"/>
-      <c r="F14" s="402"/>
+      <c r="E14" s="403"/>
+      <c r="F14" s="404"/>
       <c r="G14" s="241"/>
       <c r="H14" s="242"/>
       <c r="I14" s="243"/>
@@ -30657,12 +30668,12 @@
       <c r="M14" s="247"/>
     </row>
     <row r="15" spans="1:13" ht="16.5" customHeight="1">
-      <c r="A15" s="403" t="s">
+      <c r="A15" s="405" t="s">
         <v>392</v>
       </c>
-      <c r="B15" s="404"/>
-      <c r="C15" s="404"/>
-      <c r="D15" s="404"/>
+      <c r="B15" s="406"/>
+      <c r="C15" s="406"/>
+      <c r="D15" s="406"/>
       <c r="E15" s="248"/>
       <c r="F15" s="248"/>
       <c r="G15" s="248"/>
@@ -30760,32 +30771,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" s="407" t="s">
+      <c r="A1" s="409" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="407"/>
-      <c r="C1" s="407"/>
-      <c r="D1" s="407"/>
-      <c r="E1" s="407"/>
-      <c r="F1" s="407"/>
-      <c r="G1" s="407"/>
-      <c r="H1" s="407"/>
-      <c r="I1" s="407"/>
-      <c r="J1" s="407"/>
+      <c r="B1" s="409"/>
+      <c r="C1" s="409"/>
+      <c r="D1" s="409"/>
+      <c r="E1" s="409"/>
+      <c r="F1" s="409"/>
+      <c r="G1" s="409"/>
+      <c r="H1" s="409"/>
+      <c r="I1" s="409"/>
+      <c r="J1" s="409"/>
     </row>
     <row r="2" spans="1:10" ht="26.25">
-      <c r="A2" s="320" t="s">
+      <c r="A2" s="322" t="s">
         <v>123</v>
       </c>
-      <c r="B2" s="320"/>
-      <c r="C2" s="320"/>
-      <c r="D2" s="320"/>
-      <c r="E2" s="320"/>
-      <c r="F2" s="320"/>
-      <c r="G2" s="320"/>
-      <c r="H2" s="320"/>
-      <c r="I2" s="320"/>
-      <c r="J2" s="320"/>
+      <c r="B2" s="322"/>
+      <c r="C2" s="322"/>
+      <c r="D2" s="322"/>
+      <c r="E2" s="322"/>
+      <c r="F2" s="322"/>
+      <c r="G2" s="322"/>
+      <c r="H2" s="322"/>
+      <c r="I2" s="322"/>
+      <c r="J2" s="322"/>
     </row>
     <row r="3" spans="1:10" ht="20.25" customHeight="1">
       <c r="H3" s="56" t="s">
@@ -30801,8 +30812,8 @@
       <c r="H4" s="56" t="s">
         <v>89</v>
       </c>
-      <c r="I4" s="326"/>
-      <c r="J4" s="326"/>
+      <c r="I4" s="328"/>
+      <c r="J4" s="328"/>
     </row>
     <row r="5" spans="1:10" ht="20.25" customHeight="1">
       <c r="B5" t="s">
@@ -30846,11 +30857,11 @@
       <c r="B10" s="53" t="s">
         <v>50</v>
       </c>
-      <c r="C10" s="408" t="s">
+      <c r="C10" s="410" t="s">
         <v>51</v>
       </c>
-      <c r="D10" s="408"/>
-      <c r="E10" s="408"/>
+      <c r="D10" s="410"/>
+      <c r="E10" s="410"/>
       <c r="F10" s="53" t="s">
         <v>52</v>
       </c>
@@ -30860,442 +30871,442 @@
       <c r="H10" s="53" t="s">
         <v>54</v>
       </c>
-      <c r="I10" s="408" t="s">
+      <c r="I10" s="410" t="s">
         <v>6</v>
       </c>
-      <c r="J10" s="409"/>
+      <c r="J10" s="411"/>
     </row>
     <row r="11" spans="1:10" ht="20.25" customHeight="1" thickTop="1">
       <c r="A11" s="69">
         <v>1</v>
       </c>
       <c r="B11" s="6"/>
-      <c r="C11" s="410"/>
-      <c r="D11" s="411"/>
-      <c r="E11" s="412"/>
+      <c r="C11" s="412"/>
+      <c r="D11" s="413"/>
+      <c r="E11" s="414"/>
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
       <c r="H11" s="6"/>
-      <c r="I11" s="413"/>
-      <c r="J11" s="414"/>
+      <c r="I11" s="415"/>
+      <c r="J11" s="416"/>
     </row>
     <row r="12" spans="1:10" ht="20.25" customHeight="1">
       <c r="A12" s="70">
         <v>2</v>
       </c>
       <c r="B12" s="10"/>
-      <c r="C12" s="317"/>
-      <c r="D12" s="318"/>
-      <c r="E12" s="319"/>
+      <c r="C12" s="319"/>
+      <c r="D12" s="320"/>
+      <c r="E12" s="321"/>
       <c r="F12" s="10"/>
       <c r="G12" s="10"/>
       <c r="H12" s="10"/>
-      <c r="I12" s="328"/>
-      <c r="J12" s="415"/>
+      <c r="I12" s="330"/>
+      <c r="J12" s="417"/>
     </row>
     <row r="13" spans="1:10" ht="20.25" customHeight="1">
       <c r="A13" s="69">
         <v>3</v>
       </c>
       <c r="B13" s="10"/>
-      <c r="C13" s="317"/>
-      <c r="D13" s="318"/>
-      <c r="E13" s="319"/>
+      <c r="C13" s="319"/>
+      <c r="D13" s="320"/>
+      <c r="E13" s="321"/>
       <c r="F13" s="10"/>
       <c r="G13" s="10"/>
       <c r="H13" s="10"/>
-      <c r="I13" s="328"/>
-      <c r="J13" s="415"/>
+      <c r="I13" s="330"/>
+      <c r="J13" s="417"/>
     </row>
     <row r="14" spans="1:10" ht="20.25" customHeight="1">
       <c r="A14" s="70">
         <v>4</v>
       </c>
       <c r="B14" s="10"/>
-      <c r="C14" s="317"/>
-      <c r="D14" s="318"/>
-      <c r="E14" s="319"/>
+      <c r="C14" s="319"/>
+      <c r="D14" s="320"/>
+      <c r="E14" s="321"/>
       <c r="F14" s="10"/>
       <c r="G14" s="10"/>
       <c r="H14" s="10"/>
-      <c r="I14" s="328"/>
-      <c r="J14" s="415"/>
+      <c r="I14" s="330"/>
+      <c r="J14" s="417"/>
     </row>
     <row r="15" spans="1:10" ht="20.25" customHeight="1">
       <c r="A15" s="69">
         <v>5</v>
       </c>
       <c r="B15" s="10"/>
-      <c r="C15" s="317"/>
-      <c r="D15" s="318"/>
-      <c r="E15" s="319"/>
+      <c r="C15" s="319"/>
+      <c r="D15" s="320"/>
+      <c r="E15" s="321"/>
       <c r="F15" s="10"/>
       <c r="G15" s="10"/>
       <c r="H15" s="10"/>
-      <c r="I15" s="328"/>
-      <c r="J15" s="415"/>
+      <c r="I15" s="330"/>
+      <c r="J15" s="417"/>
     </row>
     <row r="16" spans="1:10" ht="20.25" customHeight="1">
       <c r="A16" s="70">
         <v>6</v>
       </c>
       <c r="B16" s="10"/>
-      <c r="C16" s="317"/>
-      <c r="D16" s="318"/>
-      <c r="E16" s="319"/>
+      <c r="C16" s="319"/>
+      <c r="D16" s="320"/>
+      <c r="E16" s="321"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
       <c r="H16" s="10"/>
-      <c r="I16" s="328"/>
-      <c r="J16" s="415"/>
+      <c r="I16" s="330"/>
+      <c r="J16" s="417"/>
     </row>
     <row r="17" spans="1:10" ht="20.25" customHeight="1">
       <c r="A17" s="69">
         <v>7</v>
       </c>
       <c r="B17" s="10"/>
-      <c r="C17" s="317"/>
-      <c r="D17" s="318"/>
-      <c r="E17" s="319"/>
+      <c r="C17" s="319"/>
+      <c r="D17" s="320"/>
+      <c r="E17" s="321"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
       <c r="H17" s="10"/>
-      <c r="I17" s="328"/>
-      <c r="J17" s="415"/>
+      <c r="I17" s="330"/>
+      <c r="J17" s="417"/>
     </row>
     <row r="18" spans="1:10" ht="20.25" customHeight="1">
       <c r="A18" s="70">
         <v>8</v>
       </c>
       <c r="B18" s="10"/>
-      <c r="C18" s="317"/>
-      <c r="D18" s="318"/>
-      <c r="E18" s="319"/>
+      <c r="C18" s="319"/>
+      <c r="D18" s="320"/>
+      <c r="E18" s="321"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
       <c r="H18" s="10"/>
-      <c r="I18" s="328"/>
-      <c r="J18" s="415"/>
+      <c r="I18" s="330"/>
+      <c r="J18" s="417"/>
     </row>
     <row r="19" spans="1:10" ht="20.25" customHeight="1">
       <c r="A19" s="69">
         <v>9</v>
       </c>
       <c r="B19" s="10"/>
-      <c r="C19" s="317"/>
-      <c r="D19" s="318"/>
-      <c r="E19" s="319"/>
+      <c r="C19" s="319"/>
+      <c r="D19" s="320"/>
+      <c r="E19" s="321"/>
       <c r="F19" s="10"/>
       <c r="G19" s="10"/>
       <c r="H19" s="10"/>
-      <c r="I19" s="328"/>
-      <c r="J19" s="415"/>
+      <c r="I19" s="330"/>
+      <c r="J19" s="417"/>
     </row>
     <row r="20" spans="1:10" ht="20.25" customHeight="1">
       <c r="A20" s="70">
         <v>10</v>
       </c>
       <c r="B20" s="10"/>
-      <c r="C20" s="317"/>
-      <c r="D20" s="318"/>
-      <c r="E20" s="319"/>
+      <c r="C20" s="319"/>
+      <c r="D20" s="320"/>
+      <c r="E20" s="321"/>
       <c r="F20" s="10"/>
       <c r="G20" s="10"/>
       <c r="H20" s="10"/>
-      <c r="I20" s="328"/>
-      <c r="J20" s="415"/>
+      <c r="I20" s="330"/>
+      <c r="J20" s="417"/>
     </row>
     <row r="21" spans="1:10" ht="20.25" customHeight="1">
       <c r="A21" s="69">
         <v>11</v>
       </c>
       <c r="B21" s="10"/>
-      <c r="C21" s="317"/>
-      <c r="D21" s="318"/>
-      <c r="E21" s="319"/>
+      <c r="C21" s="319"/>
+      <c r="D21" s="320"/>
+      <c r="E21" s="321"/>
       <c r="F21" s="10"/>
       <c r="G21" s="10"/>
       <c r="H21" s="10"/>
-      <c r="I21" s="328"/>
-      <c r="J21" s="415"/>
+      <c r="I21" s="330"/>
+      <c r="J21" s="417"/>
     </row>
     <row r="22" spans="1:10" ht="20.25" customHeight="1">
       <c r="A22" s="70">
         <v>12</v>
       </c>
       <c r="B22" s="10"/>
-      <c r="C22" s="317"/>
-      <c r="D22" s="318"/>
-      <c r="E22" s="319"/>
+      <c r="C22" s="319"/>
+      <c r="D22" s="320"/>
+      <c r="E22" s="321"/>
       <c r="F22" s="10"/>
       <c r="G22" s="10"/>
       <c r="H22" s="10"/>
-      <c r="I22" s="328"/>
-      <c r="J22" s="415"/>
+      <c r="I22" s="330"/>
+      <c r="J22" s="417"/>
     </row>
     <row r="23" spans="1:10" ht="20.25" customHeight="1">
       <c r="A23" s="69">
         <v>13</v>
       </c>
       <c r="B23" s="10"/>
-      <c r="C23" s="317"/>
-      <c r="D23" s="318"/>
-      <c r="E23" s="319"/>
+      <c r="C23" s="319"/>
+      <c r="D23" s="320"/>
+      <c r="E23" s="321"/>
       <c r="F23" s="10"/>
       <c r="G23" s="10"/>
       <c r="H23" s="10"/>
-      <c r="I23" s="328"/>
-      <c r="J23" s="415"/>
+      <c r="I23" s="330"/>
+      <c r="J23" s="417"/>
     </row>
     <row r="24" spans="1:10" ht="20.25" customHeight="1">
       <c r="A24" s="70">
         <v>14</v>
       </c>
       <c r="B24" s="10"/>
-      <c r="C24" s="317"/>
-      <c r="D24" s="318"/>
-      <c r="E24" s="319"/>
+      <c r="C24" s="319"/>
+      <c r="D24" s="320"/>
+      <c r="E24" s="321"/>
       <c r="F24" s="10"/>
       <c r="G24" s="10"/>
       <c r="H24" s="10"/>
-      <c r="I24" s="328"/>
-      <c r="J24" s="415"/>
+      <c r="I24" s="330"/>
+      <c r="J24" s="417"/>
     </row>
     <row r="25" spans="1:10" ht="20.25" customHeight="1">
       <c r="A25" s="69">
         <v>15</v>
       </c>
       <c r="B25" s="10"/>
-      <c r="C25" s="317"/>
-      <c r="D25" s="318"/>
-      <c r="E25" s="319"/>
+      <c r="C25" s="319"/>
+      <c r="D25" s="320"/>
+      <c r="E25" s="321"/>
       <c r="F25" s="10"/>
       <c r="G25" s="10"/>
       <c r="H25" s="10"/>
-      <c r="I25" s="328"/>
-      <c r="J25" s="415"/>
+      <c r="I25" s="330"/>
+      <c r="J25" s="417"/>
     </row>
     <row r="26" spans="1:10" ht="20.25" customHeight="1">
       <c r="A26" s="70">
         <v>16</v>
       </c>
       <c r="B26" s="10"/>
-      <c r="C26" s="317"/>
-      <c r="D26" s="318"/>
-      <c r="E26" s="319"/>
+      <c r="C26" s="319"/>
+      <c r="D26" s="320"/>
+      <c r="E26" s="321"/>
       <c r="F26" s="10"/>
       <c r="G26" s="10"/>
       <c r="H26" s="10"/>
-      <c r="I26" s="328"/>
-      <c r="J26" s="415"/>
+      <c r="I26" s="330"/>
+      <c r="J26" s="417"/>
     </row>
     <row r="27" spans="1:10" ht="20.25" customHeight="1">
       <c r="A27" s="69">
         <v>17</v>
       </c>
       <c r="B27" s="10"/>
-      <c r="C27" s="317"/>
-      <c r="D27" s="318"/>
-      <c r="E27" s="319"/>
+      <c r="C27" s="319"/>
+      <c r="D27" s="320"/>
+      <c r="E27" s="321"/>
       <c r="F27" s="10"/>
       <c r="G27" s="10"/>
       <c r="H27" s="10"/>
-      <c r="I27" s="328"/>
-      <c r="J27" s="415"/>
+      <c r="I27" s="330"/>
+      <c r="J27" s="417"/>
     </row>
     <row r="28" spans="1:10" ht="20.25" customHeight="1">
       <c r="A28" s="70">
         <v>18</v>
       </c>
       <c r="B28" s="10"/>
-      <c r="C28" s="317"/>
-      <c r="D28" s="318"/>
-      <c r="E28" s="319"/>
+      <c r="C28" s="319"/>
+      <c r="D28" s="320"/>
+      <c r="E28" s="321"/>
       <c r="F28" s="10"/>
       <c r="G28" s="10"/>
       <c r="H28" s="10"/>
-      <c r="I28" s="328"/>
-      <c r="J28" s="415"/>
+      <c r="I28" s="330"/>
+      <c r="J28" s="417"/>
     </row>
     <row r="29" spans="1:10" ht="20.25" customHeight="1">
       <c r="A29" s="69">
         <v>19</v>
       </c>
       <c r="B29" s="10"/>
-      <c r="C29" s="317"/>
-      <c r="D29" s="318"/>
-      <c r="E29" s="319"/>
+      <c r="C29" s="319"/>
+      <c r="D29" s="320"/>
+      <c r="E29" s="321"/>
       <c r="F29" s="10"/>
       <c r="G29" s="10"/>
       <c r="H29" s="10"/>
-      <c r="I29" s="328"/>
-      <c r="J29" s="415"/>
+      <c r="I29" s="330"/>
+      <c r="J29" s="417"/>
     </row>
     <row r="30" spans="1:10" ht="20.25" customHeight="1">
       <c r="A30" s="70">
         <v>20</v>
       </c>
       <c r="B30" s="10"/>
-      <c r="C30" s="317"/>
-      <c r="D30" s="318"/>
-      <c r="E30" s="319"/>
+      <c r="C30" s="319"/>
+      <c r="D30" s="320"/>
+      <c r="E30" s="321"/>
       <c r="F30" s="10"/>
       <c r="G30" s="10"/>
       <c r="H30" s="10"/>
-      <c r="I30" s="328"/>
-      <c r="J30" s="415"/>
+      <c r="I30" s="330"/>
+      <c r="J30" s="417"/>
     </row>
     <row r="31" spans="1:10" ht="20.25" customHeight="1">
       <c r="A31" s="69">
         <v>21</v>
       </c>
       <c r="B31" s="10"/>
-      <c r="C31" s="317"/>
-      <c r="D31" s="318"/>
-      <c r="E31" s="319"/>
+      <c r="C31" s="319"/>
+      <c r="D31" s="320"/>
+      <c r="E31" s="321"/>
       <c r="F31" s="10"/>
       <c r="G31" s="10"/>
       <c r="H31" s="10"/>
-      <c r="I31" s="328"/>
-      <c r="J31" s="415"/>
+      <c r="I31" s="330"/>
+      <c r="J31" s="417"/>
     </row>
     <row r="32" spans="1:10" ht="20.25" customHeight="1">
       <c r="A32" s="70">
         <v>22</v>
       </c>
       <c r="B32" s="10"/>
-      <c r="C32" s="317"/>
-      <c r="D32" s="318"/>
-      <c r="E32" s="319"/>
+      <c r="C32" s="319"/>
+      <c r="D32" s="320"/>
+      <c r="E32" s="321"/>
       <c r="F32" s="10"/>
       <c r="G32" s="10"/>
       <c r="H32" s="10"/>
-      <c r="I32" s="328"/>
-      <c r="J32" s="415"/>
+      <c r="I32" s="330"/>
+      <c r="J32" s="417"/>
     </row>
     <row r="33" spans="1:10" ht="20.25" customHeight="1">
       <c r="A33" s="69">
         <v>23</v>
       </c>
       <c r="B33" s="10"/>
-      <c r="C33" s="317"/>
-      <c r="D33" s="318"/>
-      <c r="E33" s="319"/>
+      <c r="C33" s="319"/>
+      <c r="D33" s="320"/>
+      <c r="E33" s="321"/>
       <c r="F33" s="10"/>
       <c r="G33" s="10"/>
       <c r="H33" s="10"/>
-      <c r="I33" s="328"/>
-      <c r="J33" s="415"/>
+      <c r="I33" s="330"/>
+      <c r="J33" s="417"/>
     </row>
     <row r="34" spans="1:10" ht="20.25" customHeight="1">
       <c r="A34" s="70">
         <v>24</v>
       </c>
       <c r="B34" s="10"/>
-      <c r="C34" s="317"/>
-      <c r="D34" s="318"/>
-      <c r="E34" s="319"/>
+      <c r="C34" s="319"/>
+      <c r="D34" s="320"/>
+      <c r="E34" s="321"/>
       <c r="F34" s="10"/>
       <c r="G34" s="10"/>
       <c r="H34" s="10"/>
-      <c r="I34" s="328"/>
-      <c r="J34" s="415"/>
+      <c r="I34" s="330"/>
+      <c r="J34" s="417"/>
     </row>
     <row r="35" spans="1:10" ht="20.25" customHeight="1">
       <c r="A35" s="69">
         <v>25</v>
       </c>
       <c r="B35" s="10"/>
-      <c r="C35" s="317"/>
-      <c r="D35" s="318"/>
-      <c r="E35" s="319"/>
+      <c r="C35" s="319"/>
+      <c r="D35" s="320"/>
+      <c r="E35" s="321"/>
       <c r="F35" s="10"/>
       <c r="G35" s="10"/>
       <c r="H35" s="10"/>
-      <c r="I35" s="328"/>
-      <c r="J35" s="415"/>
+      <c r="I35" s="330"/>
+      <c r="J35" s="417"/>
     </row>
     <row r="36" spans="1:10" ht="20.25" customHeight="1">
       <c r="A36" s="69">
         <v>26</v>
       </c>
       <c r="B36" s="71"/>
-      <c r="C36" s="317"/>
-      <c r="D36" s="318"/>
-      <c r="E36" s="319"/>
+      <c r="C36" s="319"/>
+      <c r="D36" s="320"/>
+      <c r="E36" s="321"/>
       <c r="F36" s="71"/>
       <c r="G36" s="71"/>
       <c r="H36" s="71"/>
-      <c r="I36" s="328"/>
-      <c r="J36" s="415"/>
+      <c r="I36" s="330"/>
+      <c r="J36" s="417"/>
     </row>
     <row r="37" spans="1:10" ht="20.25" customHeight="1">
       <c r="A37" s="69">
         <v>27</v>
       </c>
       <c r="B37" s="71"/>
-      <c r="C37" s="317"/>
-      <c r="D37" s="318"/>
-      <c r="E37" s="319"/>
+      <c r="C37" s="319"/>
+      <c r="D37" s="320"/>
+      <c r="E37" s="321"/>
       <c r="F37" s="71"/>
       <c r="G37" s="71"/>
       <c r="H37" s="71"/>
-      <c r="I37" s="328"/>
-      <c r="J37" s="415"/>
+      <c r="I37" s="330"/>
+      <c r="J37" s="417"/>
     </row>
     <row r="38" spans="1:10" ht="20.25" customHeight="1">
       <c r="A38" s="69">
         <v>28</v>
       </c>
       <c r="B38" s="71"/>
-      <c r="C38" s="317"/>
-      <c r="D38" s="318"/>
-      <c r="E38" s="319"/>
+      <c r="C38" s="319"/>
+      <c r="D38" s="320"/>
+      <c r="E38" s="321"/>
       <c r="F38" s="71"/>
       <c r="G38" s="71"/>
       <c r="H38" s="71"/>
-      <c r="I38" s="328"/>
-      <c r="J38" s="415"/>
+      <c r="I38" s="330"/>
+      <c r="J38" s="417"/>
     </row>
     <row r="39" spans="1:10" ht="20.25" customHeight="1">
       <c r="A39" s="69">
         <v>29</v>
       </c>
       <c r="B39" s="71"/>
-      <c r="C39" s="317"/>
-      <c r="D39" s="318"/>
-      <c r="E39" s="319"/>
+      <c r="C39" s="319"/>
+      <c r="D39" s="320"/>
+      <c r="E39" s="321"/>
       <c r="F39" s="71"/>
       <c r="G39" s="71"/>
       <c r="H39" s="71"/>
-      <c r="I39" s="328"/>
-      <c r="J39" s="415"/>
+      <c r="I39" s="330"/>
+      <c r="J39" s="417"/>
     </row>
     <row r="40" spans="1:10" ht="20.25" customHeight="1">
       <c r="A40" s="69">
         <v>30</v>
       </c>
       <c r="B40" s="71"/>
-      <c r="C40" s="317"/>
-      <c r="D40" s="318"/>
-      <c r="E40" s="319"/>
+      <c r="C40" s="319"/>
+      <c r="D40" s="320"/>
+      <c r="E40" s="321"/>
       <c r="F40" s="71"/>
       <c r="G40" s="71"/>
       <c r="H40" s="71"/>
-      <c r="I40" s="328"/>
-      <c r="J40" s="415"/>
+      <c r="I40" s="330"/>
+      <c r="J40" s="417"/>
     </row>
     <row r="41" spans="1:10" ht="8.25" customHeight="1" thickBot="1">
       <c r="A41" s="54"/>
       <c r="B41" s="55"/>
-      <c r="C41" s="416"/>
-      <c r="D41" s="417"/>
-      <c r="E41" s="418"/>
+      <c r="C41" s="418"/>
+      <c r="D41" s="419"/>
+      <c r="E41" s="420"/>
       <c r="F41" s="55"/>
       <c r="G41" s="55"/>
       <c r="H41" s="55"/>
-      <c r="I41" s="419"/>
-      <c r="J41" s="420"/>
+      <c r="I41" s="421"/>
+      <c r="J41" s="422"/>
     </row>
     <row r="42" spans="1:10" ht="14.25" customHeight="1">
       <c r="C42" s="72"/>
@@ -31312,26 +31323,26 @@
       <c r="J43" s="13"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="328" t="s">
+      <c r="A45" s="330" t="s">
         <v>95</v>
       </c>
-      <c r="B45" s="329"/>
-      <c r="C45" s="328" t="s">
+      <c r="B45" s="331"/>
+      <c r="C45" s="330" t="s">
         <v>94</v>
       </c>
-      <c r="D45" s="329"/>
-      <c r="E45" s="328" t="s">
+      <c r="D45" s="331"/>
+      <c r="E45" s="330" t="s">
         <v>93</v>
       </c>
-      <c r="F45" s="329"/>
-      <c r="G45" s="328" t="s">
+      <c r="F45" s="331"/>
+      <c r="G45" s="330" t="s">
         <v>114</v>
       </c>
-      <c r="H45" s="329"/>
-      <c r="I45" s="328" t="s">
+      <c r="H45" s="331"/>
+      <c r="I45" s="330" t="s">
         <v>92</v>
       </c>
-      <c r="J45" s="329"/>
+      <c r="J45" s="331"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="65"/>
@@ -32136,52 +32147,52 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="31.7" customHeight="1">
-      <c r="A1" s="254" t="s">
+      <c r="A1" s="256" t="s">
         <v>170</v>
       </c>
-      <c r="B1" s="254"/>
-      <c r="C1" s="254"/>
-      <c r="D1" s="254"/>
-      <c r="E1" s="254"/>
-      <c r="F1" s="254"/>
-      <c r="G1" s="254"/>
-      <c r="H1" s="254"/>
-      <c r="I1" s="254"/>
-      <c r="J1" s="254"/>
-      <c r="K1" s="254"/>
-      <c r="L1" s="254"/>
-      <c r="M1" s="254"/>
-      <c r="N1" s="254"/>
-      <c r="O1" s="254"/>
-      <c r="P1" s="254"/>
-      <c r="Q1" s="254"/>
+      <c r="B1" s="256"/>
+      <c r="C1" s="256"/>
+      <c r="D1" s="256"/>
+      <c r="E1" s="256"/>
+      <c r="F1" s="256"/>
+      <c r="G1" s="256"/>
+      <c r="H1" s="256"/>
+      <c r="I1" s="256"/>
+      <c r="J1" s="256"/>
+      <c r="K1" s="256"/>
+      <c r="L1" s="256"/>
+      <c r="M1" s="256"/>
+      <c r="N1" s="256"/>
+      <c r="O1" s="256"/>
+      <c r="P1" s="256"/>
+      <c r="Q1" s="256"/>
     </row>
     <row r="2" spans="1:17" s="77" customFormat="1" ht="23.45" customHeight="1">
-      <c r="A2" s="255" t="s">
+      <c r="A2" s="257" t="s">
         <v>171</v>
       </c>
-      <c r="B2" s="255"/>
-      <c r="C2" s="255"/>
-      <c r="D2" s="255"/>
-      <c r="E2" s="255"/>
-      <c r="F2" s="255"/>
-      <c r="G2" s="256" t="s">
+      <c r="B2" s="257"/>
+      <c r="C2" s="257"/>
+      <c r="D2" s="257"/>
+      <c r="E2" s="257"/>
+      <c r="F2" s="257"/>
+      <c r="G2" s="258" t="s">
         <v>98</v>
       </c>
-      <c r="H2" s="256"/>
-      <c r="I2" s="256"/>
-      <c r="J2" s="256"/>
-      <c r="K2" s="256"/>
-      <c r="L2" s="256"/>
-      <c r="M2" s="257" t="s">
+      <c r="H2" s="258"/>
+      <c r="I2" s="258"/>
+      <c r="J2" s="258"/>
+      <c r="K2" s="258"/>
+      <c r="L2" s="258"/>
+      <c r="M2" s="259" t="s">
         <v>172</v>
       </c>
-      <c r="N2" s="258" t="s">
+      <c r="N2" s="260" t="s">
         <v>173</v>
       </c>
-      <c r="O2" s="259"/>
-      <c r="P2" s="259"/>
-      <c r="Q2" s="260"/>
+      <c r="O2" s="261"/>
+      <c r="P2" s="261"/>
+      <c r="Q2" s="262"/>
     </row>
     <row r="3" spans="1:17" ht="30">
       <c r="A3" s="136"/>
@@ -32193,14 +32204,14 @@
       <c r="G3" s="139" t="s">
         <v>96</v>
       </c>
-      <c r="H3" s="261" t="s">
+      <c r="H3" s="263" t="s">
         <v>174</v>
       </c>
-      <c r="I3" s="261"/>
-      <c r="J3" s="261"/>
-      <c r="K3" s="261"/>
-      <c r="L3" s="261"/>
-      <c r="M3" s="257"/>
+      <c r="I3" s="263"/>
+      <c r="J3" s="263"/>
+      <c r="K3" s="263"/>
+      <c r="L3" s="263"/>
+      <c r="M3" s="259"/>
       <c r="N3" s="140" t="s">
         <v>175</v>
       </c>
@@ -34269,152 +34280,152 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="20.25" customHeight="1">
-      <c r="A1" s="299" t="s">
+      <c r="A1" s="301" t="s">
         <v>142</v>
       </c>
-      <c r="B1" s="300"/>
-      <c r="C1" s="300"/>
-      <c r="D1" s="300"/>
-      <c r="E1" s="300"/>
-      <c r="F1" s="300"/>
-      <c r="G1" s="300"/>
-      <c r="H1" s="301"/>
-      <c r="I1" s="302" t="s">
+      <c r="B1" s="302"/>
+      <c r="C1" s="302"/>
+      <c r="D1" s="302"/>
+      <c r="E1" s="302"/>
+      <c r="F1" s="302"/>
+      <c r="G1" s="302"/>
+      <c r="H1" s="303"/>
+      <c r="I1" s="304" t="s">
         <v>143</v>
       </c>
-      <c r="J1" s="303"/>
-      <c r="K1" s="304"/>
-      <c r="L1" s="305" t="s">
+      <c r="J1" s="305"/>
+      <c r="K1" s="306"/>
+      <c r="L1" s="307" t="s">
         <v>144</v>
       </c>
-      <c r="M1" s="306"/>
-      <c r="N1" s="307"/>
+      <c r="M1" s="308"/>
+      <c r="N1" s="309"/>
     </row>
     <row r="2" spans="1:14" ht="30" customHeight="1">
-      <c r="A2" s="308" t="s">
+      <c r="A2" s="310" t="s">
         <v>145</v>
       </c>
-      <c r="B2" s="309"/>
-      <c r="C2" s="309"/>
-      <c r="D2" s="309"/>
-      <c r="E2" s="309"/>
-      <c r="F2" s="309"/>
-      <c r="G2" s="309"/>
-      <c r="H2" s="310"/>
-      <c r="I2" s="311" t="s">
+      <c r="B2" s="311"/>
+      <c r="C2" s="311"/>
+      <c r="D2" s="311"/>
+      <c r="E2" s="311"/>
+      <c r="F2" s="311"/>
+      <c r="G2" s="311"/>
+      <c r="H2" s="312"/>
+      <c r="I2" s="313" t="s">
         <v>146</v>
       </c>
-      <c r="J2" s="312"/>
-      <c r="K2" s="313"/>
-      <c r="L2" s="314" t="s">
+      <c r="J2" s="314"/>
+      <c r="K2" s="315"/>
+      <c r="L2" s="316" t="s">
         <v>147</v>
       </c>
-      <c r="M2" s="315"/>
-      <c r="N2" s="316"/>
+      <c r="M2" s="317"/>
+      <c r="N2" s="318"/>
     </row>
     <row r="3" spans="1:14" ht="30.75" customHeight="1">
-      <c r="A3" s="287" t="s">
+      <c r="A3" s="289" t="s">
         <v>148</v>
       </c>
-      <c r="B3" s="288"/>
-      <c r="C3" s="288"/>
-      <c r="D3" s="288"/>
-      <c r="E3" s="288"/>
-      <c r="F3" s="288"/>
-      <c r="G3" s="288"/>
-      <c r="H3" s="289"/>
-      <c r="I3" s="290" t="s">
+      <c r="B3" s="290"/>
+      <c r="C3" s="290"/>
+      <c r="D3" s="290"/>
+      <c r="E3" s="290"/>
+      <c r="F3" s="290"/>
+      <c r="G3" s="290"/>
+      <c r="H3" s="291"/>
+      <c r="I3" s="292" t="s">
         <v>149</v>
       </c>
-      <c r="J3" s="291"/>
-      <c r="K3" s="290" t="s">
+      <c r="J3" s="293"/>
+      <c r="K3" s="292" t="s">
         <v>150</v>
       </c>
-      <c r="L3" s="291"/>
-      <c r="M3" s="290" t="s">
+      <c r="L3" s="293"/>
+      <c r="M3" s="292" t="s">
         <v>151</v>
       </c>
-      <c r="N3" s="292"/>
+      <c r="N3" s="294"/>
     </row>
     <row r="4" spans="1:14" ht="43.5" customHeight="1">
       <c r="A4" s="85" t="s">
         <v>152</v>
       </c>
-      <c r="B4" s="293" t="s">
+      <c r="B4" s="295" t="s">
         <v>153</v>
       </c>
-      <c r="C4" s="294"/>
-      <c r="D4" s="294"/>
-      <c r="E4" s="294"/>
-      <c r="F4" s="294"/>
-      <c r="G4" s="294"/>
-      <c r="H4" s="295"/>
-      <c r="I4" s="296"/>
-      <c r="J4" s="297"/>
-      <c r="K4" s="296"/>
-      <c r="L4" s="297"/>
-      <c r="M4" s="296"/>
-      <c r="N4" s="298"/>
+      <c r="C4" s="296"/>
+      <c r="D4" s="296"/>
+      <c r="E4" s="296"/>
+      <c r="F4" s="296"/>
+      <c r="G4" s="296"/>
+      <c r="H4" s="297"/>
+      <c r="I4" s="298"/>
+      <c r="J4" s="299"/>
+      <c r="K4" s="298"/>
+      <c r="L4" s="299"/>
+      <c r="M4" s="298"/>
+      <c r="N4" s="300"/>
     </row>
     <row r="5" spans="1:14" s="87" customFormat="1" ht="46.5" customHeight="1">
       <c r="A5" s="86">
         <v>1</v>
       </c>
-      <c r="B5" s="264" t="s">
+      <c r="B5" s="266" t="s">
         <v>154</v>
       </c>
-      <c r="C5" s="265"/>
-      <c r="D5" s="265"/>
-      <c r="E5" s="265"/>
-      <c r="F5" s="265"/>
-      <c r="G5" s="265"/>
-      <c r="H5" s="265"/>
-      <c r="I5" s="265"/>
-      <c r="J5" s="265"/>
-      <c r="K5" s="265"/>
-      <c r="L5" s="265"/>
-      <c r="M5" s="265"/>
-      <c r="N5" s="266"/>
+      <c r="C5" s="267"/>
+      <c r="D5" s="267"/>
+      <c r="E5" s="267"/>
+      <c r="F5" s="267"/>
+      <c r="G5" s="267"/>
+      <c r="H5" s="267"/>
+      <c r="I5" s="267"/>
+      <c r="J5" s="267"/>
+      <c r="K5" s="267"/>
+      <c r="L5" s="267"/>
+      <c r="M5" s="267"/>
+      <c r="N5" s="268"/>
     </row>
     <row r="6" spans="1:14" s="87" customFormat="1" ht="39" customHeight="1">
       <c r="A6" s="88">
         <v>2</v>
       </c>
-      <c r="B6" s="267" t="s">
+      <c r="B6" s="269" t="s">
         <v>155</v>
       </c>
-      <c r="C6" s="268"/>
-      <c r="D6" s="268"/>
-      <c r="E6" s="268"/>
-      <c r="F6" s="268"/>
-      <c r="G6" s="268"/>
-      <c r="H6" s="268"/>
-      <c r="I6" s="268"/>
-      <c r="J6" s="268"/>
-      <c r="K6" s="268"/>
-      <c r="L6" s="268"/>
-      <c r="M6" s="268"/>
-      <c r="N6" s="269"/>
+      <c r="C6" s="270"/>
+      <c r="D6" s="270"/>
+      <c r="E6" s="270"/>
+      <c r="F6" s="270"/>
+      <c r="G6" s="270"/>
+      <c r="H6" s="270"/>
+      <c r="I6" s="270"/>
+      <c r="J6" s="270"/>
+      <c r="K6" s="270"/>
+      <c r="L6" s="270"/>
+      <c r="M6" s="270"/>
+      <c r="N6" s="271"/>
     </row>
     <row r="7" spans="1:14" s="87" customFormat="1" ht="21" customHeight="1">
       <c r="A7" s="89" t="s">
         <v>156</v>
       </c>
-      <c r="B7" s="270" t="s">
+      <c r="B7" s="272" t="s">
         <v>157</v>
       </c>
-      <c r="C7" s="271"/>
-      <c r="D7" s="271"/>
-      <c r="E7" s="271"/>
-      <c r="F7" s="271"/>
-      <c r="G7" s="271"/>
-      <c r="H7" s="271"/>
-      <c r="I7" s="271"/>
-      <c r="J7" s="271"/>
-      <c r="K7" s="271"/>
-      <c r="L7" s="271"/>
-      <c r="M7" s="271"/>
-      <c r="N7" s="272"/>
+      <c r="C7" s="273"/>
+      <c r="D7" s="273"/>
+      <c r="E7" s="273"/>
+      <c r="F7" s="273"/>
+      <c r="G7" s="273"/>
+      <c r="H7" s="273"/>
+      <c r="I7" s="273"/>
+      <c r="J7" s="273"/>
+      <c r="K7" s="273"/>
+      <c r="L7" s="273"/>
+      <c r="M7" s="273"/>
+      <c r="N7" s="274"/>
     </row>
     <row r="8" spans="1:14" s="95" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A8" s="90"/>
@@ -34983,7 +34994,7 @@
       <c r="N42" s="99"/>
     </row>
     <row r="43" spans="1:14" s="123" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A43" s="273" t="s">
+      <c r="A43" s="275" t="s">
         <v>162</v>
       </c>
       <c r="B43" s="116" t="s">
@@ -34991,78 +35002,78 @@
       </c>
       <c r="C43" s="117"/>
       <c r="D43" s="118"/>
-      <c r="E43" s="276"/>
-      <c r="F43" s="277"/>
-      <c r="G43" s="277"/>
-      <c r="H43" s="277"/>
-      <c r="I43" s="277"/>
-      <c r="J43" s="277"/>
+      <c r="E43" s="278"/>
+      <c r="F43" s="279"/>
+      <c r="G43" s="279"/>
+      <c r="H43" s="279"/>
+      <c r="I43" s="279"/>
+      <c r="J43" s="279"/>
       <c r="K43" s="121"/>
       <c r="L43" s="120"/>
       <c r="M43" s="119"/>
       <c r="N43" s="122"/>
     </row>
     <row r="44" spans="1:14" s="123" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A44" s="274"/>
+      <c r="A44" s="276"/>
       <c r="B44" s="124" t="s">
         <v>163</v>
       </c>
       <c r="C44" s="125"/>
       <c r="D44" s="126"/>
-      <c r="E44" s="278"/>
-      <c r="F44" s="279"/>
-      <c r="G44" s="279"/>
-      <c r="H44" s="279"/>
-      <c r="I44" s="279"/>
-      <c r="J44" s="279"/>
+      <c r="E44" s="280"/>
+      <c r="F44" s="281"/>
+      <c r="G44" s="281"/>
+      <c r="H44" s="281"/>
+      <c r="I44" s="281"/>
+      <c r="J44" s="281"/>
       <c r="K44" s="127"/>
       <c r="L44" s="128"/>
       <c r="M44" s="129"/>
       <c r="N44" s="130"/>
     </row>
     <row r="45" spans="1:14" s="123" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A45" s="274"/>
+      <c r="A45" s="276"/>
       <c r="B45" s="131" t="s">
         <v>164</v>
       </c>
       <c r="C45" s="125"/>
       <c r="D45" s="126"/>
-      <c r="E45" s="280"/>
-      <c r="F45" s="281"/>
-      <c r="G45" s="281"/>
-      <c r="H45" s="281"/>
-      <c r="I45" s="281"/>
-      <c r="J45" s="281"/>
+      <c r="E45" s="282"/>
+      <c r="F45" s="283"/>
+      <c r="G45" s="283"/>
+      <c r="H45" s="283"/>
+      <c r="I45" s="283"/>
+      <c r="J45" s="283"/>
       <c r="K45" s="132"/>
       <c r="L45" s="128"/>
       <c r="M45" s="133"/>
       <c r="N45" s="134"/>
     </row>
     <row r="46" spans="1:14" s="123" customFormat="1" ht="25.5" customHeight="1" thickBot="1">
-      <c r="A46" s="275"/>
+      <c r="A46" s="277"/>
       <c r="B46" s="135" t="s">
         <v>165</v>
       </c>
-      <c r="C46" s="282" t="s">
+      <c r="C46" s="284" t="s">
         <v>166</v>
       </c>
-      <c r="D46" s="283"/>
-      <c r="E46" s="284" t="s">
+      <c r="D46" s="285"/>
+      <c r="E46" s="286" t="s">
         <v>167</v>
       </c>
-      <c r="F46" s="285"/>
-      <c r="G46" s="285"/>
-      <c r="H46" s="285"/>
-      <c r="I46" s="285"/>
-      <c r="J46" s="286"/>
-      <c r="K46" s="262" t="s">
+      <c r="F46" s="287"/>
+      <c r="G46" s="287"/>
+      <c r="H46" s="287"/>
+      <c r="I46" s="287"/>
+      <c r="J46" s="288"/>
+      <c r="K46" s="264" t="s">
         <v>168</v>
       </c>
-      <c r="L46" s="286"/>
-      <c r="M46" s="262" t="s">
+      <c r="L46" s="288"/>
+      <c r="M46" s="264" t="s">
         <v>169</v>
       </c>
-      <c r="N46" s="263"/>
+      <c r="N46" s="265"/>
     </row>
   </sheetData>
   <mergeCells count="25">
@@ -35138,20 +35149,20 @@
       </c>
     </row>
     <row r="3" spans="1:12" ht="26.25">
-      <c r="A3" s="320" t="s">
+      <c r="A3" s="322" t="s">
         <v>229</v>
       </c>
-      <c r="B3" s="320"/>
-      <c r="C3" s="320"/>
-      <c r="D3" s="320"/>
-      <c r="E3" s="320"/>
-      <c r="F3" s="320"/>
-      <c r="G3" s="320"/>
-      <c r="H3" s="320"/>
-      <c r="I3" s="320"/>
-      <c r="J3" s="320"/>
-      <c r="K3" s="320"/>
-      <c r="L3" s="320"/>
+      <c r="B3" s="322"/>
+      <c r="C3" s="322"/>
+      <c r="D3" s="322"/>
+      <c r="E3" s="322"/>
+      <c r="F3" s="322"/>
+      <c r="G3" s="322"/>
+      <c r="H3" s="322"/>
+      <c r="I3" s="322"/>
+      <c r="J3" s="322"/>
+      <c r="K3" s="322"/>
+      <c r="L3" s="322"/>
     </row>
     <row r="4" spans="1:12" ht="20.100000000000001" customHeight="1">
       <c r="H4" s="56" t="s">
@@ -35172,10 +35183,10 @@
       <c r="H5" s="56" t="s">
         <v>89</v>
       </c>
-      <c r="I5" s="326"/>
-      <c r="J5" s="326"/>
-      <c r="K5" s="326"/>
-      <c r="L5" s="326"/>
+      <c r="I5" s="328"/>
+      <c r="J5" s="328"/>
+      <c r="K5" s="328"/>
+      <c r="L5" s="328"/>
     </row>
     <row r="6" spans="1:12" ht="20.25" customHeight="1">
       <c r="B6" t="s">
@@ -35214,32 +35225,32 @@
       <c r="L8" s="13"/>
     </row>
     <row r="9" spans="1:12" ht="15.75" thickBot="1">
-      <c r="J9" s="327" t="s">
+      <c r="J9" s="329" t="s">
         <v>132</v>
       </c>
-      <c r="K9" s="328" t="s">
+      <c r="K9" s="330" t="s">
         <v>140</v>
       </c>
-      <c r="L9" s="329"/>
+      <c r="L9" s="331"/>
     </row>
     <row r="10" spans="1:12">
       <c r="B10" s="50" t="s">
         <v>55</v>
       </c>
-      <c r="C10" s="323" t="s">
+      <c r="C10" s="325" t="s">
         <v>56</v>
       </c>
-      <c r="D10" s="324"/>
-      <c r="E10" s="325"/>
+      <c r="D10" s="326"/>
+      <c r="E10" s="327"/>
       <c r="F10" s="50" t="s">
         <v>55</v>
       </c>
-      <c r="G10" s="323" t="s">
+      <c r="G10" s="325" t="s">
         <v>56</v>
       </c>
-      <c r="H10" s="324"/>
+      <c r="H10" s="326"/>
       <c r="I10" s="13"/>
-      <c r="J10" s="327"/>
+      <c r="J10" s="329"/>
       <c r="K10" s="9" t="s">
         <v>141</v>
       </c>
@@ -35249,12 +35260,12 @@
     </row>
     <row r="11" spans="1:12" ht="26.25" customHeight="1" thickBot="1">
       <c r="B11" s="51"/>
-      <c r="C11" s="321"/>
-      <c r="D11" s="322"/>
-      <c r="E11" s="325"/>
+      <c r="C11" s="323"/>
+      <c r="D11" s="324"/>
+      <c r="E11" s="327"/>
       <c r="F11" s="51"/>
-      <c r="G11" s="321"/>
-      <c r="H11" s="322"/>
+      <c r="G11" s="323"/>
+      <c r="H11" s="324"/>
       <c r="I11" s="13"/>
       <c r="J11" s="9"/>
       <c r="K11" s="10"/>
@@ -35937,23 +35948,23 @@
       <c r="L54" s="13"/>
     </row>
     <row r="56" spans="1:12">
-      <c r="A56" s="328" t="s">
+      <c r="A56" s="330" t="s">
         <v>95</v>
       </c>
-      <c r="B56" s="329"/>
-      <c r="C56" s="328" t="s">
+      <c r="B56" s="331"/>
+      <c r="C56" s="330" t="s">
         <v>93</v>
       </c>
-      <c r="D56" s="329"/>
-      <c r="E56" s="328" t="s">
+      <c r="D56" s="331"/>
+      <c r="E56" s="330" t="s">
         <v>221</v>
       </c>
-      <c r="F56" s="329"/>
-      <c r="G56" s="327" t="s">
+      <c r="F56" s="331"/>
+      <c r="G56" s="329" t="s">
         <v>231</v>
       </c>
-      <c r="H56" s="327"/>
-      <c r="I56" s="327"/>
+      <c r="H56" s="329"/>
+      <c r="I56" s="329"/>
       <c r="J56" s="58" t="s">
         <v>230</v>
       </c>
@@ -36013,11 +36024,11 @@
         <v>88</v>
       </c>
       <c r="F61" s="68"/>
-      <c r="G61" s="317" t="s">
+      <c r="G61" s="319" t="s">
         <v>88</v>
       </c>
-      <c r="H61" s="318"/>
-      <c r="I61" s="319"/>
+      <c r="H61" s="320"/>
+      <c r="I61" s="321"/>
       <c r="J61" s="10" t="s">
         <v>88</v>
       </c>
@@ -36065,52 +36076,52 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="31.7" customHeight="1">
-      <c r="A1" s="254" t="s">
+      <c r="A1" s="256" t="s">
         <v>170</v>
       </c>
-      <c r="B1" s="254"/>
-      <c r="C1" s="254"/>
-      <c r="D1" s="254"/>
-      <c r="E1" s="254"/>
-      <c r="F1" s="254"/>
-      <c r="G1" s="254"/>
-      <c r="H1" s="254"/>
-      <c r="I1" s="254"/>
-      <c r="J1" s="254"/>
-      <c r="K1" s="254"/>
-      <c r="L1" s="254"/>
-      <c r="M1" s="254"/>
-      <c r="N1" s="254"/>
-      <c r="O1" s="254"/>
-      <c r="P1" s="254"/>
-      <c r="Q1" s="254"/>
+      <c r="B1" s="256"/>
+      <c r="C1" s="256"/>
+      <c r="D1" s="256"/>
+      <c r="E1" s="256"/>
+      <c r="F1" s="256"/>
+      <c r="G1" s="256"/>
+      <c r="H1" s="256"/>
+      <c r="I1" s="256"/>
+      <c r="J1" s="256"/>
+      <c r="K1" s="256"/>
+      <c r="L1" s="256"/>
+      <c r="M1" s="256"/>
+      <c r="N1" s="256"/>
+      <c r="O1" s="256"/>
+      <c r="P1" s="256"/>
+      <c r="Q1" s="256"/>
     </row>
     <row r="2" spans="1:17" s="77" customFormat="1" ht="23.45" customHeight="1">
-      <c r="A2" s="255" t="s">
+      <c r="A2" s="257" t="s">
         <v>171</v>
       </c>
-      <c r="B2" s="255"/>
-      <c r="C2" s="255"/>
-      <c r="D2" s="255"/>
-      <c r="E2" s="255"/>
-      <c r="F2" s="255"/>
-      <c r="G2" s="255" t="s">
+      <c r="B2" s="257"/>
+      <c r="C2" s="257"/>
+      <c r="D2" s="257"/>
+      <c r="E2" s="257"/>
+      <c r="F2" s="257"/>
+      <c r="G2" s="257" t="s">
         <v>98</v>
       </c>
-      <c r="H2" s="255"/>
-      <c r="I2" s="255"/>
-      <c r="J2" s="255"/>
-      <c r="K2" s="255"/>
-      <c r="L2" s="255"/>
-      <c r="M2" s="257" t="s">
+      <c r="H2" s="257"/>
+      <c r="I2" s="257"/>
+      <c r="J2" s="257"/>
+      <c r="K2" s="257"/>
+      <c r="L2" s="257"/>
+      <c r="M2" s="259" t="s">
         <v>172</v>
       </c>
-      <c r="N2" s="258" t="s">
+      <c r="N2" s="260" t="s">
         <v>173</v>
       </c>
-      <c r="O2" s="259"/>
-      <c r="P2" s="259"/>
-      <c r="Q2" s="260"/>
+      <c r="O2" s="261"/>
+      <c r="P2" s="261"/>
+      <c r="Q2" s="262"/>
     </row>
     <row r="3" spans="1:17" ht="30">
       <c r="A3" s="136"/>
@@ -36122,14 +36133,14 @@
       <c r="G3" s="139" t="s">
         <v>96</v>
       </c>
-      <c r="H3" s="261" t="s">
+      <c r="H3" s="263" t="s">
         <v>174</v>
       </c>
-      <c r="I3" s="261"/>
-      <c r="J3" s="261"/>
-      <c r="K3" s="261"/>
-      <c r="L3" s="261"/>
-      <c r="M3" s="257"/>
+      <c r="I3" s="263"/>
+      <c r="J3" s="263"/>
+      <c r="K3" s="263"/>
+      <c r="L3" s="263"/>
+      <c r="M3" s="259"/>
       <c r="N3" s="140" t="s">
         <v>175</v>
       </c>
@@ -38351,152 +38362,152 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="20.25" customHeight="1">
-      <c r="A1" s="367" t="s">
+      <c r="A1" s="369" t="s">
         <v>142</v>
       </c>
-      <c r="B1" s="368"/>
-      <c r="C1" s="368"/>
-      <c r="D1" s="368"/>
-      <c r="E1" s="368"/>
-      <c r="F1" s="368"/>
-      <c r="G1" s="368"/>
-      <c r="H1" s="369"/>
-      <c r="I1" s="370" t="s">
+      <c r="B1" s="370"/>
+      <c r="C1" s="370"/>
+      <c r="D1" s="370"/>
+      <c r="E1" s="370"/>
+      <c r="F1" s="370"/>
+      <c r="G1" s="370"/>
+      <c r="H1" s="371"/>
+      <c r="I1" s="372" t="s">
         <v>143</v>
       </c>
-      <c r="J1" s="371"/>
-      <c r="K1" s="372"/>
-      <c r="L1" s="373" t="s">
+      <c r="J1" s="373"/>
+      <c r="K1" s="374"/>
+      <c r="L1" s="375" t="s">
         <v>144</v>
       </c>
-      <c r="M1" s="374"/>
-      <c r="N1" s="375"/>
+      <c r="M1" s="376"/>
+      <c r="N1" s="377"/>
     </row>
     <row r="2" spans="1:14" ht="30" customHeight="1">
-      <c r="A2" s="376" t="s">
+      <c r="A2" s="378" t="s">
         <v>145</v>
       </c>
-      <c r="B2" s="377"/>
-      <c r="C2" s="377"/>
-      <c r="D2" s="377"/>
-      <c r="E2" s="377"/>
-      <c r="F2" s="377"/>
-      <c r="G2" s="377"/>
-      <c r="H2" s="378"/>
-      <c r="I2" s="379" t="s">
+      <c r="B2" s="379"/>
+      <c r="C2" s="379"/>
+      <c r="D2" s="379"/>
+      <c r="E2" s="379"/>
+      <c r="F2" s="379"/>
+      <c r="G2" s="379"/>
+      <c r="H2" s="380"/>
+      <c r="I2" s="381" t="s">
         <v>146</v>
       </c>
-      <c r="J2" s="380"/>
-      <c r="K2" s="381"/>
-      <c r="L2" s="382" t="s">
+      <c r="J2" s="382"/>
+      <c r="K2" s="383"/>
+      <c r="L2" s="384" t="s">
         <v>147</v>
       </c>
-      <c r="M2" s="383"/>
-      <c r="N2" s="384"/>
+      <c r="M2" s="385"/>
+      <c r="N2" s="386"/>
     </row>
     <row r="3" spans="1:14" ht="30.75" customHeight="1">
-      <c r="A3" s="355" t="s">
+      <c r="A3" s="357" t="s">
         <v>148</v>
       </c>
-      <c r="B3" s="356"/>
-      <c r="C3" s="356"/>
-      <c r="D3" s="356"/>
-      <c r="E3" s="356"/>
-      <c r="F3" s="356"/>
-      <c r="G3" s="356"/>
-      <c r="H3" s="357"/>
-      <c r="I3" s="358" t="s">
+      <c r="B3" s="358"/>
+      <c r="C3" s="358"/>
+      <c r="D3" s="358"/>
+      <c r="E3" s="358"/>
+      <c r="F3" s="358"/>
+      <c r="G3" s="358"/>
+      <c r="H3" s="359"/>
+      <c r="I3" s="360" t="s">
         <v>149</v>
       </c>
-      <c r="J3" s="359"/>
-      <c r="K3" s="358" t="s">
+      <c r="J3" s="361"/>
+      <c r="K3" s="360" t="s">
         <v>150</v>
       </c>
-      <c r="L3" s="359"/>
-      <c r="M3" s="358" t="s">
+      <c r="L3" s="361"/>
+      <c r="M3" s="360" t="s">
         <v>151</v>
       </c>
-      <c r="N3" s="360"/>
+      <c r="N3" s="362"/>
     </row>
     <row r="4" spans="1:14" ht="43.5" customHeight="1">
       <c r="A4" s="165" t="s">
         <v>152</v>
       </c>
-      <c r="B4" s="361" t="s">
+      <c r="B4" s="363" t="s">
         <v>153</v>
       </c>
-      <c r="C4" s="362"/>
-      <c r="D4" s="362"/>
-      <c r="E4" s="362"/>
-      <c r="F4" s="362"/>
-      <c r="G4" s="362"/>
-      <c r="H4" s="363"/>
-      <c r="I4" s="364"/>
-      <c r="J4" s="365"/>
-      <c r="K4" s="364"/>
-      <c r="L4" s="365"/>
-      <c r="M4" s="364"/>
-      <c r="N4" s="366"/>
+      <c r="C4" s="364"/>
+      <c r="D4" s="364"/>
+      <c r="E4" s="364"/>
+      <c r="F4" s="364"/>
+      <c r="G4" s="364"/>
+      <c r="H4" s="365"/>
+      <c r="I4" s="366"/>
+      <c r="J4" s="367"/>
+      <c r="K4" s="366"/>
+      <c r="L4" s="367"/>
+      <c r="M4" s="366"/>
+      <c r="N4" s="368"/>
     </row>
     <row r="5" spans="1:14" s="167" customFormat="1" ht="46.5" customHeight="1">
       <c r="A5" s="166">
         <v>1</v>
       </c>
-      <c r="B5" s="332" t="s">
+      <c r="B5" s="334" t="s">
         <v>154</v>
       </c>
-      <c r="C5" s="333"/>
-      <c r="D5" s="333"/>
-      <c r="E5" s="333"/>
-      <c r="F5" s="333"/>
-      <c r="G5" s="333"/>
-      <c r="H5" s="333"/>
-      <c r="I5" s="333"/>
-      <c r="J5" s="333"/>
-      <c r="K5" s="333"/>
-      <c r="L5" s="333"/>
-      <c r="M5" s="333"/>
-      <c r="N5" s="334"/>
+      <c r="C5" s="335"/>
+      <c r="D5" s="335"/>
+      <c r="E5" s="335"/>
+      <c r="F5" s="335"/>
+      <c r="G5" s="335"/>
+      <c r="H5" s="335"/>
+      <c r="I5" s="335"/>
+      <c r="J5" s="335"/>
+      <c r="K5" s="335"/>
+      <c r="L5" s="335"/>
+      <c r="M5" s="335"/>
+      <c r="N5" s="336"/>
     </row>
     <row r="6" spans="1:14" s="167" customFormat="1" ht="39" customHeight="1">
       <c r="A6" s="168">
         <v>2</v>
       </c>
-      <c r="B6" s="335" t="s">
+      <c r="B6" s="337" t="s">
         <v>155</v>
       </c>
-      <c r="C6" s="336"/>
-      <c r="D6" s="336"/>
-      <c r="E6" s="336"/>
-      <c r="F6" s="336"/>
-      <c r="G6" s="336"/>
-      <c r="H6" s="336"/>
-      <c r="I6" s="336"/>
-      <c r="J6" s="336"/>
-      <c r="K6" s="336"/>
-      <c r="L6" s="336"/>
-      <c r="M6" s="336"/>
-      <c r="N6" s="337"/>
+      <c r="C6" s="338"/>
+      <c r="D6" s="338"/>
+      <c r="E6" s="338"/>
+      <c r="F6" s="338"/>
+      <c r="G6" s="338"/>
+      <c r="H6" s="338"/>
+      <c r="I6" s="338"/>
+      <c r="J6" s="338"/>
+      <c r="K6" s="338"/>
+      <c r="L6" s="338"/>
+      <c r="M6" s="338"/>
+      <c r="N6" s="339"/>
     </row>
     <row r="7" spans="1:14" s="167" customFormat="1" ht="21" customHeight="1">
       <c r="A7" s="169" t="s">
         <v>156</v>
       </c>
-      <c r="B7" s="338" t="s">
+      <c r="B7" s="340" t="s">
         <v>157</v>
       </c>
-      <c r="C7" s="339"/>
-      <c r="D7" s="339"/>
-      <c r="E7" s="339"/>
-      <c r="F7" s="339"/>
-      <c r="G7" s="339"/>
-      <c r="H7" s="339"/>
-      <c r="I7" s="339"/>
-      <c r="J7" s="339"/>
-      <c r="K7" s="339"/>
-      <c r="L7" s="339"/>
-      <c r="M7" s="339"/>
-      <c r="N7" s="340"/>
+      <c r="C7" s="341"/>
+      <c r="D7" s="341"/>
+      <c r="E7" s="341"/>
+      <c r="F7" s="341"/>
+      <c r="G7" s="341"/>
+      <c r="H7" s="341"/>
+      <c r="I7" s="341"/>
+      <c r="J7" s="341"/>
+      <c r="K7" s="341"/>
+      <c r="L7" s="341"/>
+      <c r="M7" s="341"/>
+      <c r="N7" s="342"/>
     </row>
     <row r="8" spans="1:14" s="174" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A8" s="170"/>
@@ -39065,7 +39076,7 @@
       <c r="N42" s="178"/>
     </row>
     <row r="43" spans="1:14" s="202" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A43" s="341" t="s">
+      <c r="A43" s="343" t="s">
         <v>162</v>
       </c>
       <c r="B43" s="195" t="s">
@@ -39073,78 +39084,78 @@
       </c>
       <c r="C43" s="196"/>
       <c r="D43" s="197"/>
-      <c r="E43" s="344"/>
-      <c r="F43" s="345"/>
-      <c r="G43" s="345"/>
-      <c r="H43" s="345"/>
-      <c r="I43" s="345"/>
-      <c r="J43" s="345"/>
+      <c r="E43" s="346"/>
+      <c r="F43" s="347"/>
+      <c r="G43" s="347"/>
+      <c r="H43" s="347"/>
+      <c r="I43" s="347"/>
+      <c r="J43" s="347"/>
       <c r="K43" s="200"/>
       <c r="L43" s="199"/>
       <c r="M43" s="198"/>
       <c r="N43" s="201"/>
     </row>
     <row r="44" spans="1:14" s="202" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A44" s="342"/>
+      <c r="A44" s="344"/>
       <c r="B44" s="203" t="s">
         <v>163</v>
       </c>
       <c r="C44" s="204"/>
       <c r="D44" s="205"/>
-      <c r="E44" s="346"/>
-      <c r="F44" s="347"/>
-      <c r="G44" s="347"/>
-      <c r="H44" s="347"/>
-      <c r="I44" s="347"/>
-      <c r="J44" s="347"/>
+      <c r="E44" s="348"/>
+      <c r="F44" s="349"/>
+      <c r="G44" s="349"/>
+      <c r="H44" s="349"/>
+      <c r="I44" s="349"/>
+      <c r="J44" s="349"/>
       <c r="K44" s="206"/>
       <c r="L44" s="207"/>
       <c r="M44" s="208"/>
       <c r="N44" s="209"/>
     </row>
     <row r="45" spans="1:14" s="202" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A45" s="342"/>
+      <c r="A45" s="344"/>
       <c r="B45" s="210" t="s">
         <v>164</v>
       </c>
       <c r="C45" s="204"/>
       <c r="D45" s="205"/>
-      <c r="E45" s="348"/>
-      <c r="F45" s="349"/>
-      <c r="G45" s="349"/>
-      <c r="H45" s="349"/>
-      <c r="I45" s="349"/>
-      <c r="J45" s="349"/>
+      <c r="E45" s="350"/>
+      <c r="F45" s="351"/>
+      <c r="G45" s="351"/>
+      <c r="H45" s="351"/>
+      <c r="I45" s="351"/>
+      <c r="J45" s="351"/>
       <c r="K45" s="211"/>
       <c r="L45" s="207"/>
       <c r="M45" s="212"/>
       <c r="N45" s="213"/>
     </row>
     <row r="46" spans="1:14" s="202" customFormat="1" ht="25.5" customHeight="1" thickBot="1">
-      <c r="A46" s="343"/>
+      <c r="A46" s="345"/>
       <c r="B46" s="214" t="s">
         <v>165</v>
       </c>
-      <c r="C46" s="350" t="s">
+      <c r="C46" s="352" t="s">
         <v>166</v>
       </c>
-      <c r="D46" s="351"/>
-      <c r="E46" s="352" t="s">
+      <c r="D46" s="353"/>
+      <c r="E46" s="354" t="s">
         <v>167</v>
       </c>
-      <c r="F46" s="353"/>
-      <c r="G46" s="353"/>
-      <c r="H46" s="353"/>
-      <c r="I46" s="353"/>
-      <c r="J46" s="354"/>
-      <c r="K46" s="330" t="s">
+      <c r="F46" s="355"/>
+      <c r="G46" s="355"/>
+      <c r="H46" s="355"/>
+      <c r="I46" s="355"/>
+      <c r="J46" s="356"/>
+      <c r="K46" s="332" t="s">
         <v>168</v>
       </c>
-      <c r="L46" s="354"/>
-      <c r="M46" s="330" t="s">
+      <c r="L46" s="356"/>
+      <c r="M46" s="332" t="s">
         <v>169</v>
       </c>
-      <c r="N46" s="331"/>
+      <c r="N46" s="333"/>
     </row>
   </sheetData>
   <mergeCells count="25">
@@ -39217,29 +39228,29 @@
       </c>
     </row>
     <row r="3" spans="1:12" ht="26.25">
-      <c r="A3" s="320" t="s">
+      <c r="A3" s="322" t="s">
         <v>229</v>
       </c>
-      <c r="B3" s="320"/>
-      <c r="C3" s="320"/>
-      <c r="D3" s="320"/>
-      <c r="E3" s="320"/>
-      <c r="F3" s="320"/>
-      <c r="G3" s="320"/>
-      <c r="H3" s="320"/>
-      <c r="I3" s="320"/>
-      <c r="J3" s="320"/>
-      <c r="K3" s="320"/>
-      <c r="L3" s="320"/>
+      <c r="B3" s="322"/>
+      <c r="C3" s="322"/>
+      <c r="D3" s="322"/>
+      <c r="E3" s="322"/>
+      <c r="F3" s="322"/>
+      <c r="G3" s="322"/>
+      <c r="H3" s="322"/>
+      <c r="I3" s="322"/>
+      <c r="J3" s="322"/>
+      <c r="K3" s="322"/>
+      <c r="L3" s="322"/>
     </row>
     <row r="4" spans="1:12" ht="20.100000000000001" customHeight="1">
       <c r="H4" s="56" t="s">
         <v>88</v>
       </c>
-      <c r="I4" s="389">
+      <c r="I4" s="391">
         <v>45390</v>
       </c>
-      <c r="J4" s="389"/>
+      <c r="J4" s="391"/>
       <c r="K4" s="73"/>
       <c r="L4" s="73"/>
     </row>
@@ -39253,12 +39264,12 @@
       <c r="H5" s="56" t="s">
         <v>89</v>
       </c>
-      <c r="I5" s="326" t="s">
+      <c r="I5" s="328" t="s">
         <v>319</v>
       </c>
-      <c r="J5" s="326"/>
-      <c r="K5" s="326"/>
-      <c r="L5" s="326"/>
+      <c r="J5" s="328"/>
+      <c r="K5" s="328"/>
+      <c r="L5" s="328"/>
     </row>
     <row r="6" spans="1:12" ht="20.25" customHeight="1">
       <c r="B6" t="s">
@@ -39267,10 +39278,10 @@
       <c r="H6" s="56" t="s">
         <v>90</v>
       </c>
-      <c r="I6" s="326" t="s">
+      <c r="I6" s="328" t="s">
         <v>235</v>
       </c>
-      <c r="J6" s="326"/>
+      <c r="J6" s="328"/>
       <c r="K6" s="74"/>
       <c r="L6" s="74"/>
     </row>
@@ -39299,32 +39310,32 @@
       <c r="L8" s="13"/>
     </row>
     <row r="9" spans="1:12" ht="15.75" thickBot="1">
-      <c r="J9" s="327" t="s">
+      <c r="J9" s="329" t="s">
         <v>132</v>
       </c>
-      <c r="K9" s="328" t="s">
+      <c r="K9" s="330" t="s">
         <v>140</v>
       </c>
-      <c r="L9" s="329"/>
+      <c r="L9" s="331"/>
     </row>
     <row r="10" spans="1:12">
       <c r="B10" s="50" t="s">
         <v>55</v>
       </c>
-      <c r="C10" s="323" t="s">
+      <c r="C10" s="325" t="s">
         <v>56</v>
       </c>
-      <c r="D10" s="324"/>
-      <c r="E10" s="325"/>
+      <c r="D10" s="326"/>
+      <c r="E10" s="327"/>
       <c r="F10" s="50" t="s">
         <v>55</v>
       </c>
-      <c r="G10" s="323" t="s">
+      <c r="G10" s="325" t="s">
         <v>56</v>
       </c>
-      <c r="H10" s="324"/>
+      <c r="H10" s="326"/>
       <c r="I10" s="13"/>
-      <c r="J10" s="327"/>
+      <c r="J10" s="329"/>
       <c r="K10" s="9" t="s">
         <v>141</v>
       </c>
@@ -39336,14 +39347,14 @@
       <c r="B11" s="221" t="s">
         <v>234</v>
       </c>
-      <c r="C11" s="387" t="s">
+      <c r="C11" s="389" t="s">
         <v>235</v>
       </c>
-      <c r="D11" s="388"/>
-      <c r="E11" s="325"/>
+      <c r="D11" s="390"/>
+      <c r="E11" s="327"/>
       <c r="F11" s="51"/>
-      <c r="G11" s="321"/>
-      <c r="H11" s="322"/>
+      <c r="G11" s="323"/>
+      <c r="H11" s="324"/>
       <c r="I11" s="13"/>
       <c r="J11" s="9"/>
       <c r="K11" s="10"/>
@@ -40683,10 +40694,10 @@
       <c r="L48" s="9"/>
     </row>
     <row r="49" spans="1:12" ht="17.25" customHeight="1">
-      <c r="A49" s="385" t="s">
+      <c r="A49" s="387" t="s">
         <v>392</v>
       </c>
-      <c r="B49" s="386"/>
+      <c r="B49" s="388"/>
       <c r="C49" s="219"/>
       <c r="D49" s="219"/>
       <c r="E49" s="219"/>
@@ -40710,23 +40721,23 @@
     </row>
     <row r="51" spans="1:12" ht="18" customHeight="1"/>
     <row r="52" spans="1:12">
-      <c r="A52" s="328" t="s">
+      <c r="A52" s="330" t="s">
         <v>95</v>
       </c>
-      <c r="B52" s="329"/>
-      <c r="C52" s="328" t="s">
+      <c r="B52" s="331"/>
+      <c r="C52" s="330" t="s">
         <v>93</v>
       </c>
-      <c r="D52" s="329"/>
-      <c r="E52" s="328" t="s">
+      <c r="D52" s="331"/>
+      <c r="E52" s="330" t="s">
         <v>221</v>
       </c>
-      <c r="F52" s="329"/>
-      <c r="G52" s="327" t="s">
+      <c r="F52" s="331"/>
+      <c r="G52" s="329" t="s">
         <v>231</v>
       </c>
-      <c r="H52" s="327"/>
-      <c r="I52" s="327"/>
+      <c r="H52" s="329"/>
+      <c r="I52" s="329"/>
       <c r="J52" s="58" t="s">
         <v>230</v>
       </c>
@@ -40786,11 +40797,11 @@
         <v>88</v>
       </c>
       <c r="F57" s="68"/>
-      <c r="G57" s="317" t="s">
+      <c r="G57" s="319" t="s">
         <v>88</v>
       </c>
-      <c r="H57" s="318"/>
-      <c r="I57" s="319"/>
+      <c r="H57" s="320"/>
+      <c r="I57" s="321"/>
       <c r="J57" s="10" t="s">
         <v>88</v>
       </c>
@@ -40860,29 +40871,29 @@
       </c>
     </row>
     <row r="3" spans="1:12" ht="26.25">
-      <c r="A3" s="320" t="s">
+      <c r="A3" s="322" t="s">
         <v>229</v>
       </c>
-      <c r="B3" s="320"/>
-      <c r="C3" s="320"/>
-      <c r="D3" s="320"/>
-      <c r="E3" s="320"/>
-      <c r="F3" s="320"/>
-      <c r="G3" s="320"/>
-      <c r="H3" s="320"/>
-      <c r="I3" s="320"/>
-      <c r="J3" s="320"/>
-      <c r="K3" s="320"/>
-      <c r="L3" s="320"/>
+      <c r="B3" s="322"/>
+      <c r="C3" s="322"/>
+      <c r="D3" s="322"/>
+      <c r="E3" s="322"/>
+      <c r="F3" s="322"/>
+      <c r="G3" s="322"/>
+      <c r="H3" s="322"/>
+      <c r="I3" s="322"/>
+      <c r="J3" s="322"/>
+      <c r="K3" s="322"/>
+      <c r="L3" s="322"/>
     </row>
     <row r="4" spans="1:12" ht="20.100000000000001" customHeight="1">
       <c r="H4" s="56" t="s">
         <v>88</v>
       </c>
-      <c r="I4" s="389">
+      <c r="I4" s="391">
         <v>45390</v>
       </c>
-      <c r="J4" s="389"/>
+      <c r="J4" s="391"/>
       <c r="K4" s="73"/>
       <c r="L4" s="73"/>
     </row>
@@ -40896,12 +40907,12 @@
       <c r="H5" s="56" t="s">
         <v>89</v>
       </c>
-      <c r="I5" s="326" t="s">
+      <c r="I5" s="328" t="s">
         <v>319</v>
       </c>
-      <c r="J5" s="326"/>
-      <c r="K5" s="326"/>
-      <c r="L5" s="326"/>
+      <c r="J5" s="328"/>
+      <c r="K5" s="328"/>
+      <c r="L5" s="328"/>
     </row>
     <row r="6" spans="1:12" ht="20.25" customHeight="1">
       <c r="B6" t="s">
@@ -40910,10 +40921,10 @@
       <c r="H6" s="56" t="s">
         <v>90</v>
       </c>
-      <c r="I6" s="326" t="s">
+      <c r="I6" s="328" t="s">
         <v>235</v>
       </c>
-      <c r="J6" s="326"/>
+      <c r="J6" s="328"/>
       <c r="K6" s="74"/>
       <c r="L6" s="74"/>
     </row>
@@ -40942,32 +40953,32 @@
       <c r="L8" s="13"/>
     </row>
     <row r="9" spans="1:12" ht="13.5" customHeight="1" thickBot="1">
-      <c r="J9" s="327" t="s">
+      <c r="J9" s="329" t="s">
         <v>132</v>
       </c>
-      <c r="K9" s="328" t="s">
+      <c r="K9" s="330" t="s">
         <v>140</v>
       </c>
-      <c r="L9" s="329"/>
+      <c r="L9" s="331"/>
     </row>
     <row r="10" spans="1:12">
       <c r="B10" s="50" t="s">
         <v>55</v>
       </c>
-      <c r="C10" s="323" t="s">
+      <c r="C10" s="325" t="s">
         <v>56</v>
       </c>
-      <c r="D10" s="324"/>
-      <c r="E10" s="325"/>
+      <c r="D10" s="326"/>
+      <c r="E10" s="327"/>
       <c r="F10" s="50" t="s">
         <v>55</v>
       </c>
-      <c r="G10" s="323" t="s">
+      <c r="G10" s="325" t="s">
         <v>56</v>
       </c>
-      <c r="H10" s="324"/>
+      <c r="H10" s="326"/>
       <c r="I10" s="13"/>
-      <c r="J10" s="327"/>
+      <c r="J10" s="329"/>
       <c r="K10" s="9" t="s">
         <v>141</v>
       </c>
@@ -40979,14 +40990,14 @@
       <c r="B11" s="221" t="s">
         <v>234</v>
       </c>
-      <c r="C11" s="387" t="s">
+      <c r="C11" s="389" t="s">
         <v>235</v>
       </c>
-      <c r="D11" s="388"/>
-      <c r="E11" s="325"/>
+      <c r="D11" s="390"/>
+      <c r="E11" s="327"/>
       <c r="F11" s="51"/>
-      <c r="G11" s="321"/>
-      <c r="H11" s="322"/>
+      <c r="G11" s="323"/>
+      <c r="H11" s="324"/>
       <c r="I11" s="13"/>
       <c r="J11" s="9"/>
       <c r="K11" s="10"/>
@@ -42660,10 +42671,10 @@
       <c r="L57" s="9"/>
     </row>
     <row r="58" spans="1:12" ht="16.5" customHeight="1">
-      <c r="A58" s="390" t="s">
+      <c r="A58" s="392" t="s">
         <v>392</v>
       </c>
-      <c r="B58" s="390"/>
+      <c r="B58" s="392"/>
       <c r="C58" s="67"/>
       <c r="D58" s="222"/>
       <c r="E58" s="219"/>
@@ -42680,23 +42691,23 @@
     </row>
     <row r="59" spans="1:12" ht="21" customHeight="1"/>
     <row r="60" spans="1:12">
-      <c r="A60" s="328" t="s">
+      <c r="A60" s="330" t="s">
         <v>95</v>
       </c>
-      <c r="B60" s="329"/>
-      <c r="C60" s="328" t="s">
+      <c r="B60" s="331"/>
+      <c r="C60" s="330" t="s">
         <v>93</v>
       </c>
-      <c r="D60" s="329"/>
-      <c r="E60" s="328" t="s">
+      <c r="D60" s="331"/>
+      <c r="E60" s="330" t="s">
         <v>221</v>
       </c>
-      <c r="F60" s="329"/>
-      <c r="G60" s="327" t="s">
+      <c r="F60" s="331"/>
+      <c r="G60" s="329" t="s">
         <v>231</v>
       </c>
-      <c r="H60" s="327"/>
-      <c r="I60" s="327"/>
+      <c r="H60" s="329"/>
+      <c r="I60" s="329"/>
       <c r="J60" s="58" t="s">
         <v>230</v>
       </c>
@@ -42756,11 +42767,11 @@
         <v>88</v>
       </c>
       <c r="F65" s="68"/>
-      <c r="G65" s="317" t="s">
+      <c r="G65" s="319" t="s">
         <v>88</v>
       </c>
-      <c r="H65" s="318"/>
-      <c r="I65" s="319"/>
+      <c r="H65" s="320"/>
+      <c r="I65" s="321"/>
       <c r="J65" s="10" t="s">
         <v>88</v>
       </c>

</xml_diff>

<commit_message>
Update NG Search funct - Revise Excel PrintOut Template
</commit_message>
<xml_diff>
--- a/bin/Debug/Template/NGReq_Template.xlsx
+++ b/bin/Debug/Template/NGReq_Template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Current Works\MC-Dept-App\bin\Debug\Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0D31F02-5E06-480F-AC16-EF07850AE593}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E8E4D9C-C787-47E8-86D4-5FD4F61FEC64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="10" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1747,7 +1747,7 @@
     <numFmt numFmtId="166" formatCode="#,##0.0000"/>
     <numFmt numFmtId="167" formatCode="#,##0.000"/>
   </numFmts>
-  <fonts count="54">
+  <fonts count="55">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2087,6 +2087,13 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
@@ -3727,9 +3734,6 @@
     <xf numFmtId="0" fontId="52" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="52" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="52" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -3791,96 +3795,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="56" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="57" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="58" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="59" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="60" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="61" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="59" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="60" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="62" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="63" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="29" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="37" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="27" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="28" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="27" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="44" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="64" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="27" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="28" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="28" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="44" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="27" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="28" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="28" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="44" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="19" fillId="0" borderId="45" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3957,6 +3871,96 @@
     <xf numFmtId="49" fontId="19" fillId="0" borderId="47" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="64" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="27" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="28" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="28" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="44" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="27" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="28" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="28" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="44" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="56" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="57" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="58" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="59" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="60" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="61" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="59" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="60" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="62" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="63" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="29" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="37" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="27" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="28" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="27" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="44" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -3995,96 +3999,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="64" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="19" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -4161,6 +4075,96 @@
     <xf numFmtId="49" fontId="19" fillId="0" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="64" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4191,6 +4195,18 @@
     <xf numFmtId="0" fontId="48" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="51" fillId="4" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="50" fillId="4" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="50" fillId="4" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="50" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -4215,16 +4231,31 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="51" fillId="4" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="49" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="15" fontId="50" fillId="4" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="50" fillId="4" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
@@ -4242,34 +4273,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="165" fontId="54" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="52" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="54" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -29180,29 +29187,29 @@
       </c>
     </row>
     <row r="3" spans="1:12" ht="26.25">
-      <c r="A3" s="321" t="s">
+      <c r="A3" s="320" t="s">
         <v>229</v>
       </c>
-      <c r="B3" s="321"/>
-      <c r="C3" s="321"/>
-      <c r="D3" s="321"/>
-      <c r="E3" s="321"/>
-      <c r="F3" s="321"/>
-      <c r="G3" s="321"/>
-      <c r="H3" s="321"/>
-      <c r="I3" s="321"/>
-      <c r="J3" s="321"/>
-      <c r="K3" s="321"/>
-      <c r="L3" s="321"/>
+      <c r="B3" s="320"/>
+      <c r="C3" s="320"/>
+      <c r="D3" s="320"/>
+      <c r="E3" s="320"/>
+      <c r="F3" s="320"/>
+      <c r="G3" s="320"/>
+      <c r="H3" s="320"/>
+      <c r="I3" s="320"/>
+      <c r="J3" s="320"/>
+      <c r="K3" s="320"/>
+      <c r="L3" s="320"/>
     </row>
     <row r="4" spans="1:12" ht="20.100000000000001" customHeight="1">
       <c r="H4" s="56" t="s">
         <v>88</v>
       </c>
-      <c r="I4" s="390">
+      <c r="I4" s="389">
         <v>45390</v>
       </c>
-      <c r="J4" s="390"/>
+      <c r="J4" s="389"/>
       <c r="K4" s="73"/>
       <c r="L4" s="73"/>
     </row>
@@ -29216,12 +29223,12 @@
       <c r="H5" s="56" t="s">
         <v>89</v>
       </c>
-      <c r="I5" s="327" t="s">
+      <c r="I5" s="326" t="s">
         <v>418</v>
       </c>
-      <c r="J5" s="327"/>
-      <c r="K5" s="327"/>
-      <c r="L5" s="327"/>
+      <c r="J5" s="326"/>
+      <c r="K5" s="326"/>
+      <c r="L5" s="326"/>
     </row>
     <row r="6" spans="1:12" ht="20.25" customHeight="1">
       <c r="B6" t="s">
@@ -29230,10 +29237,10 @@
       <c r="H6" s="56" t="s">
         <v>90</v>
       </c>
-      <c r="I6" s="327" t="s">
+      <c r="I6" s="326" t="s">
         <v>419</v>
       </c>
-      <c r="J6" s="327"/>
+      <c r="J6" s="326"/>
       <c r="K6" s="74"/>
       <c r="L6" s="74"/>
     </row>
@@ -29264,32 +29271,32 @@
       <c r="L8" s="13"/>
     </row>
     <row r="9" spans="1:12" ht="13.5" customHeight="1" thickBot="1">
-      <c r="J9" s="328" t="s">
+      <c r="J9" s="327" t="s">
         <v>132</v>
       </c>
-      <c r="K9" s="329" t="s">
+      <c r="K9" s="328" t="s">
         <v>140</v>
       </c>
-      <c r="L9" s="330"/>
+      <c r="L9" s="329"/>
     </row>
     <row r="10" spans="1:12">
       <c r="B10" s="50" t="s">
         <v>55</v>
       </c>
-      <c r="C10" s="324" t="s">
+      <c r="C10" s="323" t="s">
         <v>56</v>
       </c>
-      <c r="D10" s="325"/>
-      <c r="E10" s="326"/>
+      <c r="D10" s="324"/>
+      <c r="E10" s="325"/>
       <c r="F10" s="50" t="s">
         <v>55</v>
       </c>
-      <c r="G10" s="324" t="s">
+      <c r="G10" s="323" t="s">
         <v>56</v>
       </c>
-      <c r="H10" s="325"/>
+      <c r="H10" s="324"/>
       <c r="I10" s="13"/>
-      <c r="J10" s="328"/>
+      <c r="J10" s="327"/>
       <c r="K10" s="9" t="s">
         <v>141</v>
       </c>
@@ -29301,14 +29308,14 @@
       <c r="B11" s="221" t="s">
         <v>417</v>
       </c>
-      <c r="C11" s="388" t="s">
+      <c r="C11" s="387" t="s">
         <v>69</v>
       </c>
-      <c r="D11" s="389"/>
-      <c r="E11" s="326"/>
+      <c r="D11" s="388"/>
+      <c r="E11" s="325"/>
       <c r="F11" s="51"/>
-      <c r="G11" s="322"/>
-      <c r="H11" s="323"/>
+      <c r="G11" s="321"/>
+      <c r="H11" s="322"/>
       <c r="I11" s="13"/>
       <c r="J11" s="9"/>
       <c r="K11" s="10"/>
@@ -30074,10 +30081,10 @@
       <c r="L33" s="9"/>
     </row>
     <row r="34" spans="1:12" ht="16.5" customHeight="1">
-      <c r="A34" s="391" t="s">
+      <c r="A34" s="390" t="s">
         <v>392</v>
       </c>
-      <c r="B34" s="391"/>
+      <c r="B34" s="390"/>
       <c r="C34" s="67"/>
       <c r="D34" s="222"/>
       <c r="E34" s="219"/>
@@ -30094,27 +30101,27 @@
     </row>
     <row r="35" spans="1:12" ht="13.5" customHeight="1"/>
     <row r="36" spans="1:12">
-      <c r="A36" s="329" t="s">
+      <c r="A36" s="328" t="s">
         <v>95</v>
       </c>
-      <c r="B36" s="330"/>
-      <c r="C36" s="394" t="s">
+      <c r="B36" s="329"/>
+      <c r="C36" s="393" t="s">
         <v>93</v>
       </c>
-      <c r="D36" s="395"/>
-      <c r="E36" s="329" t="s">
+      <c r="D36" s="394"/>
+      <c r="E36" s="328" t="s">
         <v>221</v>
       </c>
-      <c r="F36" s="330"/>
-      <c r="G36" s="328" t="s">
+      <c r="F36" s="329"/>
+      <c r="G36" s="327" t="s">
         <v>231</v>
       </c>
-      <c r="H36" s="328"/>
-      <c r="I36" s="328"/>
-      <c r="J36" s="392" t="s">
+      <c r="H36" s="327"/>
+      <c r="I36" s="327"/>
+      <c r="J36" s="391" t="s">
         <v>230</v>
       </c>
-      <c r="K36" s="393"/>
+      <c r="K36" s="392"/>
     </row>
     <row r="37" spans="1:12">
       <c r="A37" s="65"/>
@@ -30175,11 +30182,11 @@
         <v>88</v>
       </c>
       <c r="F41" s="68"/>
-      <c r="G41" s="318" t="s">
+      <c r="G41" s="317" t="s">
         <v>88</v>
       </c>
-      <c r="H41" s="319"/>
-      <c r="I41" s="320"/>
+      <c r="H41" s="318"/>
+      <c r="I41" s="319"/>
       <c r="J41" s="67" t="s">
         <v>88</v>
       </c>
@@ -30187,16 +30194,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="K9:L9"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="A3:L3"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="I6:J6"/>
     <mergeCell ref="G41:I41"/>
     <mergeCell ref="J36:K36"/>
     <mergeCell ref="C11:D11"/>
@@ -30206,6 +30203,16 @@
     <mergeCell ref="C36:D36"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="G36:I36"/>
+    <mergeCell ref="A3:L3"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="G10:H10"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.5" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="70" orientation="portrait" r:id="rId1"/>
@@ -30221,7 +30228,7 @@
   <dimension ref="A1:M27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="A3" sqref="A3:M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -30245,7 +30252,7 @@
       <c r="A1" s="227" t="s">
         <v>142</v>
       </c>
-      <c r="I1" s="253" t="s">
+      <c r="I1" s="252" t="s">
         <v>429</v>
       </c>
       <c r="J1" s="228" t="s">
@@ -30258,28 +30265,28 @@
       </c>
     </row>
     <row r="3" spans="1:13" ht="25.5">
-      <c r="A3" s="405" t="s">
+      <c r="A3" s="396" t="s">
         <v>229</v>
       </c>
-      <c r="B3" s="405"/>
-      <c r="C3" s="405"/>
-      <c r="D3" s="405"/>
-      <c r="E3" s="405"/>
-      <c r="F3" s="405"/>
-      <c r="G3" s="405"/>
-      <c r="H3" s="405"/>
-      <c r="I3" s="405"/>
-      <c r="J3" s="405"/>
-      <c r="K3" s="405"/>
-      <c r="L3" s="405"/>
-      <c r="M3" s="405"/>
+      <c r="B3" s="396"/>
+      <c r="C3" s="396"/>
+      <c r="D3" s="396"/>
+      <c r="E3" s="396"/>
+      <c r="F3" s="396"/>
+      <c r="G3" s="396"/>
+      <c r="H3" s="396"/>
+      <c r="I3" s="396"/>
+      <c r="J3" s="396"/>
+      <c r="K3" s="396"/>
+      <c r="L3" s="396"/>
+      <c r="M3" s="396"/>
     </row>
     <row r="4" spans="1:13" ht="20.100000000000001" customHeight="1">
       <c r="I4" s="230" t="s">
         <v>88</v>
       </c>
-      <c r="J4" s="406"/>
-      <c r="K4" s="406"/>
+      <c r="J4" s="397"/>
+      <c r="K4" s="397"/>
       <c r="L4" s="231"/>
       <c r="M4" s="231"/>
     </row>
@@ -30287,19 +30294,19 @@
       <c r="I5" s="230" t="s">
         <v>89</v>
       </c>
-      <c r="J5" s="407"/>
-      <c r="K5" s="407"/>
-      <c r="L5" s="404"/>
-      <c r="M5" s="404"/>
+      <c r="J5" s="398"/>
+      <c r="K5" s="398"/>
+      <c r="L5" s="395"/>
+      <c r="M5" s="395"/>
     </row>
     <row r="6" spans="1:13" ht="20.25" customHeight="1">
       <c r="I6" s="230" t="s">
         <v>90</v>
       </c>
-      <c r="J6" s="407" t="s">
+      <c r="J6" s="398" t="s">
         <v>423</v>
       </c>
-      <c r="K6" s="407"/>
+      <c r="K6" s="398"/>
       <c r="L6" s="232"/>
       <c r="M6" s="232"/>
     </row>
@@ -30307,13 +30314,13 @@
       <c r="I7" s="230" t="s">
         <v>91</v>
       </c>
-      <c r="J7" s="404"/>
-      <c r="K7" s="404"/>
-      <c r="L7" s="404"/>
+      <c r="J7" s="395"/>
+      <c r="K7" s="395"/>
+      <c r="L7" s="395"/>
       <c r="M7" s="232"/>
     </row>
     <row r="8" spans="1:13" ht="20.25" customHeight="1">
-      <c r="E8" s="254" t="s">
+      <c r="E8" s="253" t="s">
         <v>430</v>
       </c>
       <c r="I8" s="233"/>
@@ -30323,33 +30330,33 @@
       <c r="M8" s="234"/>
     </row>
     <row r="9" spans="1:13" ht="13.5" customHeight="1">
-      <c r="K9" s="402"/>
-      <c r="L9" s="403"/>
-      <c r="M9" s="403"/>
+      <c r="K9" s="405"/>
+      <c r="L9" s="406"/>
+      <c r="M9" s="406"/>
     </row>
     <row r="10" spans="1:13">
       <c r="B10" s="234"/>
-      <c r="C10" s="403"/>
-      <c r="D10" s="403"/>
-      <c r="E10" s="402"/>
+      <c r="C10" s="406"/>
+      <c r="D10" s="406"/>
+      <c r="E10" s="405"/>
       <c r="F10" s="235"/>
       <c r="G10" s="234"/>
-      <c r="H10" s="403"/>
-      <c r="I10" s="403"/>
+      <c r="H10" s="406"/>
+      <c r="I10" s="406"/>
       <c r="J10" s="234"/>
-      <c r="K10" s="402"/>
+      <c r="K10" s="405"/>
       <c r="L10" s="234"/>
       <c r="M10" s="236"/>
     </row>
     <row r="11" spans="1:13" ht="26.25" customHeight="1">
       <c r="B11" s="235"/>
-      <c r="C11" s="402"/>
-      <c r="D11" s="402"/>
-      <c r="E11" s="402"/>
+      <c r="C11" s="405"/>
+      <c r="D11" s="405"/>
+      <c r="E11" s="405"/>
       <c r="F11" s="235"/>
       <c r="G11" s="235"/>
-      <c r="H11" s="402"/>
-      <c r="I11" s="402"/>
+      <c r="H11" s="405"/>
+      <c r="I11" s="405"/>
       <c r="J11" s="234"/>
       <c r="K11" s="234"/>
     </row>
@@ -30367,10 +30374,10 @@
       <c r="D13" s="238" t="s">
         <v>425</v>
       </c>
-      <c r="E13" s="396" t="s">
+      <c r="E13" s="399" t="s">
         <v>51</v>
       </c>
-      <c r="F13" s="397"/>
+      <c r="F13" s="400"/>
       <c r="G13" s="238" t="s">
         <v>52</v>
       </c>
@@ -30397,62 +30404,56 @@
       <c r="A14" s="237"/>
       <c r="B14" s="239"/>
       <c r="C14" s="239"/>
-      <c r="D14" s="240"/>
-      <c r="E14" s="398"/>
-      <c r="F14" s="399"/>
-      <c r="G14" s="241"/>
-      <c r="H14" s="242"/>
+      <c r="D14" s="421"/>
+      <c r="E14" s="401"/>
+      <c r="F14" s="402"/>
+      <c r="G14" s="240"/>
+      <c r="H14" s="241"/>
       <c r="I14" s="422"/>
-      <c r="J14" s="243"/>
-      <c r="K14" s="244"/>
-      <c r="L14" s="245" t="s">
+      <c r="J14" s="242"/>
+      <c r="K14" s="243"/>
+      <c r="L14" s="244" t="s">
         <v>430</v>
       </c>
-      <c r="M14" s="246"/>
+      <c r="M14" s="245"/>
     </row>
     <row r="15" spans="1:13" ht="16.5" customHeight="1">
-      <c r="A15" s="400" t="s">
+      <c r="A15" s="403" t="s">
         <v>392</v>
       </c>
-      <c r="B15" s="401"/>
-      <c r="C15" s="401"/>
-      <c r="D15" s="401"/>
-      <c r="E15" s="247"/>
-      <c r="F15" s="247"/>
-      <c r="G15" s="247"/>
-      <c r="H15" s="248"/>
-      <c r="I15" s="248"/>
-      <c r="J15" s="248"/>
-      <c r="K15" s="249">
+      <c r="B15" s="404"/>
+      <c r="C15" s="404"/>
+      <c r="D15" s="404"/>
+      <c r="E15" s="246"/>
+      <c r="F15" s="246"/>
+      <c r="G15" s="246"/>
+      <c r="H15" s="247"/>
+      <c r="I15" s="247"/>
+      <c r="J15" s="247"/>
+      <c r="K15" s="248">
         <f>SUM(K14:K14)</f>
         <v>0</v>
       </c>
-      <c r="L15" s="248"/>
-      <c r="M15" s="250"/>
+      <c r="L15" s="247"/>
+      <c r="M15" s="249"/>
     </row>
     <row r="16" spans="1:13" ht="13.5" customHeight="1"/>
     <row r="26" spans="4:5">
-      <c r="D26" s="251" t="s">
+      <c r="D26" s="250" t="s">
         <v>426</v>
       </c>
-      <c r="E26" s="252" t="s">
+      <c r="E26" s="251" t="s">
         <v>427</v>
       </c>
     </row>
     <row r="27" spans="4:5">
-      <c r="D27" s="252"/>
-      <c r="E27" s="252" t="s">
+      <c r="D27" s="251"/>
+      <c r="E27" s="251" t="s">
         <v>428</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="J7:L7"/>
-    <mergeCell ref="A3:M3"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="L5:M5"/>
-    <mergeCell ref="J6:K6"/>
     <mergeCell ref="E13:F13"/>
     <mergeCell ref="E14:F14"/>
     <mergeCell ref="A15:D15"/>
@@ -30463,6 +30464,12 @@
     <mergeCell ref="H10:I10"/>
     <mergeCell ref="C11:D11"/>
     <mergeCell ref="H11:I11"/>
+    <mergeCell ref="J7:L7"/>
+    <mergeCell ref="A3:M3"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="J6:K6"/>
   </mergeCells>
   <pageMargins left="0.1" right="0.1" top="0.2" bottom="0.2" header="0.1" footer="0.1"/>
   <pageSetup paperSize="9" scale="71" fitToHeight="0" orientation="portrait" r:id="rId1"/>
@@ -30479,7 +30486,7 @@
   <dimension ref="A1:M27"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="A3" sqref="A3:M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -30503,7 +30510,7 @@
       <c r="A1" s="227" t="s">
         <v>142</v>
       </c>
-      <c r="I1" s="253" t="s">
+      <c r="I1" s="252" t="s">
         <v>429</v>
       </c>
       <c r="J1" s="228" t="s">
@@ -30516,28 +30523,28 @@
       </c>
     </row>
     <row r="3" spans="1:13" ht="25.5">
-      <c r="A3" s="405" t="s">
+      <c r="A3" s="396" t="s">
         <v>229</v>
       </c>
-      <c r="B3" s="405"/>
-      <c r="C3" s="405"/>
-      <c r="D3" s="405"/>
-      <c r="E3" s="405"/>
-      <c r="F3" s="405"/>
-      <c r="G3" s="405"/>
-      <c r="H3" s="405"/>
-      <c r="I3" s="405"/>
-      <c r="J3" s="405"/>
-      <c r="K3" s="405"/>
-      <c r="L3" s="405"/>
-      <c r="M3" s="405"/>
+      <c r="B3" s="396"/>
+      <c r="C3" s="396"/>
+      <c r="D3" s="396"/>
+      <c r="E3" s="396"/>
+      <c r="F3" s="396"/>
+      <c r="G3" s="396"/>
+      <c r="H3" s="396"/>
+      <c r="I3" s="396"/>
+      <c r="J3" s="396"/>
+      <c r="K3" s="396"/>
+      <c r="L3" s="396"/>
+      <c r="M3" s="396"/>
     </row>
     <row r="4" spans="1:13" ht="20.100000000000001" customHeight="1">
       <c r="I4" s="230" t="s">
         <v>88</v>
       </c>
-      <c r="J4" s="406"/>
-      <c r="K4" s="406"/>
+      <c r="J4" s="397"/>
+      <c r="K4" s="397"/>
       <c r="L4" s="231"/>
       <c r="M4" s="231"/>
     </row>
@@ -30545,19 +30552,19 @@
       <c r="I5" s="230" t="s">
         <v>89</v>
       </c>
-      <c r="J5" s="407"/>
-      <c r="K5" s="407"/>
-      <c r="L5" s="404"/>
-      <c r="M5" s="404"/>
+      <c r="J5" s="398"/>
+      <c r="K5" s="398"/>
+      <c r="L5" s="395"/>
+      <c r="M5" s="395"/>
     </row>
     <row r="6" spans="1:13" ht="20.25" customHeight="1">
       <c r="I6" s="230" t="s">
         <v>90</v>
       </c>
-      <c r="J6" s="407" t="s">
+      <c r="J6" s="398" t="s">
         <v>423</v>
       </c>
-      <c r="K6" s="407"/>
+      <c r="K6" s="398"/>
       <c r="L6" s="232"/>
       <c r="M6" s="232"/>
     </row>
@@ -30565,13 +30572,13 @@
       <c r="I7" s="230" t="s">
         <v>91</v>
       </c>
-      <c r="J7" s="404"/>
-      <c r="K7" s="404"/>
-      <c r="L7" s="404"/>
+      <c r="J7" s="395"/>
+      <c r="K7" s="395"/>
+      <c r="L7" s="395"/>
       <c r="M7" s="232"/>
     </row>
     <row r="8" spans="1:13" ht="20.25" customHeight="1">
-      <c r="E8" s="254" t="s">
+      <c r="E8" s="253" t="s">
         <v>430</v>
       </c>
       <c r="I8" s="233"/>
@@ -30581,33 +30588,33 @@
       <c r="M8" s="234"/>
     </row>
     <row r="9" spans="1:13" ht="13.5" customHeight="1">
-      <c r="K9" s="402"/>
-      <c r="L9" s="403"/>
-      <c r="M9" s="403"/>
+      <c r="K9" s="405"/>
+      <c r="L9" s="406"/>
+      <c r="M9" s="406"/>
     </row>
     <row r="10" spans="1:13">
       <c r="B10" s="234"/>
-      <c r="C10" s="403"/>
-      <c r="D10" s="403"/>
-      <c r="E10" s="402"/>
+      <c r="C10" s="406"/>
+      <c r="D10" s="406"/>
+      <c r="E10" s="405"/>
       <c r="F10" s="235"/>
       <c r="G10" s="234"/>
-      <c r="H10" s="403"/>
-      <c r="I10" s="403"/>
+      <c r="H10" s="406"/>
+      <c r="I10" s="406"/>
       <c r="J10" s="234"/>
-      <c r="K10" s="402"/>
+      <c r="K10" s="405"/>
       <c r="L10" s="234"/>
       <c r="M10" s="236"/>
     </row>
     <row r="11" spans="1:13" ht="26.25" customHeight="1">
       <c r="B11" s="235"/>
-      <c r="C11" s="402"/>
-      <c r="D11" s="402"/>
-      <c r="E11" s="402"/>
+      <c r="C11" s="405"/>
+      <c r="D11" s="405"/>
+      <c r="E11" s="405"/>
       <c r="F11" s="235"/>
       <c r="G11" s="235"/>
-      <c r="H11" s="402"/>
-      <c r="I11" s="402"/>
+      <c r="H11" s="405"/>
+      <c r="I11" s="405"/>
       <c r="J11" s="234"/>
       <c r="K11" s="234"/>
     </row>
@@ -30625,10 +30632,10 @@
       <c r="D13" s="238" t="s">
         <v>425</v>
       </c>
-      <c r="E13" s="396" t="s">
+      <c r="E13" s="399" t="s">
         <v>51</v>
       </c>
-      <c r="F13" s="397"/>
+      <c r="F13" s="400"/>
       <c r="G13" s="238" t="s">
         <v>52</v>
       </c>
@@ -30655,56 +30662,62 @@
       <c r="A14" s="237"/>
       <c r="B14" s="239"/>
       <c r="C14" s="239"/>
-      <c r="D14" s="240"/>
-      <c r="E14" s="398"/>
-      <c r="F14" s="399"/>
-      <c r="G14" s="241"/>
-      <c r="H14" s="242"/>
+      <c r="D14" s="421"/>
+      <c r="E14" s="401"/>
+      <c r="F14" s="402"/>
+      <c r="G14" s="240"/>
+      <c r="H14" s="241"/>
       <c r="I14" s="422"/>
-      <c r="J14" s="243"/>
-      <c r="K14" s="244"/>
-      <c r="L14" s="245" t="s">
+      <c r="J14" s="242"/>
+      <c r="K14" s="243"/>
+      <c r="L14" s="244" t="s">
         <v>430</v>
       </c>
-      <c r="M14" s="246"/>
+      <c r="M14" s="245"/>
     </row>
     <row r="15" spans="1:13" ht="16.5" customHeight="1">
-      <c r="A15" s="400" t="s">
+      <c r="A15" s="403" t="s">
         <v>392</v>
       </c>
-      <c r="B15" s="401"/>
-      <c r="C15" s="401"/>
-      <c r="D15" s="401"/>
-      <c r="E15" s="247"/>
-      <c r="F15" s="247"/>
-      <c r="G15" s="247"/>
-      <c r="H15" s="248"/>
-      <c r="I15" s="248"/>
-      <c r="J15" s="248"/>
-      <c r="K15" s="249">
+      <c r="B15" s="404"/>
+      <c r="C15" s="404"/>
+      <c r="D15" s="404"/>
+      <c r="E15" s="246"/>
+      <c r="F15" s="246"/>
+      <c r="G15" s="246"/>
+      <c r="H15" s="247"/>
+      <c r="I15" s="247"/>
+      <c r="J15" s="247"/>
+      <c r="K15" s="248">
         <f>SUM(K14:K14)</f>
         <v>0</v>
       </c>
-      <c r="L15" s="248"/>
-      <c r="M15" s="250"/>
+      <c r="L15" s="247"/>
+      <c r="M15" s="249"/>
     </row>
     <row r="16" spans="1:13" ht="13.5" customHeight="1"/>
     <row r="26" spans="4:5">
-      <c r="D26" s="251" t="s">
+      <c r="D26" s="250" t="s">
         <v>426</v>
       </c>
-      <c r="E26" s="252" t="s">
+      <c r="E26" s="251" t="s">
         <v>427</v>
       </c>
     </row>
     <row r="27" spans="4:5">
-      <c r="D27" s="252"/>
-      <c r="E27" s="252" t="s">
+      <c r="D27" s="251"/>
+      <c r="E27" s="251" t="s">
         <v>428</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="J7:L7"/>
+    <mergeCell ref="A3:M3"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="J6:K6"/>
     <mergeCell ref="E13:F13"/>
     <mergeCell ref="E14:F14"/>
     <mergeCell ref="A15:D15"/>
@@ -30715,12 +30728,6 @@
     <mergeCell ref="H10:I10"/>
     <mergeCell ref="C11:D11"/>
     <mergeCell ref="H11:I11"/>
-    <mergeCell ref="J7:L7"/>
-    <mergeCell ref="A3:M3"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="L5:M5"/>
-    <mergeCell ref="J6:K6"/>
   </mergeCells>
   <pageMargins left="0.1" right="0.1" top="0.2" bottom="0.2" header="0.1" footer="0.1"/>
   <pageSetup paperSize="9" scale="71" fitToHeight="0" orientation="portrait" r:id="rId1"/>
@@ -30772,32 +30779,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" s="419" t="s">
+      <c r="A1" s="407" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="419"/>
-      <c r="C1" s="419"/>
-      <c r="D1" s="419"/>
-      <c r="E1" s="419"/>
-      <c r="F1" s="419"/>
-      <c r="G1" s="419"/>
-      <c r="H1" s="419"/>
-      <c r="I1" s="419"/>
-      <c r="J1" s="419"/>
+      <c r="B1" s="407"/>
+      <c r="C1" s="407"/>
+      <c r="D1" s="407"/>
+      <c r="E1" s="407"/>
+      <c r="F1" s="407"/>
+      <c r="G1" s="407"/>
+      <c r="H1" s="407"/>
+      <c r="I1" s="407"/>
+      <c r="J1" s="407"/>
     </row>
     <row r="2" spans="1:10" ht="26.25">
-      <c r="A2" s="321" t="s">
+      <c r="A2" s="320" t="s">
         <v>123</v>
       </c>
-      <c r="B2" s="321"/>
-      <c r="C2" s="321"/>
-      <c r="D2" s="321"/>
-      <c r="E2" s="321"/>
-      <c r="F2" s="321"/>
-      <c r="G2" s="321"/>
-      <c r="H2" s="321"/>
-      <c r="I2" s="321"/>
-      <c r="J2" s="321"/>
+      <c r="B2" s="320"/>
+      <c r="C2" s="320"/>
+      <c r="D2" s="320"/>
+      <c r="E2" s="320"/>
+      <c r="F2" s="320"/>
+      <c r="G2" s="320"/>
+      <c r="H2" s="320"/>
+      <c r="I2" s="320"/>
+      <c r="J2" s="320"/>
     </row>
     <row r="3" spans="1:10" ht="20.25" customHeight="1">
       <c r="H3" s="56" t="s">
@@ -30813,8 +30820,8 @@
       <c r="H4" s="56" t="s">
         <v>89</v>
       </c>
-      <c r="I4" s="327"/>
-      <c r="J4" s="327"/>
+      <c r="I4" s="326"/>
+      <c r="J4" s="326"/>
     </row>
     <row r="5" spans="1:10" ht="20.25" customHeight="1">
       <c r="B5" t="s">
@@ -30858,11 +30865,11 @@
       <c r="B10" s="53" t="s">
         <v>50</v>
       </c>
-      <c r="C10" s="420" t="s">
+      <c r="C10" s="408" t="s">
         <v>51</v>
       </c>
-      <c r="D10" s="420"/>
-      <c r="E10" s="420"/>
+      <c r="D10" s="408"/>
+      <c r="E10" s="408"/>
       <c r="F10" s="53" t="s">
         <v>52</v>
       </c>
@@ -30872,442 +30879,442 @@
       <c r="H10" s="53" t="s">
         <v>54</v>
       </c>
-      <c r="I10" s="420" t="s">
+      <c r="I10" s="408" t="s">
         <v>6</v>
       </c>
-      <c r="J10" s="421"/>
+      <c r="J10" s="409"/>
     </row>
     <row r="11" spans="1:10" ht="20.25" customHeight="1" thickTop="1">
       <c r="A11" s="69">
         <v>1</v>
       </c>
       <c r="B11" s="6"/>
-      <c r="C11" s="414"/>
-      <c r="D11" s="415"/>
-      <c r="E11" s="416"/>
+      <c r="C11" s="410"/>
+      <c r="D11" s="411"/>
+      <c r="E11" s="412"/>
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
       <c r="H11" s="6"/>
-      <c r="I11" s="417"/>
-      <c r="J11" s="418"/>
+      <c r="I11" s="413"/>
+      <c r="J11" s="414"/>
     </row>
     <row r="12" spans="1:10" ht="20.25" customHeight="1">
       <c r="A12" s="70">
         <v>2</v>
       </c>
       <c r="B12" s="10"/>
-      <c r="C12" s="318"/>
-      <c r="D12" s="319"/>
-      <c r="E12" s="320"/>
+      <c r="C12" s="317"/>
+      <c r="D12" s="318"/>
+      <c r="E12" s="319"/>
       <c r="F12" s="10"/>
       <c r="G12" s="10"/>
       <c r="H12" s="10"/>
-      <c r="I12" s="329"/>
-      <c r="J12" s="413"/>
+      <c r="I12" s="328"/>
+      <c r="J12" s="415"/>
     </row>
     <row r="13" spans="1:10" ht="20.25" customHeight="1">
       <c r="A13" s="69">
         <v>3</v>
       </c>
       <c r="B13" s="10"/>
-      <c r="C13" s="318"/>
-      <c r="D13" s="319"/>
-      <c r="E13" s="320"/>
+      <c r="C13" s="317"/>
+      <c r="D13" s="318"/>
+      <c r="E13" s="319"/>
       <c r="F13" s="10"/>
       <c r="G13" s="10"/>
       <c r="H13" s="10"/>
-      <c r="I13" s="329"/>
-      <c r="J13" s="413"/>
+      <c r="I13" s="328"/>
+      <c r="J13" s="415"/>
     </row>
     <row r="14" spans="1:10" ht="20.25" customHeight="1">
       <c r="A14" s="70">
         <v>4</v>
       </c>
       <c r="B14" s="10"/>
-      <c r="C14" s="318"/>
-      <c r="D14" s="319"/>
-      <c r="E14" s="320"/>
+      <c r="C14" s="317"/>
+      <c r="D14" s="318"/>
+      <c r="E14" s="319"/>
       <c r="F14" s="10"/>
       <c r="G14" s="10"/>
       <c r="H14" s="10"/>
-      <c r="I14" s="329"/>
-      <c r="J14" s="413"/>
+      <c r="I14" s="328"/>
+      <c r="J14" s="415"/>
     </row>
     <row r="15" spans="1:10" ht="20.25" customHeight="1">
       <c r="A15" s="69">
         <v>5</v>
       </c>
       <c r="B15" s="10"/>
-      <c r="C15" s="318"/>
-      <c r="D15" s="319"/>
-      <c r="E15" s="320"/>
+      <c r="C15" s="317"/>
+      <c r="D15" s="318"/>
+      <c r="E15" s="319"/>
       <c r="F15" s="10"/>
       <c r="G15" s="10"/>
       <c r="H15" s="10"/>
-      <c r="I15" s="329"/>
-      <c r="J15" s="413"/>
+      <c r="I15" s="328"/>
+      <c r="J15" s="415"/>
     </row>
     <row r="16" spans="1:10" ht="20.25" customHeight="1">
       <c r="A16" s="70">
         <v>6</v>
       </c>
       <c r="B16" s="10"/>
-      <c r="C16" s="318"/>
-      <c r="D16" s="319"/>
-      <c r="E16" s="320"/>
+      <c r="C16" s="317"/>
+      <c r="D16" s="318"/>
+      <c r="E16" s="319"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
       <c r="H16" s="10"/>
-      <c r="I16" s="329"/>
-      <c r="J16" s="413"/>
+      <c r="I16" s="328"/>
+      <c r="J16" s="415"/>
     </row>
     <row r="17" spans="1:10" ht="20.25" customHeight="1">
       <c r="A17" s="69">
         <v>7</v>
       </c>
       <c r="B17" s="10"/>
-      <c r="C17" s="318"/>
-      <c r="D17" s="319"/>
-      <c r="E17" s="320"/>
+      <c r="C17" s="317"/>
+      <c r="D17" s="318"/>
+      <c r="E17" s="319"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
       <c r="H17" s="10"/>
-      <c r="I17" s="329"/>
-      <c r="J17" s="413"/>
+      <c r="I17" s="328"/>
+      <c r="J17" s="415"/>
     </row>
     <row r="18" spans="1:10" ht="20.25" customHeight="1">
       <c r="A18" s="70">
         <v>8</v>
       </c>
       <c r="B18" s="10"/>
-      <c r="C18" s="318"/>
-      <c r="D18" s="319"/>
-      <c r="E18" s="320"/>
+      <c r="C18" s="317"/>
+      <c r="D18" s="318"/>
+      <c r="E18" s="319"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
       <c r="H18" s="10"/>
-      <c r="I18" s="329"/>
-      <c r="J18" s="413"/>
+      <c r="I18" s="328"/>
+      <c r="J18" s="415"/>
     </row>
     <row r="19" spans="1:10" ht="20.25" customHeight="1">
       <c r="A19" s="69">
         <v>9</v>
       </c>
       <c r="B19" s="10"/>
-      <c r="C19" s="318"/>
-      <c r="D19" s="319"/>
-      <c r="E19" s="320"/>
+      <c r="C19" s="317"/>
+      <c r="D19" s="318"/>
+      <c r="E19" s="319"/>
       <c r="F19" s="10"/>
       <c r="G19" s="10"/>
       <c r="H19" s="10"/>
-      <c r="I19" s="329"/>
-      <c r="J19" s="413"/>
+      <c r="I19" s="328"/>
+      <c r="J19" s="415"/>
     </row>
     <row r="20" spans="1:10" ht="20.25" customHeight="1">
       <c r="A20" s="70">
         <v>10</v>
       </c>
       <c r="B20" s="10"/>
-      <c r="C20" s="318"/>
-      <c r="D20" s="319"/>
-      <c r="E20" s="320"/>
+      <c r="C20" s="317"/>
+      <c r="D20" s="318"/>
+      <c r="E20" s="319"/>
       <c r="F20" s="10"/>
       <c r="G20" s="10"/>
       <c r="H20" s="10"/>
-      <c r="I20" s="329"/>
-      <c r="J20" s="413"/>
+      <c r="I20" s="328"/>
+      <c r="J20" s="415"/>
     </row>
     <row r="21" spans="1:10" ht="20.25" customHeight="1">
       <c r="A21" s="69">
         <v>11</v>
       </c>
       <c r="B21" s="10"/>
-      <c r="C21" s="318"/>
-      <c r="D21" s="319"/>
-      <c r="E21" s="320"/>
+      <c r="C21" s="317"/>
+      <c r="D21" s="318"/>
+      <c r="E21" s="319"/>
       <c r="F21" s="10"/>
       <c r="G21" s="10"/>
       <c r="H21" s="10"/>
-      <c r="I21" s="329"/>
-      <c r="J21" s="413"/>
+      <c r="I21" s="328"/>
+      <c r="J21" s="415"/>
     </row>
     <row r="22" spans="1:10" ht="20.25" customHeight="1">
       <c r="A22" s="70">
         <v>12</v>
       </c>
       <c r="B22" s="10"/>
-      <c r="C22" s="318"/>
-      <c r="D22" s="319"/>
-      <c r="E22" s="320"/>
+      <c r="C22" s="317"/>
+      <c r="D22" s="318"/>
+      <c r="E22" s="319"/>
       <c r="F22" s="10"/>
       <c r="G22" s="10"/>
       <c r="H22" s="10"/>
-      <c r="I22" s="329"/>
-      <c r="J22" s="413"/>
+      <c r="I22" s="328"/>
+      <c r="J22" s="415"/>
     </row>
     <row r="23" spans="1:10" ht="20.25" customHeight="1">
       <c r="A23" s="69">
         <v>13</v>
       </c>
       <c r="B23" s="10"/>
-      <c r="C23" s="318"/>
-      <c r="D23" s="319"/>
-      <c r="E23" s="320"/>
+      <c r="C23" s="317"/>
+      <c r="D23" s="318"/>
+      <c r="E23" s="319"/>
       <c r="F23" s="10"/>
       <c r="G23" s="10"/>
       <c r="H23" s="10"/>
-      <c r="I23" s="329"/>
-      <c r="J23" s="413"/>
+      <c r="I23" s="328"/>
+      <c r="J23" s="415"/>
     </row>
     <row r="24" spans="1:10" ht="20.25" customHeight="1">
       <c r="A24" s="70">
         <v>14</v>
       </c>
       <c r="B24" s="10"/>
-      <c r="C24" s="318"/>
-      <c r="D24" s="319"/>
-      <c r="E24" s="320"/>
+      <c r="C24" s="317"/>
+      <c r="D24" s="318"/>
+      <c r="E24" s="319"/>
       <c r="F24" s="10"/>
       <c r="G24" s="10"/>
       <c r="H24" s="10"/>
-      <c r="I24" s="329"/>
-      <c r="J24" s="413"/>
+      <c r="I24" s="328"/>
+      <c r="J24" s="415"/>
     </row>
     <row r="25" spans="1:10" ht="20.25" customHeight="1">
       <c r="A25" s="69">
         <v>15</v>
       </c>
       <c r="B25" s="10"/>
-      <c r="C25" s="318"/>
-      <c r="D25" s="319"/>
-      <c r="E25" s="320"/>
+      <c r="C25" s="317"/>
+      <c r="D25" s="318"/>
+      <c r="E25" s="319"/>
       <c r="F25" s="10"/>
       <c r="G25" s="10"/>
       <c r="H25" s="10"/>
-      <c r="I25" s="329"/>
-      <c r="J25" s="413"/>
+      <c r="I25" s="328"/>
+      <c r="J25" s="415"/>
     </row>
     <row r="26" spans="1:10" ht="20.25" customHeight="1">
       <c r="A26" s="70">
         <v>16</v>
       </c>
       <c r="B26" s="10"/>
-      <c r="C26" s="318"/>
-      <c r="D26" s="319"/>
-      <c r="E26" s="320"/>
+      <c r="C26" s="317"/>
+      <c r="D26" s="318"/>
+      <c r="E26" s="319"/>
       <c r="F26" s="10"/>
       <c r="G26" s="10"/>
       <c r="H26" s="10"/>
-      <c r="I26" s="329"/>
-      <c r="J26" s="413"/>
+      <c r="I26" s="328"/>
+      <c r="J26" s="415"/>
     </row>
     <row r="27" spans="1:10" ht="20.25" customHeight="1">
       <c r="A27" s="69">
         <v>17</v>
       </c>
       <c r="B27" s="10"/>
-      <c r="C27" s="318"/>
-      <c r="D27" s="319"/>
-      <c r="E27" s="320"/>
+      <c r="C27" s="317"/>
+      <c r="D27" s="318"/>
+      <c r="E27" s="319"/>
       <c r="F27" s="10"/>
       <c r="G27" s="10"/>
       <c r="H27" s="10"/>
-      <c r="I27" s="329"/>
-      <c r="J27" s="413"/>
+      <c r="I27" s="328"/>
+      <c r="J27" s="415"/>
     </row>
     <row r="28" spans="1:10" ht="20.25" customHeight="1">
       <c r="A28" s="70">
         <v>18</v>
       </c>
       <c r="B28" s="10"/>
-      <c r="C28" s="318"/>
-      <c r="D28" s="319"/>
-      <c r="E28" s="320"/>
+      <c r="C28" s="317"/>
+      <c r="D28" s="318"/>
+      <c r="E28" s="319"/>
       <c r="F28" s="10"/>
       <c r="G28" s="10"/>
       <c r="H28" s="10"/>
-      <c r="I28" s="329"/>
-      <c r="J28" s="413"/>
+      <c r="I28" s="328"/>
+      <c r="J28" s="415"/>
     </row>
     <row r="29" spans="1:10" ht="20.25" customHeight="1">
       <c r="A29" s="69">
         <v>19</v>
       </c>
       <c r="B29" s="10"/>
-      <c r="C29" s="318"/>
-      <c r="D29" s="319"/>
-      <c r="E29" s="320"/>
+      <c r="C29" s="317"/>
+      <c r="D29" s="318"/>
+      <c r="E29" s="319"/>
       <c r="F29" s="10"/>
       <c r="G29" s="10"/>
       <c r="H29" s="10"/>
-      <c r="I29" s="329"/>
-      <c r="J29" s="413"/>
+      <c r="I29" s="328"/>
+      <c r="J29" s="415"/>
     </row>
     <row r="30" spans="1:10" ht="20.25" customHeight="1">
       <c r="A30" s="70">
         <v>20</v>
       </c>
       <c r="B30" s="10"/>
-      <c r="C30" s="318"/>
-      <c r="D30" s="319"/>
-      <c r="E30" s="320"/>
+      <c r="C30" s="317"/>
+      <c r="D30" s="318"/>
+      <c r="E30" s="319"/>
       <c r="F30" s="10"/>
       <c r="G30" s="10"/>
       <c r="H30" s="10"/>
-      <c r="I30" s="329"/>
-      <c r="J30" s="413"/>
+      <c r="I30" s="328"/>
+      <c r="J30" s="415"/>
     </row>
     <row r="31" spans="1:10" ht="20.25" customHeight="1">
       <c r="A31" s="69">
         <v>21</v>
       </c>
       <c r="B31" s="10"/>
-      <c r="C31" s="318"/>
-      <c r="D31" s="319"/>
-      <c r="E31" s="320"/>
+      <c r="C31" s="317"/>
+      <c r="D31" s="318"/>
+      <c r="E31" s="319"/>
       <c r="F31" s="10"/>
       <c r="G31" s="10"/>
       <c r="H31" s="10"/>
-      <c r="I31" s="329"/>
-      <c r="J31" s="413"/>
+      <c r="I31" s="328"/>
+      <c r="J31" s="415"/>
     </row>
     <row r="32" spans="1:10" ht="20.25" customHeight="1">
       <c r="A32" s="70">
         <v>22</v>
       </c>
       <c r="B32" s="10"/>
-      <c r="C32" s="318"/>
-      <c r="D32" s="319"/>
-      <c r="E32" s="320"/>
+      <c r="C32" s="317"/>
+      <c r="D32" s="318"/>
+      <c r="E32" s="319"/>
       <c r="F32" s="10"/>
       <c r="G32" s="10"/>
       <c r="H32" s="10"/>
-      <c r="I32" s="329"/>
-      <c r="J32" s="413"/>
+      <c r="I32" s="328"/>
+      <c r="J32" s="415"/>
     </row>
     <row r="33" spans="1:10" ht="20.25" customHeight="1">
       <c r="A33" s="69">
         <v>23</v>
       </c>
       <c r="B33" s="10"/>
-      <c r="C33" s="318"/>
-      <c r="D33" s="319"/>
-      <c r="E33" s="320"/>
+      <c r="C33" s="317"/>
+      <c r="D33" s="318"/>
+      <c r="E33" s="319"/>
       <c r="F33" s="10"/>
       <c r="G33" s="10"/>
       <c r="H33" s="10"/>
-      <c r="I33" s="329"/>
-      <c r="J33" s="413"/>
+      <c r="I33" s="328"/>
+      <c r="J33" s="415"/>
     </row>
     <row r="34" spans="1:10" ht="20.25" customHeight="1">
       <c r="A34" s="70">
         <v>24</v>
       </c>
       <c r="B34" s="10"/>
-      <c r="C34" s="318"/>
-      <c r="D34" s="319"/>
-      <c r="E34" s="320"/>
+      <c r="C34" s="317"/>
+      <c r="D34" s="318"/>
+      <c r="E34" s="319"/>
       <c r="F34" s="10"/>
       <c r="G34" s="10"/>
       <c r="H34" s="10"/>
-      <c r="I34" s="329"/>
-      <c r="J34" s="413"/>
+      <c r="I34" s="328"/>
+      <c r="J34" s="415"/>
     </row>
     <row r="35" spans="1:10" ht="20.25" customHeight="1">
       <c r="A35" s="69">
         <v>25</v>
       </c>
       <c r="B35" s="10"/>
-      <c r="C35" s="318"/>
-      <c r="D35" s="319"/>
-      <c r="E35" s="320"/>
+      <c r="C35" s="317"/>
+      <c r="D35" s="318"/>
+      <c r="E35" s="319"/>
       <c r="F35" s="10"/>
       <c r="G35" s="10"/>
       <c r="H35" s="10"/>
-      <c r="I35" s="329"/>
-      <c r="J35" s="413"/>
+      <c r="I35" s="328"/>
+      <c r="J35" s="415"/>
     </row>
     <row r="36" spans="1:10" ht="20.25" customHeight="1">
       <c r="A36" s="69">
         <v>26</v>
       </c>
       <c r="B36" s="71"/>
-      <c r="C36" s="318"/>
-      <c r="D36" s="319"/>
-      <c r="E36" s="320"/>
+      <c r="C36" s="317"/>
+      <c r="D36" s="318"/>
+      <c r="E36" s="319"/>
       <c r="F36" s="71"/>
       <c r="G36" s="71"/>
       <c r="H36" s="71"/>
-      <c r="I36" s="329"/>
-      <c r="J36" s="413"/>
+      <c r="I36" s="328"/>
+      <c r="J36" s="415"/>
     </row>
     <row r="37" spans="1:10" ht="20.25" customHeight="1">
       <c r="A37" s="69">
         <v>27</v>
       </c>
       <c r="B37" s="71"/>
-      <c r="C37" s="318"/>
-      <c r="D37" s="319"/>
-      <c r="E37" s="320"/>
+      <c r="C37" s="317"/>
+      <c r="D37" s="318"/>
+      <c r="E37" s="319"/>
       <c r="F37" s="71"/>
       <c r="G37" s="71"/>
       <c r="H37" s="71"/>
-      <c r="I37" s="329"/>
-      <c r="J37" s="413"/>
+      <c r="I37" s="328"/>
+      <c r="J37" s="415"/>
     </row>
     <row r="38" spans="1:10" ht="20.25" customHeight="1">
       <c r="A38" s="69">
         <v>28</v>
       </c>
       <c r="B38" s="71"/>
-      <c r="C38" s="318"/>
-      <c r="D38" s="319"/>
-      <c r="E38" s="320"/>
+      <c r="C38" s="317"/>
+      <c r="D38" s="318"/>
+      <c r="E38" s="319"/>
       <c r="F38" s="71"/>
       <c r="G38" s="71"/>
       <c r="H38" s="71"/>
-      <c r="I38" s="329"/>
-      <c r="J38" s="413"/>
+      <c r="I38" s="328"/>
+      <c r="J38" s="415"/>
     </row>
     <row r="39" spans="1:10" ht="20.25" customHeight="1">
       <c r="A39" s="69">
         <v>29</v>
       </c>
       <c r="B39" s="71"/>
-      <c r="C39" s="318"/>
-      <c r="D39" s="319"/>
-      <c r="E39" s="320"/>
+      <c r="C39" s="317"/>
+      <c r="D39" s="318"/>
+      <c r="E39" s="319"/>
       <c r="F39" s="71"/>
       <c r="G39" s="71"/>
       <c r="H39" s="71"/>
-      <c r="I39" s="329"/>
-      <c r="J39" s="413"/>
+      <c r="I39" s="328"/>
+      <c r="J39" s="415"/>
     </row>
     <row r="40" spans="1:10" ht="20.25" customHeight="1">
       <c r="A40" s="69">
         <v>30</v>
       </c>
       <c r="B40" s="71"/>
-      <c r="C40" s="318"/>
-      <c r="D40" s="319"/>
-      <c r="E40" s="320"/>
+      <c r="C40" s="317"/>
+      <c r="D40" s="318"/>
+      <c r="E40" s="319"/>
       <c r="F40" s="71"/>
       <c r="G40" s="71"/>
       <c r="H40" s="71"/>
-      <c r="I40" s="329"/>
-      <c r="J40" s="413"/>
+      <c r="I40" s="328"/>
+      <c r="J40" s="415"/>
     </row>
     <row r="41" spans="1:10" ht="8.25" customHeight="1" thickBot="1">
       <c r="A41" s="54"/>
       <c r="B41" s="55"/>
-      <c r="C41" s="408"/>
-      <c r="D41" s="409"/>
-      <c r="E41" s="410"/>
+      <c r="C41" s="416"/>
+      <c r="D41" s="417"/>
+      <c r="E41" s="418"/>
       <c r="F41" s="55"/>
       <c r="G41" s="55"/>
       <c r="H41" s="55"/>
-      <c r="I41" s="411"/>
-      <c r="J41" s="412"/>
+      <c r="I41" s="419"/>
+      <c r="J41" s="420"/>
     </row>
     <row r="42" spans="1:10" ht="14.25" customHeight="1">
       <c r="C42" s="72"/>
@@ -31324,26 +31331,26 @@
       <c r="J43" s="13"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="329" t="s">
+      <c r="A45" s="328" t="s">
         <v>95</v>
       </c>
-      <c r="B45" s="330"/>
-      <c r="C45" s="329" t="s">
+      <c r="B45" s="329"/>
+      <c r="C45" s="328" t="s">
         <v>94</v>
       </c>
-      <c r="D45" s="330"/>
-      <c r="E45" s="329" t="s">
+      <c r="D45" s="329"/>
+      <c r="E45" s="328" t="s">
         <v>93</v>
       </c>
-      <c r="F45" s="330"/>
-      <c r="G45" s="329" t="s">
+      <c r="F45" s="329"/>
+      <c r="G45" s="328" t="s">
         <v>114</v>
       </c>
-      <c r="H45" s="330"/>
-      <c r="I45" s="329" t="s">
+      <c r="H45" s="329"/>
+      <c r="I45" s="328" t="s">
         <v>92</v>
       </c>
-      <c r="J45" s="330"/>
+      <c r="J45" s="329"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="65"/>
@@ -31417,71 +31424,6 @@
     </row>
   </sheetData>
   <mergeCells count="72">
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="C11:E11"/>
-    <mergeCell ref="I11:J11"/>
-    <mergeCell ref="C12:E12"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="C13:E13"/>
-    <mergeCell ref="I13:J13"/>
-    <mergeCell ref="C14:E14"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="C15:E15"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="C16:E16"/>
-    <mergeCell ref="I16:J16"/>
-    <mergeCell ref="C17:E17"/>
-    <mergeCell ref="I17:J17"/>
-    <mergeCell ref="C18:E18"/>
-    <mergeCell ref="I18:J18"/>
-    <mergeCell ref="C19:E19"/>
-    <mergeCell ref="I19:J19"/>
-    <mergeCell ref="C20:E20"/>
-    <mergeCell ref="I20:J20"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="C22:E22"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="C23:E23"/>
-    <mergeCell ref="I23:J23"/>
-    <mergeCell ref="C24:E24"/>
-    <mergeCell ref="I24:J24"/>
-    <mergeCell ref="C25:E25"/>
-    <mergeCell ref="I25:J25"/>
-    <mergeCell ref="C26:E26"/>
-    <mergeCell ref="I26:J26"/>
-    <mergeCell ref="C27:E27"/>
-    <mergeCell ref="I27:J27"/>
-    <mergeCell ref="C28:E28"/>
-    <mergeCell ref="I28:J28"/>
-    <mergeCell ref="C29:E29"/>
-    <mergeCell ref="I29:J29"/>
-    <mergeCell ref="C30:E30"/>
-    <mergeCell ref="I30:J30"/>
-    <mergeCell ref="C31:E31"/>
-    <mergeCell ref="I31:J31"/>
-    <mergeCell ref="C32:E32"/>
-    <mergeCell ref="I32:J32"/>
-    <mergeCell ref="C33:E33"/>
-    <mergeCell ref="I33:J33"/>
-    <mergeCell ref="C34:E34"/>
-    <mergeCell ref="I34:J34"/>
-    <mergeCell ref="C35:E35"/>
-    <mergeCell ref="I35:J35"/>
-    <mergeCell ref="C36:E36"/>
-    <mergeCell ref="I36:J36"/>
-    <mergeCell ref="C37:E37"/>
-    <mergeCell ref="I37:J37"/>
-    <mergeCell ref="C38:E38"/>
-    <mergeCell ref="I38:J38"/>
-    <mergeCell ref="C39:E39"/>
-    <mergeCell ref="I39:J39"/>
-    <mergeCell ref="C40:E40"/>
-    <mergeCell ref="I40:J40"/>
     <mergeCell ref="C41:E41"/>
     <mergeCell ref="I41:J41"/>
     <mergeCell ref="A45:B45"/>
@@ -31489,6 +31431,71 @@
     <mergeCell ref="E45:F45"/>
     <mergeCell ref="G45:H45"/>
     <mergeCell ref="I45:J45"/>
+    <mergeCell ref="C38:E38"/>
+    <mergeCell ref="I38:J38"/>
+    <mergeCell ref="C39:E39"/>
+    <mergeCell ref="I39:J39"/>
+    <mergeCell ref="C40:E40"/>
+    <mergeCell ref="I40:J40"/>
+    <mergeCell ref="C35:E35"/>
+    <mergeCell ref="I35:J35"/>
+    <mergeCell ref="C36:E36"/>
+    <mergeCell ref="I36:J36"/>
+    <mergeCell ref="C37:E37"/>
+    <mergeCell ref="I37:J37"/>
+    <mergeCell ref="C32:E32"/>
+    <mergeCell ref="I32:J32"/>
+    <mergeCell ref="C33:E33"/>
+    <mergeCell ref="I33:J33"/>
+    <mergeCell ref="C34:E34"/>
+    <mergeCell ref="I34:J34"/>
+    <mergeCell ref="C29:E29"/>
+    <mergeCell ref="I29:J29"/>
+    <mergeCell ref="C30:E30"/>
+    <mergeCell ref="I30:J30"/>
+    <mergeCell ref="C31:E31"/>
+    <mergeCell ref="I31:J31"/>
+    <mergeCell ref="C26:E26"/>
+    <mergeCell ref="I26:J26"/>
+    <mergeCell ref="C27:E27"/>
+    <mergeCell ref="I27:J27"/>
+    <mergeCell ref="C28:E28"/>
+    <mergeCell ref="I28:J28"/>
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="I23:J23"/>
+    <mergeCell ref="C24:E24"/>
+    <mergeCell ref="I24:J24"/>
+    <mergeCell ref="C25:E25"/>
+    <mergeCell ref="I25:J25"/>
+    <mergeCell ref="C20:E20"/>
+    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="C17:E17"/>
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="C19:E19"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="C14:E14"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="C15:E15"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="C16:E16"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="C11:E11"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="C12:E12"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="I13:J13"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="I10:J10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -32148,52 +32155,52 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="31.7" customHeight="1">
-      <c r="A1" s="255" t="s">
+      <c r="A1" s="254" t="s">
         <v>170</v>
       </c>
-      <c r="B1" s="255"/>
-      <c r="C1" s="255"/>
-      <c r="D1" s="255"/>
-      <c r="E1" s="255"/>
-      <c r="F1" s="255"/>
-      <c r="G1" s="255"/>
-      <c r="H1" s="255"/>
-      <c r="I1" s="255"/>
-      <c r="J1" s="255"/>
-      <c r="K1" s="255"/>
-      <c r="L1" s="255"/>
-      <c r="M1" s="255"/>
-      <c r="N1" s="255"/>
-      <c r="O1" s="255"/>
-      <c r="P1" s="255"/>
-      <c r="Q1" s="255"/>
+      <c r="B1" s="254"/>
+      <c r="C1" s="254"/>
+      <c r="D1" s="254"/>
+      <c r="E1" s="254"/>
+      <c r="F1" s="254"/>
+      <c r="G1" s="254"/>
+      <c r="H1" s="254"/>
+      <c r="I1" s="254"/>
+      <c r="J1" s="254"/>
+      <c r="K1" s="254"/>
+      <c r="L1" s="254"/>
+      <c r="M1" s="254"/>
+      <c r="N1" s="254"/>
+      <c r="O1" s="254"/>
+      <c r="P1" s="254"/>
+      <c r="Q1" s="254"/>
     </row>
     <row r="2" spans="1:17" s="77" customFormat="1" ht="23.45" customHeight="1">
-      <c r="A2" s="256" t="s">
+      <c r="A2" s="255" t="s">
         <v>171</v>
       </c>
-      <c r="B2" s="256"/>
-      <c r="C2" s="256"/>
-      <c r="D2" s="256"/>
-      <c r="E2" s="256"/>
-      <c r="F2" s="256"/>
-      <c r="G2" s="257" t="s">
+      <c r="B2" s="255"/>
+      <c r="C2" s="255"/>
+      <c r="D2" s="255"/>
+      <c r="E2" s="255"/>
+      <c r="F2" s="255"/>
+      <c r="G2" s="256" t="s">
         <v>98</v>
       </c>
-      <c r="H2" s="257"/>
-      <c r="I2" s="257"/>
-      <c r="J2" s="257"/>
-      <c r="K2" s="257"/>
-      <c r="L2" s="257"/>
-      <c r="M2" s="258" t="s">
+      <c r="H2" s="256"/>
+      <c r="I2" s="256"/>
+      <c r="J2" s="256"/>
+      <c r="K2" s="256"/>
+      <c r="L2" s="256"/>
+      <c r="M2" s="257" t="s">
         <v>172</v>
       </c>
-      <c r="N2" s="259" t="s">
+      <c r="N2" s="258" t="s">
         <v>173</v>
       </c>
-      <c r="O2" s="260"/>
-      <c r="P2" s="260"/>
-      <c r="Q2" s="261"/>
+      <c r="O2" s="259"/>
+      <c r="P2" s="259"/>
+      <c r="Q2" s="260"/>
     </row>
     <row r="3" spans="1:17" ht="30">
       <c r="A3" s="136"/>
@@ -32205,14 +32212,14 @@
       <c r="G3" s="139" t="s">
         <v>96</v>
       </c>
-      <c r="H3" s="262" t="s">
+      <c r="H3" s="261" t="s">
         <v>174</v>
       </c>
-      <c r="I3" s="262"/>
-      <c r="J3" s="262"/>
-      <c r="K3" s="262"/>
-      <c r="L3" s="262"/>
-      <c r="M3" s="258"/>
+      <c r="I3" s="261"/>
+      <c r="J3" s="261"/>
+      <c r="K3" s="261"/>
+      <c r="L3" s="261"/>
+      <c r="M3" s="257"/>
       <c r="N3" s="140" t="s">
         <v>175</v>
       </c>
@@ -34281,152 +34288,152 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="20.25" customHeight="1">
-      <c r="A1" s="263" t="s">
+      <c r="A1" s="299" t="s">
         <v>142</v>
       </c>
-      <c r="B1" s="264"/>
-      <c r="C1" s="264"/>
-      <c r="D1" s="264"/>
-      <c r="E1" s="264"/>
-      <c r="F1" s="264"/>
-      <c r="G1" s="264"/>
-      <c r="H1" s="265"/>
-      <c r="I1" s="266" t="s">
+      <c r="B1" s="300"/>
+      <c r="C1" s="300"/>
+      <c r="D1" s="300"/>
+      <c r="E1" s="300"/>
+      <c r="F1" s="300"/>
+      <c r="G1" s="300"/>
+      <c r="H1" s="301"/>
+      <c r="I1" s="302" t="s">
         <v>143</v>
       </c>
-      <c r="J1" s="267"/>
-      <c r="K1" s="268"/>
-      <c r="L1" s="269" t="s">
+      <c r="J1" s="303"/>
+      <c r="K1" s="304"/>
+      <c r="L1" s="305" t="s">
         <v>144</v>
       </c>
-      <c r="M1" s="270"/>
-      <c r="N1" s="271"/>
+      <c r="M1" s="306"/>
+      <c r="N1" s="307"/>
     </row>
     <row r="2" spans="1:14" ht="30" customHeight="1">
-      <c r="A2" s="272" t="s">
+      <c r="A2" s="308" t="s">
         <v>145</v>
       </c>
-      <c r="B2" s="273"/>
-      <c r="C2" s="273"/>
-      <c r="D2" s="273"/>
-      <c r="E2" s="273"/>
-      <c r="F2" s="273"/>
-      <c r="G2" s="273"/>
-      <c r="H2" s="274"/>
-      <c r="I2" s="275" t="s">
+      <c r="B2" s="309"/>
+      <c r="C2" s="309"/>
+      <c r="D2" s="309"/>
+      <c r="E2" s="309"/>
+      <c r="F2" s="309"/>
+      <c r="G2" s="309"/>
+      <c r="H2" s="310"/>
+      <c r="I2" s="311" t="s">
         <v>146</v>
       </c>
-      <c r="J2" s="276"/>
-      <c r="K2" s="277"/>
-      <c r="L2" s="278" t="s">
+      <c r="J2" s="312"/>
+      <c r="K2" s="313"/>
+      <c r="L2" s="314" t="s">
         <v>147</v>
       </c>
-      <c r="M2" s="279"/>
-      <c r="N2" s="280"/>
+      <c r="M2" s="315"/>
+      <c r="N2" s="316"/>
     </row>
     <row r="3" spans="1:14" ht="30.75" customHeight="1">
-      <c r="A3" s="281" t="s">
+      <c r="A3" s="287" t="s">
         <v>148</v>
       </c>
-      <c r="B3" s="282"/>
-      <c r="C3" s="282"/>
-      <c r="D3" s="282"/>
-      <c r="E3" s="282"/>
-      <c r="F3" s="282"/>
-      <c r="G3" s="282"/>
-      <c r="H3" s="283"/>
-      <c r="I3" s="284" t="s">
+      <c r="B3" s="288"/>
+      <c r="C3" s="288"/>
+      <c r="D3" s="288"/>
+      <c r="E3" s="288"/>
+      <c r="F3" s="288"/>
+      <c r="G3" s="288"/>
+      <c r="H3" s="289"/>
+      <c r="I3" s="290" t="s">
         <v>149</v>
       </c>
-      <c r="J3" s="285"/>
-      <c r="K3" s="284" t="s">
+      <c r="J3" s="291"/>
+      <c r="K3" s="290" t="s">
         <v>150</v>
       </c>
-      <c r="L3" s="285"/>
-      <c r="M3" s="284" t="s">
+      <c r="L3" s="291"/>
+      <c r="M3" s="290" t="s">
         <v>151</v>
       </c>
-      <c r="N3" s="286"/>
+      <c r="N3" s="292"/>
     </row>
     <row r="4" spans="1:14" ht="43.5" customHeight="1">
       <c r="A4" s="85" t="s">
         <v>152</v>
       </c>
-      <c r="B4" s="287" t="s">
+      <c r="B4" s="293" t="s">
         <v>153</v>
       </c>
-      <c r="C4" s="288"/>
-      <c r="D4" s="288"/>
-      <c r="E4" s="288"/>
-      <c r="F4" s="288"/>
-      <c r="G4" s="288"/>
-      <c r="H4" s="289"/>
-      <c r="I4" s="290"/>
-      <c r="J4" s="291"/>
-      <c r="K4" s="290"/>
-      <c r="L4" s="291"/>
-      <c r="M4" s="290"/>
-      <c r="N4" s="292"/>
+      <c r="C4" s="294"/>
+      <c r="D4" s="294"/>
+      <c r="E4" s="294"/>
+      <c r="F4" s="294"/>
+      <c r="G4" s="294"/>
+      <c r="H4" s="295"/>
+      <c r="I4" s="296"/>
+      <c r="J4" s="297"/>
+      <c r="K4" s="296"/>
+      <c r="L4" s="297"/>
+      <c r="M4" s="296"/>
+      <c r="N4" s="298"/>
     </row>
     <row r="5" spans="1:14" s="87" customFormat="1" ht="46.5" customHeight="1">
       <c r="A5" s="86">
         <v>1</v>
       </c>
-      <c r="B5" s="295" t="s">
+      <c r="B5" s="264" t="s">
         <v>154</v>
       </c>
-      <c r="C5" s="296"/>
-      <c r="D5" s="296"/>
-      <c r="E5" s="296"/>
-      <c r="F5" s="296"/>
-      <c r="G5" s="296"/>
-      <c r="H5" s="296"/>
-      <c r="I5" s="296"/>
-      <c r="J5" s="296"/>
-      <c r="K5" s="296"/>
-      <c r="L5" s="296"/>
-      <c r="M5" s="296"/>
-      <c r="N5" s="297"/>
+      <c r="C5" s="265"/>
+      <c r="D5" s="265"/>
+      <c r="E5" s="265"/>
+      <c r="F5" s="265"/>
+      <c r="G5" s="265"/>
+      <c r="H5" s="265"/>
+      <c r="I5" s="265"/>
+      <c r="J5" s="265"/>
+      <c r="K5" s="265"/>
+      <c r="L5" s="265"/>
+      <c r="M5" s="265"/>
+      <c r="N5" s="266"/>
     </row>
     <row r="6" spans="1:14" s="87" customFormat="1" ht="39" customHeight="1">
       <c r="A6" s="88">
         <v>2</v>
       </c>
-      <c r="B6" s="298" t="s">
+      <c r="B6" s="267" t="s">
         <v>155</v>
       </c>
-      <c r="C6" s="299"/>
-      <c r="D6" s="299"/>
-      <c r="E6" s="299"/>
-      <c r="F6" s="299"/>
-      <c r="G6" s="299"/>
-      <c r="H6" s="299"/>
-      <c r="I6" s="299"/>
-      <c r="J6" s="299"/>
-      <c r="K6" s="299"/>
-      <c r="L6" s="299"/>
-      <c r="M6" s="299"/>
-      <c r="N6" s="300"/>
+      <c r="C6" s="268"/>
+      <c r="D6" s="268"/>
+      <c r="E6" s="268"/>
+      <c r="F6" s="268"/>
+      <c r="G6" s="268"/>
+      <c r="H6" s="268"/>
+      <c r="I6" s="268"/>
+      <c r="J6" s="268"/>
+      <c r="K6" s="268"/>
+      <c r="L6" s="268"/>
+      <c r="M6" s="268"/>
+      <c r="N6" s="269"/>
     </row>
     <row r="7" spans="1:14" s="87" customFormat="1" ht="21" customHeight="1">
       <c r="A7" s="89" t="s">
         <v>156</v>
       </c>
-      <c r="B7" s="301" t="s">
+      <c r="B7" s="270" t="s">
         <v>157</v>
       </c>
-      <c r="C7" s="302"/>
-      <c r="D7" s="302"/>
-      <c r="E7" s="302"/>
-      <c r="F7" s="302"/>
-      <c r="G7" s="302"/>
-      <c r="H7" s="302"/>
-      <c r="I7" s="302"/>
-      <c r="J7" s="302"/>
-      <c r="K7" s="302"/>
-      <c r="L7" s="302"/>
-      <c r="M7" s="302"/>
-      <c r="N7" s="303"/>
+      <c r="C7" s="271"/>
+      <c r="D7" s="271"/>
+      <c r="E7" s="271"/>
+      <c r="F7" s="271"/>
+      <c r="G7" s="271"/>
+      <c r="H7" s="271"/>
+      <c r="I7" s="271"/>
+      <c r="J7" s="271"/>
+      <c r="K7" s="271"/>
+      <c r="L7" s="271"/>
+      <c r="M7" s="271"/>
+      <c r="N7" s="272"/>
     </row>
     <row r="8" spans="1:14" s="95" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A8" s="90"/>
@@ -34995,7 +35002,7 @@
       <c r="N42" s="99"/>
     </row>
     <row r="43" spans="1:14" s="123" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A43" s="304" t="s">
+      <c r="A43" s="273" t="s">
         <v>162</v>
       </c>
       <c r="B43" s="116" t="s">
@@ -35003,81 +35010,95 @@
       </c>
       <c r="C43" s="117"/>
       <c r="D43" s="118"/>
-      <c r="E43" s="307"/>
-      <c r="F43" s="308"/>
-      <c r="G43" s="308"/>
-      <c r="H43" s="308"/>
-      <c r="I43" s="308"/>
-      <c r="J43" s="308"/>
+      <c r="E43" s="276"/>
+      <c r="F43" s="277"/>
+      <c r="G43" s="277"/>
+      <c r="H43" s="277"/>
+      <c r="I43" s="277"/>
+      <c r="J43" s="277"/>
       <c r="K43" s="121"/>
       <c r="L43" s="120"/>
       <c r="M43" s="119"/>
       <c r="N43" s="122"/>
     </row>
     <row r="44" spans="1:14" s="123" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A44" s="305"/>
+      <c r="A44" s="274"/>
       <c r="B44" s="124" t="s">
         <v>163</v>
       </c>
       <c r="C44" s="125"/>
       <c r="D44" s="126"/>
-      <c r="E44" s="309"/>
-      <c r="F44" s="310"/>
-      <c r="G44" s="310"/>
-      <c r="H44" s="310"/>
-      <c r="I44" s="310"/>
-      <c r="J44" s="310"/>
+      <c r="E44" s="278"/>
+      <c r="F44" s="279"/>
+      <c r="G44" s="279"/>
+      <c r="H44" s="279"/>
+      <c r="I44" s="279"/>
+      <c r="J44" s="279"/>
       <c r="K44" s="127"/>
       <c r="L44" s="128"/>
       <c r="M44" s="129"/>
       <c r="N44" s="130"/>
     </row>
     <row r="45" spans="1:14" s="123" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A45" s="305"/>
+      <c r="A45" s="274"/>
       <c r="B45" s="131" t="s">
         <v>164</v>
       </c>
       <c r="C45" s="125"/>
       <c r="D45" s="126"/>
-      <c r="E45" s="311"/>
-      <c r="F45" s="312"/>
-      <c r="G45" s="312"/>
-      <c r="H45" s="312"/>
-      <c r="I45" s="312"/>
-      <c r="J45" s="312"/>
+      <c r="E45" s="280"/>
+      <c r="F45" s="281"/>
+      <c r="G45" s="281"/>
+      <c r="H45" s="281"/>
+      <c r="I45" s="281"/>
+      <c r="J45" s="281"/>
       <c r="K45" s="132"/>
       <c r="L45" s="128"/>
       <c r="M45" s="133"/>
       <c r="N45" s="134"/>
     </row>
     <row r="46" spans="1:14" s="123" customFormat="1" ht="25.5" customHeight="1" thickBot="1">
-      <c r="A46" s="306"/>
+      <c r="A46" s="275"/>
       <c r="B46" s="135" t="s">
         <v>165</v>
       </c>
-      <c r="C46" s="313" t="s">
+      <c r="C46" s="282" t="s">
         <v>166</v>
       </c>
-      <c r="D46" s="314"/>
-      <c r="E46" s="315" t="s">
+      <c r="D46" s="283"/>
+      <c r="E46" s="284" t="s">
         <v>167</v>
       </c>
-      <c r="F46" s="316"/>
-      <c r="G46" s="316"/>
-      <c r="H46" s="316"/>
-      <c r="I46" s="316"/>
-      <c r="J46" s="317"/>
-      <c r="K46" s="293" t="s">
+      <c r="F46" s="285"/>
+      <c r="G46" s="285"/>
+      <c r="H46" s="285"/>
+      <c r="I46" s="285"/>
+      <c r="J46" s="286"/>
+      <c r="K46" s="262" t="s">
         <v>168</v>
       </c>
-      <c r="L46" s="317"/>
-      <c r="M46" s="293" t="s">
+      <c r="L46" s="286"/>
+      <c r="M46" s="262" t="s">
         <v>169</v>
       </c>
-      <c r="N46" s="294"/>
+      <c r="N46" s="263"/>
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="L1:N1"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="I2:K2"/>
+    <mergeCell ref="L2:N2"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="B4:H4"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="M4:N4"/>
     <mergeCell ref="M46:N46"/>
     <mergeCell ref="B5:N5"/>
     <mergeCell ref="B6:N6"/>
@@ -35089,20 +35110,6 @@
     <mergeCell ref="C46:D46"/>
     <mergeCell ref="E46:J46"/>
     <mergeCell ref="K46:L46"/>
-    <mergeCell ref="A3:H3"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="M3:N3"/>
-    <mergeCell ref="B4:H4"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="M4:N4"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="I1:K1"/>
-    <mergeCell ref="L1:N1"/>
-    <mergeCell ref="A2:H2"/>
-    <mergeCell ref="I2:K2"/>
-    <mergeCell ref="L2:N2"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -35150,20 +35157,20 @@
       </c>
     </row>
     <row r="3" spans="1:12" ht="26.25">
-      <c r="A3" s="321" t="s">
+      <c r="A3" s="320" t="s">
         <v>229</v>
       </c>
-      <c r="B3" s="321"/>
-      <c r="C3" s="321"/>
-      <c r="D3" s="321"/>
-      <c r="E3" s="321"/>
-      <c r="F3" s="321"/>
-      <c r="G3" s="321"/>
-      <c r="H3" s="321"/>
-      <c r="I3" s="321"/>
-      <c r="J3" s="321"/>
-      <c r="K3" s="321"/>
-      <c r="L3" s="321"/>
+      <c r="B3" s="320"/>
+      <c r="C3" s="320"/>
+      <c r="D3" s="320"/>
+      <c r="E3" s="320"/>
+      <c r="F3" s="320"/>
+      <c r="G3" s="320"/>
+      <c r="H3" s="320"/>
+      <c r="I3" s="320"/>
+      <c r="J3" s="320"/>
+      <c r="K3" s="320"/>
+      <c r="L3" s="320"/>
     </row>
     <row r="4" spans="1:12" ht="20.100000000000001" customHeight="1">
       <c r="H4" s="56" t="s">
@@ -35184,10 +35191,10 @@
       <c r="H5" s="56" t="s">
         <v>89</v>
       </c>
-      <c r="I5" s="327"/>
-      <c r="J5" s="327"/>
-      <c r="K5" s="327"/>
-      <c r="L5" s="327"/>
+      <c r="I5" s="326"/>
+      <c r="J5" s="326"/>
+      <c r="K5" s="326"/>
+      <c r="L5" s="326"/>
     </row>
     <row r="6" spans="1:12" ht="20.25" customHeight="1">
       <c r="B6" t="s">
@@ -35226,32 +35233,32 @@
       <c r="L8" s="13"/>
     </row>
     <row r="9" spans="1:12" ht="15.75" thickBot="1">
-      <c r="J9" s="328" t="s">
+      <c r="J9" s="327" t="s">
         <v>132</v>
       </c>
-      <c r="K9" s="329" t="s">
+      <c r="K9" s="328" t="s">
         <v>140</v>
       </c>
-      <c r="L9" s="330"/>
+      <c r="L9" s="329"/>
     </row>
     <row r="10" spans="1:12">
       <c r="B10" s="50" t="s">
         <v>55</v>
       </c>
-      <c r="C10" s="324" t="s">
+      <c r="C10" s="323" t="s">
         <v>56</v>
       </c>
-      <c r="D10" s="325"/>
-      <c r="E10" s="326"/>
+      <c r="D10" s="324"/>
+      <c r="E10" s="325"/>
       <c r="F10" s="50" t="s">
         <v>55</v>
       </c>
-      <c r="G10" s="324" t="s">
+      <c r="G10" s="323" t="s">
         <v>56</v>
       </c>
-      <c r="H10" s="325"/>
+      <c r="H10" s="324"/>
       <c r="I10" s="13"/>
-      <c r="J10" s="328"/>
+      <c r="J10" s="327"/>
       <c r="K10" s="9" t="s">
         <v>141</v>
       </c>
@@ -35261,12 +35268,12 @@
     </row>
     <row r="11" spans="1:12" ht="26.25" customHeight="1" thickBot="1">
       <c r="B11" s="51"/>
-      <c r="C11" s="322"/>
-      <c r="D11" s="323"/>
-      <c r="E11" s="326"/>
+      <c r="C11" s="321"/>
+      <c r="D11" s="322"/>
+      <c r="E11" s="325"/>
       <c r="F11" s="51"/>
-      <c r="G11" s="322"/>
-      <c r="H11" s="323"/>
+      <c r="G11" s="321"/>
+      <c r="H11" s="322"/>
       <c r="I11" s="13"/>
       <c r="J11" s="9"/>
       <c r="K11" s="10"/>
@@ -35949,23 +35956,23 @@
       <c r="L54" s="13"/>
     </row>
     <row r="56" spans="1:12">
-      <c r="A56" s="329" t="s">
+      <c r="A56" s="328" t="s">
         <v>95</v>
       </c>
-      <c r="B56" s="330"/>
-      <c r="C56" s="329" t="s">
+      <c r="B56" s="329"/>
+      <c r="C56" s="328" t="s">
         <v>93</v>
       </c>
-      <c r="D56" s="330"/>
-      <c r="E56" s="329" t="s">
+      <c r="D56" s="329"/>
+      <c r="E56" s="328" t="s">
         <v>221</v>
       </c>
-      <c r="F56" s="330"/>
-      <c r="G56" s="328" t="s">
+      <c r="F56" s="329"/>
+      <c r="G56" s="327" t="s">
         <v>231</v>
       </c>
-      <c r="H56" s="328"/>
-      <c r="I56" s="328"/>
+      <c r="H56" s="327"/>
+      <c r="I56" s="327"/>
       <c r="J56" s="58" t="s">
         <v>230</v>
       </c>
@@ -36025,11 +36032,11 @@
         <v>88</v>
       </c>
       <c r="F61" s="68"/>
-      <c r="G61" s="318" t="s">
+      <c r="G61" s="317" t="s">
         <v>88</v>
       </c>
-      <c r="H61" s="319"/>
-      <c r="I61" s="320"/>
+      <c r="H61" s="318"/>
+      <c r="I61" s="319"/>
       <c r="J61" s="10" t="s">
         <v>88</v>
       </c>
@@ -36077,52 +36084,52 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="31.7" customHeight="1">
-      <c r="A1" s="255" t="s">
+      <c r="A1" s="254" t="s">
         <v>170</v>
       </c>
-      <c r="B1" s="255"/>
-      <c r="C1" s="255"/>
-      <c r="D1" s="255"/>
-      <c r="E1" s="255"/>
-      <c r="F1" s="255"/>
-      <c r="G1" s="255"/>
-      <c r="H1" s="255"/>
-      <c r="I1" s="255"/>
-      <c r="J1" s="255"/>
-      <c r="K1" s="255"/>
-      <c r="L1" s="255"/>
-      <c r="M1" s="255"/>
-      <c r="N1" s="255"/>
-      <c r="O1" s="255"/>
-      <c r="P1" s="255"/>
-      <c r="Q1" s="255"/>
+      <c r="B1" s="254"/>
+      <c r="C1" s="254"/>
+      <c r="D1" s="254"/>
+      <c r="E1" s="254"/>
+      <c r="F1" s="254"/>
+      <c r="G1" s="254"/>
+      <c r="H1" s="254"/>
+      <c r="I1" s="254"/>
+      <c r="J1" s="254"/>
+      <c r="K1" s="254"/>
+      <c r="L1" s="254"/>
+      <c r="M1" s="254"/>
+      <c r="N1" s="254"/>
+      <c r="O1" s="254"/>
+      <c r="P1" s="254"/>
+      <c r="Q1" s="254"/>
     </row>
     <row r="2" spans="1:17" s="77" customFormat="1" ht="23.45" customHeight="1">
-      <c r="A2" s="256" t="s">
+      <c r="A2" s="255" t="s">
         <v>171</v>
       </c>
-      <c r="B2" s="256"/>
-      <c r="C2" s="256"/>
-      <c r="D2" s="256"/>
-      <c r="E2" s="256"/>
-      <c r="F2" s="256"/>
-      <c r="G2" s="256" t="s">
+      <c r="B2" s="255"/>
+      <c r="C2" s="255"/>
+      <c r="D2" s="255"/>
+      <c r="E2" s="255"/>
+      <c r="F2" s="255"/>
+      <c r="G2" s="255" t="s">
         <v>98</v>
       </c>
-      <c r="H2" s="256"/>
-      <c r="I2" s="256"/>
-      <c r="J2" s="256"/>
-      <c r="K2" s="256"/>
-      <c r="L2" s="256"/>
-      <c r="M2" s="258" t="s">
+      <c r="H2" s="255"/>
+      <c r="I2" s="255"/>
+      <c r="J2" s="255"/>
+      <c r="K2" s="255"/>
+      <c r="L2" s="255"/>
+      <c r="M2" s="257" t="s">
         <v>172</v>
       </c>
-      <c r="N2" s="259" t="s">
+      <c r="N2" s="258" t="s">
         <v>173</v>
       </c>
-      <c r="O2" s="260"/>
-      <c r="P2" s="260"/>
-      <c r="Q2" s="261"/>
+      <c r="O2" s="259"/>
+      <c r="P2" s="259"/>
+      <c r="Q2" s="260"/>
     </row>
     <row r="3" spans="1:17" ht="30">
       <c r="A3" s="136"/>
@@ -36134,14 +36141,14 @@
       <c r="G3" s="139" t="s">
         <v>96</v>
       </c>
-      <c r="H3" s="262" t="s">
+      <c r="H3" s="261" t="s">
         <v>174</v>
       </c>
-      <c r="I3" s="262"/>
-      <c r="J3" s="262"/>
-      <c r="K3" s="262"/>
-      <c r="L3" s="262"/>
-      <c r="M3" s="258"/>
+      <c r="I3" s="261"/>
+      <c r="J3" s="261"/>
+      <c r="K3" s="261"/>
+      <c r="L3" s="261"/>
+      <c r="M3" s="257"/>
       <c r="N3" s="140" t="s">
         <v>175</v>
       </c>
@@ -38363,152 +38370,152 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="20.25" customHeight="1">
-      <c r="A1" s="331" t="s">
+      <c r="A1" s="367" t="s">
         <v>142</v>
       </c>
-      <c r="B1" s="332"/>
-      <c r="C1" s="332"/>
-      <c r="D1" s="332"/>
-      <c r="E1" s="332"/>
-      <c r="F1" s="332"/>
-      <c r="G1" s="332"/>
-      <c r="H1" s="333"/>
-      <c r="I1" s="334" t="s">
+      <c r="B1" s="368"/>
+      <c r="C1" s="368"/>
+      <c r="D1" s="368"/>
+      <c r="E1" s="368"/>
+      <c r="F1" s="368"/>
+      <c r="G1" s="368"/>
+      <c r="H1" s="369"/>
+      <c r="I1" s="370" t="s">
         <v>143</v>
       </c>
-      <c r="J1" s="335"/>
-      <c r="K1" s="336"/>
-      <c r="L1" s="337" t="s">
+      <c r="J1" s="371"/>
+      <c r="K1" s="372"/>
+      <c r="L1" s="373" t="s">
         <v>144</v>
       </c>
-      <c r="M1" s="338"/>
-      <c r="N1" s="339"/>
+      <c r="M1" s="374"/>
+      <c r="N1" s="375"/>
     </row>
     <row r="2" spans="1:14" ht="30" customHeight="1">
-      <c r="A2" s="340" t="s">
+      <c r="A2" s="376" t="s">
         <v>145</v>
       </c>
-      <c r="B2" s="341"/>
-      <c r="C2" s="341"/>
-      <c r="D2" s="341"/>
-      <c r="E2" s="341"/>
-      <c r="F2" s="341"/>
-      <c r="G2" s="341"/>
-      <c r="H2" s="342"/>
-      <c r="I2" s="343" t="s">
+      <c r="B2" s="377"/>
+      <c r="C2" s="377"/>
+      <c r="D2" s="377"/>
+      <c r="E2" s="377"/>
+      <c r="F2" s="377"/>
+      <c r="G2" s="377"/>
+      <c r="H2" s="378"/>
+      <c r="I2" s="379" t="s">
         <v>146</v>
       </c>
-      <c r="J2" s="344"/>
-      <c r="K2" s="345"/>
-      <c r="L2" s="346" t="s">
+      <c r="J2" s="380"/>
+      <c r="K2" s="381"/>
+      <c r="L2" s="382" t="s">
         <v>147</v>
       </c>
-      <c r="M2" s="347"/>
-      <c r="N2" s="348"/>
+      <c r="M2" s="383"/>
+      <c r="N2" s="384"/>
     </row>
     <row r="3" spans="1:14" ht="30.75" customHeight="1">
-      <c r="A3" s="349" t="s">
+      <c r="A3" s="355" t="s">
         <v>148</v>
       </c>
-      <c r="B3" s="350"/>
-      <c r="C3" s="350"/>
-      <c r="D3" s="350"/>
-      <c r="E3" s="350"/>
-      <c r="F3" s="350"/>
-      <c r="G3" s="350"/>
-      <c r="H3" s="351"/>
-      <c r="I3" s="352" t="s">
+      <c r="B3" s="356"/>
+      <c r="C3" s="356"/>
+      <c r="D3" s="356"/>
+      <c r="E3" s="356"/>
+      <c r="F3" s="356"/>
+      <c r="G3" s="356"/>
+      <c r="H3" s="357"/>
+      <c r="I3" s="358" t="s">
         <v>149</v>
       </c>
-      <c r="J3" s="353"/>
-      <c r="K3" s="352" t="s">
+      <c r="J3" s="359"/>
+      <c r="K3" s="358" t="s">
         <v>150</v>
       </c>
-      <c r="L3" s="353"/>
-      <c r="M3" s="352" t="s">
+      <c r="L3" s="359"/>
+      <c r="M3" s="358" t="s">
         <v>151</v>
       </c>
-      <c r="N3" s="354"/>
+      <c r="N3" s="360"/>
     </row>
     <row r="4" spans="1:14" ht="43.5" customHeight="1">
       <c r="A4" s="165" t="s">
         <v>152</v>
       </c>
-      <c r="B4" s="355" t="s">
+      <c r="B4" s="361" t="s">
         <v>153</v>
       </c>
-      <c r="C4" s="356"/>
-      <c r="D4" s="356"/>
-      <c r="E4" s="356"/>
-      <c r="F4" s="356"/>
-      <c r="G4" s="356"/>
-      <c r="H4" s="357"/>
-      <c r="I4" s="358"/>
-      <c r="J4" s="359"/>
-      <c r="K4" s="358"/>
-      <c r="L4" s="359"/>
-      <c r="M4" s="358"/>
-      <c r="N4" s="360"/>
+      <c r="C4" s="362"/>
+      <c r="D4" s="362"/>
+      <c r="E4" s="362"/>
+      <c r="F4" s="362"/>
+      <c r="G4" s="362"/>
+      <c r="H4" s="363"/>
+      <c r="I4" s="364"/>
+      <c r="J4" s="365"/>
+      <c r="K4" s="364"/>
+      <c r="L4" s="365"/>
+      <c r="M4" s="364"/>
+      <c r="N4" s="366"/>
     </row>
     <row r="5" spans="1:14" s="167" customFormat="1" ht="46.5" customHeight="1">
       <c r="A5" s="166">
         <v>1</v>
       </c>
-      <c r="B5" s="363" t="s">
+      <c r="B5" s="332" t="s">
         <v>154</v>
       </c>
-      <c r="C5" s="364"/>
-      <c r="D5" s="364"/>
-      <c r="E5" s="364"/>
-      <c r="F5" s="364"/>
-      <c r="G5" s="364"/>
-      <c r="H5" s="364"/>
-      <c r="I5" s="364"/>
-      <c r="J5" s="364"/>
-      <c r="K5" s="364"/>
-      <c r="L5" s="364"/>
-      <c r="M5" s="364"/>
-      <c r="N5" s="365"/>
+      <c r="C5" s="333"/>
+      <c r="D5" s="333"/>
+      <c r="E5" s="333"/>
+      <c r="F5" s="333"/>
+      <c r="G5" s="333"/>
+      <c r="H5" s="333"/>
+      <c r="I5" s="333"/>
+      <c r="J5" s="333"/>
+      <c r="K5" s="333"/>
+      <c r="L5" s="333"/>
+      <c r="M5" s="333"/>
+      <c r="N5" s="334"/>
     </row>
     <row r="6" spans="1:14" s="167" customFormat="1" ht="39" customHeight="1">
       <c r="A6" s="168">
         <v>2</v>
       </c>
-      <c r="B6" s="366" t="s">
+      <c r="B6" s="335" t="s">
         <v>155</v>
       </c>
-      <c r="C6" s="367"/>
-      <c r="D6" s="367"/>
-      <c r="E6" s="367"/>
-      <c r="F6" s="367"/>
-      <c r="G6" s="367"/>
-      <c r="H6" s="367"/>
-      <c r="I6" s="367"/>
-      <c r="J6" s="367"/>
-      <c r="K6" s="367"/>
-      <c r="L6" s="367"/>
-      <c r="M6" s="367"/>
-      <c r="N6" s="368"/>
+      <c r="C6" s="336"/>
+      <c r="D6" s="336"/>
+      <c r="E6" s="336"/>
+      <c r="F6" s="336"/>
+      <c r="G6" s="336"/>
+      <c r="H6" s="336"/>
+      <c r="I6" s="336"/>
+      <c r="J6" s="336"/>
+      <c r="K6" s="336"/>
+      <c r="L6" s="336"/>
+      <c r="M6" s="336"/>
+      <c r="N6" s="337"/>
     </row>
     <row r="7" spans="1:14" s="167" customFormat="1" ht="21" customHeight="1">
       <c r="A7" s="169" t="s">
         <v>156</v>
       </c>
-      <c r="B7" s="369" t="s">
+      <c r="B7" s="338" t="s">
         <v>157</v>
       </c>
-      <c r="C7" s="370"/>
-      <c r="D7" s="370"/>
-      <c r="E7" s="370"/>
-      <c r="F7" s="370"/>
-      <c r="G7" s="370"/>
-      <c r="H7" s="370"/>
-      <c r="I7" s="370"/>
-      <c r="J7" s="370"/>
-      <c r="K7" s="370"/>
-      <c r="L7" s="370"/>
-      <c r="M7" s="370"/>
-      <c r="N7" s="371"/>
+      <c r="C7" s="339"/>
+      <c r="D7" s="339"/>
+      <c r="E7" s="339"/>
+      <c r="F7" s="339"/>
+      <c r="G7" s="339"/>
+      <c r="H7" s="339"/>
+      <c r="I7" s="339"/>
+      <c r="J7" s="339"/>
+      <c r="K7" s="339"/>
+      <c r="L7" s="339"/>
+      <c r="M7" s="339"/>
+      <c r="N7" s="340"/>
     </row>
     <row r="8" spans="1:14" s="174" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A8" s="170"/>
@@ -39077,7 +39084,7 @@
       <c r="N42" s="178"/>
     </row>
     <row r="43" spans="1:14" s="202" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A43" s="372" t="s">
+      <c r="A43" s="341" t="s">
         <v>162</v>
       </c>
       <c r="B43" s="195" t="s">
@@ -39085,81 +39092,95 @@
       </c>
       <c r="C43" s="196"/>
       <c r="D43" s="197"/>
-      <c r="E43" s="375"/>
-      <c r="F43" s="376"/>
-      <c r="G43" s="376"/>
-      <c r="H43" s="376"/>
-      <c r="I43" s="376"/>
-      <c r="J43" s="376"/>
+      <c r="E43" s="344"/>
+      <c r="F43" s="345"/>
+      <c r="G43" s="345"/>
+      <c r="H43" s="345"/>
+      <c r="I43" s="345"/>
+      <c r="J43" s="345"/>
       <c r="K43" s="200"/>
       <c r="L43" s="199"/>
       <c r="M43" s="198"/>
       <c r="N43" s="201"/>
     </row>
     <row r="44" spans="1:14" s="202" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A44" s="373"/>
+      <c r="A44" s="342"/>
       <c r="B44" s="203" t="s">
         <v>163</v>
       </c>
       <c r="C44" s="204"/>
       <c r="D44" s="205"/>
-      <c r="E44" s="377"/>
-      <c r="F44" s="378"/>
-      <c r="G44" s="378"/>
-      <c r="H44" s="378"/>
-      <c r="I44" s="378"/>
-      <c r="J44" s="378"/>
+      <c r="E44" s="346"/>
+      <c r="F44" s="347"/>
+      <c r="G44" s="347"/>
+      <c r="H44" s="347"/>
+      <c r="I44" s="347"/>
+      <c r="J44" s="347"/>
       <c r="K44" s="206"/>
       <c r="L44" s="207"/>
       <c r="M44" s="208"/>
       <c r="N44" s="209"/>
     </row>
     <row r="45" spans="1:14" s="202" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A45" s="373"/>
+      <c r="A45" s="342"/>
       <c r="B45" s="210" t="s">
         <v>164</v>
       </c>
       <c r="C45" s="204"/>
       <c r="D45" s="205"/>
-      <c r="E45" s="379"/>
-      <c r="F45" s="380"/>
-      <c r="G45" s="380"/>
-      <c r="H45" s="380"/>
-      <c r="I45" s="380"/>
-      <c r="J45" s="380"/>
+      <c r="E45" s="348"/>
+      <c r="F45" s="349"/>
+      <c r="G45" s="349"/>
+      <c r="H45" s="349"/>
+      <c r="I45" s="349"/>
+      <c r="J45" s="349"/>
       <c r="K45" s="211"/>
       <c r="L45" s="207"/>
       <c r="M45" s="212"/>
       <c r="N45" s="213"/>
     </row>
     <row r="46" spans="1:14" s="202" customFormat="1" ht="25.5" customHeight="1" thickBot="1">
-      <c r="A46" s="374"/>
+      <c r="A46" s="343"/>
       <c r="B46" s="214" t="s">
         <v>165</v>
       </c>
-      <c r="C46" s="381" t="s">
+      <c r="C46" s="350" t="s">
         <v>166</v>
       </c>
-      <c r="D46" s="382"/>
-      <c r="E46" s="383" t="s">
+      <c r="D46" s="351"/>
+      <c r="E46" s="352" t="s">
         <v>167</v>
       </c>
-      <c r="F46" s="384"/>
-      <c r="G46" s="384"/>
-      <c r="H46" s="384"/>
-      <c r="I46" s="384"/>
-      <c r="J46" s="385"/>
-      <c r="K46" s="361" t="s">
+      <c r="F46" s="353"/>
+      <c r="G46" s="353"/>
+      <c r="H46" s="353"/>
+      <c r="I46" s="353"/>
+      <c r="J46" s="354"/>
+      <c r="K46" s="330" t="s">
         <v>168</v>
       </c>
-      <c r="L46" s="385"/>
-      <c r="M46" s="361" t="s">
+      <c r="L46" s="354"/>
+      <c r="M46" s="330" t="s">
         <v>169</v>
       </c>
-      <c r="N46" s="362"/>
+      <c r="N46" s="331"/>
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="L1:N1"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="I2:K2"/>
+    <mergeCell ref="L2:N2"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="B4:H4"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="M4:N4"/>
     <mergeCell ref="M46:N46"/>
     <mergeCell ref="B5:N5"/>
     <mergeCell ref="B6:N6"/>
@@ -39171,20 +39192,6 @@
     <mergeCell ref="C46:D46"/>
     <mergeCell ref="E46:J46"/>
     <mergeCell ref="K46:L46"/>
-    <mergeCell ref="A3:H3"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="M3:N3"/>
-    <mergeCell ref="B4:H4"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="M4:N4"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="I1:K1"/>
-    <mergeCell ref="L1:N1"/>
-    <mergeCell ref="A2:H2"/>
-    <mergeCell ref="I2:K2"/>
-    <mergeCell ref="L2:N2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -39229,29 +39236,29 @@
       </c>
     </row>
     <row r="3" spans="1:12" ht="26.25">
-      <c r="A3" s="321" t="s">
+      <c r="A3" s="320" t="s">
         <v>229</v>
       </c>
-      <c r="B3" s="321"/>
-      <c r="C3" s="321"/>
-      <c r="D3" s="321"/>
-      <c r="E3" s="321"/>
-      <c r="F3" s="321"/>
-      <c r="G3" s="321"/>
-      <c r="H3" s="321"/>
-      <c r="I3" s="321"/>
-      <c r="J3" s="321"/>
-      <c r="K3" s="321"/>
-      <c r="L3" s="321"/>
+      <c r="B3" s="320"/>
+      <c r="C3" s="320"/>
+      <c r="D3" s="320"/>
+      <c r="E3" s="320"/>
+      <c r="F3" s="320"/>
+      <c r="G3" s="320"/>
+      <c r="H3" s="320"/>
+      <c r="I3" s="320"/>
+      <c r="J3" s="320"/>
+      <c r="K3" s="320"/>
+      <c r="L3" s="320"/>
     </row>
     <row r="4" spans="1:12" ht="20.100000000000001" customHeight="1">
       <c r="H4" s="56" t="s">
         <v>88</v>
       </c>
-      <c r="I4" s="390">
+      <c r="I4" s="389">
         <v>45390</v>
       </c>
-      <c r="J4" s="390"/>
+      <c r="J4" s="389"/>
       <c r="K4" s="73"/>
       <c r="L4" s="73"/>
     </row>
@@ -39265,12 +39272,12 @@
       <c r="H5" s="56" t="s">
         <v>89</v>
       </c>
-      <c r="I5" s="327" t="s">
+      <c r="I5" s="326" t="s">
         <v>319</v>
       </c>
-      <c r="J5" s="327"/>
-      <c r="K5" s="327"/>
-      <c r="L5" s="327"/>
+      <c r="J5" s="326"/>
+      <c r="K5" s="326"/>
+      <c r="L5" s="326"/>
     </row>
     <row r="6" spans="1:12" ht="20.25" customHeight="1">
       <c r="B6" t="s">
@@ -39279,10 +39286,10 @@
       <c r="H6" s="56" t="s">
         <v>90</v>
       </c>
-      <c r="I6" s="327" t="s">
+      <c r="I6" s="326" t="s">
         <v>235</v>
       </c>
-      <c r="J6" s="327"/>
+      <c r="J6" s="326"/>
       <c r="K6" s="74"/>
       <c r="L6" s="74"/>
     </row>
@@ -39311,32 +39318,32 @@
       <c r="L8" s="13"/>
     </row>
     <row r="9" spans="1:12" ht="15.75" thickBot="1">
-      <c r="J9" s="328" t="s">
+      <c r="J9" s="327" t="s">
         <v>132</v>
       </c>
-      <c r="K9" s="329" t="s">
+      <c r="K9" s="328" t="s">
         <v>140</v>
       </c>
-      <c r="L9" s="330"/>
+      <c r="L9" s="329"/>
     </row>
     <row r="10" spans="1:12">
       <c r="B10" s="50" t="s">
         <v>55</v>
       </c>
-      <c r="C10" s="324" t="s">
+      <c r="C10" s="323" t="s">
         <v>56</v>
       </c>
-      <c r="D10" s="325"/>
-      <c r="E10" s="326"/>
+      <c r="D10" s="324"/>
+      <c r="E10" s="325"/>
       <c r="F10" s="50" t="s">
         <v>55</v>
       </c>
-      <c r="G10" s="324" t="s">
+      <c r="G10" s="323" t="s">
         <v>56</v>
       </c>
-      <c r="H10" s="325"/>
+      <c r="H10" s="324"/>
       <c r="I10" s="13"/>
-      <c r="J10" s="328"/>
+      <c r="J10" s="327"/>
       <c r="K10" s="9" t="s">
         <v>141</v>
       </c>
@@ -39348,14 +39355,14 @@
       <c r="B11" s="221" t="s">
         <v>234</v>
       </c>
-      <c r="C11" s="388" t="s">
+      <c r="C11" s="387" t="s">
         <v>235</v>
       </c>
-      <c r="D11" s="389"/>
-      <c r="E11" s="326"/>
+      <c r="D11" s="388"/>
+      <c r="E11" s="325"/>
       <c r="F11" s="51"/>
-      <c r="G11" s="322"/>
-      <c r="H11" s="323"/>
+      <c r="G11" s="321"/>
+      <c r="H11" s="322"/>
       <c r="I11" s="13"/>
       <c r="J11" s="9"/>
       <c r="K11" s="10"/>
@@ -40695,10 +40702,10 @@
       <c r="L48" s="9"/>
     </row>
     <row r="49" spans="1:12" ht="17.25" customHeight="1">
-      <c r="A49" s="386" t="s">
+      <c r="A49" s="385" t="s">
         <v>392</v>
       </c>
-      <c r="B49" s="387"/>
+      <c r="B49" s="386"/>
       <c r="C49" s="219"/>
       <c r="D49" s="219"/>
       <c r="E49" s="219"/>
@@ -40722,23 +40729,23 @@
     </row>
     <row r="51" spans="1:12" ht="18" customHeight="1"/>
     <row r="52" spans="1:12">
-      <c r="A52" s="329" t="s">
+      <c r="A52" s="328" t="s">
         <v>95</v>
       </c>
-      <c r="B52" s="330"/>
-      <c r="C52" s="329" t="s">
+      <c r="B52" s="329"/>
+      <c r="C52" s="328" t="s">
         <v>93</v>
       </c>
-      <c r="D52" s="330"/>
-      <c r="E52" s="329" t="s">
+      <c r="D52" s="329"/>
+      <c r="E52" s="328" t="s">
         <v>221</v>
       </c>
-      <c r="F52" s="330"/>
-      <c r="G52" s="328" t="s">
+      <c r="F52" s="329"/>
+      <c r="G52" s="327" t="s">
         <v>231</v>
       </c>
-      <c r="H52" s="328"/>
-      <c r="I52" s="328"/>
+      <c r="H52" s="327"/>
+      <c r="I52" s="327"/>
       <c r="J52" s="58" t="s">
         <v>230</v>
       </c>
@@ -40798,17 +40805,22 @@
         <v>88</v>
       </c>
       <c r="F57" s="68"/>
-      <c r="G57" s="318" t="s">
+      <c r="G57" s="317" t="s">
         <v>88</v>
       </c>
-      <c r="H57" s="319"/>
-      <c r="I57" s="320"/>
+      <c r="H57" s="318"/>
+      <c r="I57" s="319"/>
       <c r="J57" s="10" t="s">
         <v>88</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="C52:D52"/>
+    <mergeCell ref="E52:F52"/>
+    <mergeCell ref="G52:I52"/>
+    <mergeCell ref="G57:I57"/>
     <mergeCell ref="A49:B49"/>
     <mergeCell ref="I6:J6"/>
     <mergeCell ref="A3:L3"/>
@@ -40822,11 +40834,6 @@
     <mergeCell ref="C11:D11"/>
     <mergeCell ref="G11:H11"/>
     <mergeCell ref="I4:J4"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="C52:D52"/>
-    <mergeCell ref="E52:F52"/>
-    <mergeCell ref="G52:I52"/>
-    <mergeCell ref="G57:I57"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.25" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="68" orientation="portrait" r:id="rId1"/>
@@ -40872,29 +40879,29 @@
       </c>
     </row>
     <row r="3" spans="1:12" ht="26.25">
-      <c r="A3" s="321" t="s">
+      <c r="A3" s="320" t="s">
         <v>229</v>
       </c>
-      <c r="B3" s="321"/>
-      <c r="C3" s="321"/>
-      <c r="D3" s="321"/>
-      <c r="E3" s="321"/>
-      <c r="F3" s="321"/>
-      <c r="G3" s="321"/>
-      <c r="H3" s="321"/>
-      <c r="I3" s="321"/>
-      <c r="J3" s="321"/>
-      <c r="K3" s="321"/>
-      <c r="L3" s="321"/>
+      <c r="B3" s="320"/>
+      <c r="C3" s="320"/>
+      <c r="D3" s="320"/>
+      <c r="E3" s="320"/>
+      <c r="F3" s="320"/>
+      <c r="G3" s="320"/>
+      <c r="H3" s="320"/>
+      <c r="I3" s="320"/>
+      <c r="J3" s="320"/>
+      <c r="K3" s="320"/>
+      <c r="L3" s="320"/>
     </row>
     <row r="4" spans="1:12" ht="20.100000000000001" customHeight="1">
       <c r="H4" s="56" t="s">
         <v>88</v>
       </c>
-      <c r="I4" s="390">
+      <c r="I4" s="389">
         <v>45390</v>
       </c>
-      <c r="J4" s="390"/>
+      <c r="J4" s="389"/>
       <c r="K4" s="73"/>
       <c r="L4" s="73"/>
     </row>
@@ -40908,12 +40915,12 @@
       <c r="H5" s="56" t="s">
         <v>89</v>
       </c>
-      <c r="I5" s="327" t="s">
+      <c r="I5" s="326" t="s">
         <v>319</v>
       </c>
-      <c r="J5" s="327"/>
-      <c r="K5" s="327"/>
-      <c r="L5" s="327"/>
+      <c r="J5" s="326"/>
+      <c r="K5" s="326"/>
+      <c r="L5" s="326"/>
     </row>
     <row r="6" spans="1:12" ht="20.25" customHeight="1">
       <c r="B6" t="s">
@@ -40922,10 +40929,10 @@
       <c r="H6" s="56" t="s">
         <v>90</v>
       </c>
-      <c r="I6" s="327" t="s">
+      <c r="I6" s="326" t="s">
         <v>235</v>
       </c>
-      <c r="J6" s="327"/>
+      <c r="J6" s="326"/>
       <c r="K6" s="74"/>
       <c r="L6" s="74"/>
     </row>
@@ -40954,32 +40961,32 @@
       <c r="L8" s="13"/>
     </row>
     <row r="9" spans="1:12" ht="13.5" customHeight="1" thickBot="1">
-      <c r="J9" s="328" t="s">
+      <c r="J9" s="327" t="s">
         <v>132</v>
       </c>
-      <c r="K9" s="329" t="s">
+      <c r="K9" s="328" t="s">
         <v>140</v>
       </c>
-      <c r="L9" s="330"/>
+      <c r="L9" s="329"/>
     </row>
     <row r="10" spans="1:12">
       <c r="B10" s="50" t="s">
         <v>55</v>
       </c>
-      <c r="C10" s="324" t="s">
+      <c r="C10" s="323" t="s">
         <v>56</v>
       </c>
-      <c r="D10" s="325"/>
-      <c r="E10" s="326"/>
+      <c r="D10" s="324"/>
+      <c r="E10" s="325"/>
       <c r="F10" s="50" t="s">
         <v>55</v>
       </c>
-      <c r="G10" s="324" t="s">
+      <c r="G10" s="323" t="s">
         <v>56</v>
       </c>
-      <c r="H10" s="325"/>
+      <c r="H10" s="324"/>
       <c r="I10" s="13"/>
-      <c r="J10" s="328"/>
+      <c r="J10" s="327"/>
       <c r="K10" s="9" t="s">
         <v>141</v>
       </c>
@@ -40991,14 +40998,14 @@
       <c r="B11" s="221" t="s">
         <v>234</v>
       </c>
-      <c r="C11" s="388" t="s">
+      <c r="C11" s="387" t="s">
         <v>235</v>
       </c>
-      <c r="D11" s="389"/>
-      <c r="E11" s="326"/>
+      <c r="D11" s="388"/>
+      <c r="E11" s="325"/>
       <c r="F11" s="51"/>
-      <c r="G11" s="322"/>
-      <c r="H11" s="323"/>
+      <c r="G11" s="321"/>
+      <c r="H11" s="322"/>
       <c r="I11" s="13"/>
       <c r="J11" s="9"/>
       <c r="K11" s="10"/>
@@ -42672,10 +42679,10 @@
       <c r="L57" s="9"/>
     </row>
     <row r="58" spans="1:12" ht="16.5" customHeight="1">
-      <c r="A58" s="391" t="s">
+      <c r="A58" s="390" t="s">
         <v>392</v>
       </c>
-      <c r="B58" s="391"/>
+      <c r="B58" s="390"/>
       <c r="C58" s="67"/>
       <c r="D58" s="222"/>
       <c r="E58" s="219"/>
@@ -42692,23 +42699,23 @@
     </row>
     <row r="59" spans="1:12" ht="21" customHeight="1"/>
     <row r="60" spans="1:12">
-      <c r="A60" s="329" t="s">
+      <c r="A60" s="328" t="s">
         <v>95</v>
       </c>
-      <c r="B60" s="330"/>
-      <c r="C60" s="329" t="s">
+      <c r="B60" s="329"/>
+      <c r="C60" s="328" t="s">
         <v>93</v>
       </c>
-      <c r="D60" s="330"/>
-      <c r="E60" s="329" t="s">
+      <c r="D60" s="329"/>
+      <c r="E60" s="328" t="s">
         <v>221</v>
       </c>
-      <c r="F60" s="330"/>
-      <c r="G60" s="328" t="s">
+      <c r="F60" s="329"/>
+      <c r="G60" s="327" t="s">
         <v>231</v>
       </c>
-      <c r="H60" s="328"/>
-      <c r="I60" s="328"/>
+      <c r="H60" s="327"/>
+      <c r="I60" s="327"/>
       <c r="J60" s="58" t="s">
         <v>230</v>
       </c>
@@ -42768,17 +42775,27 @@
         <v>88</v>
       </c>
       <c r="F65" s="68"/>
-      <c r="G65" s="318" t="s">
+      <c r="G65" s="317" t="s">
         <v>88</v>
       </c>
-      <c r="H65" s="319"/>
-      <c r="I65" s="320"/>
+      <c r="H65" s="318"/>
+      <c r="I65" s="319"/>
       <c r="J65" s="10" t="s">
         <v>88</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="A3:L3"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="I6:J6"/>
     <mergeCell ref="G65:I65"/>
     <mergeCell ref="A58:B58"/>
     <mergeCell ref="C11:D11"/>
@@ -42787,16 +42804,6 @@
     <mergeCell ref="C60:D60"/>
     <mergeCell ref="E60:F60"/>
     <mergeCell ref="G60:I60"/>
-    <mergeCell ref="A3:L3"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="K9:L9"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="G10:H10"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.25" bottom="0.25" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="68" orientation="portrait" r:id="rId1"/>

</xml_diff>